<commit_message>
line item correction update
</commit_message>
<xml_diff>
--- a/PIT4/Schema Publication Changelog.xlsx
+++ b/PIT4/Schema Publication Changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owalsh01\IdeaProjects\paye-employers-documentation\src\main\resources\PIT4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0B35D0-CD59-4F35-93B5-5A955F6B09DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E4498C-A9FA-4BDE-B1A3-BD840A246A3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="494">
   <si>
     <t>Document</t>
   </si>
@@ -3356,6 +3356,9 @@
   </si>
   <si>
     <t>updated pay period description</t>
+  </si>
+  <si>
+    <t>Reference 55</t>
   </si>
 </sst>
 </file>
@@ -3979,7 +3982,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="224">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -4299,9 +4302,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4503,6 +4503,18 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4520,12 +4532,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4551,13 +4557,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5002,12 +5002,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="143" t="s">
+      <c r="A2" s="142" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="144"/>
-      <c r="C2" s="144"/>
-      <c r="D2" s="145"/>
+      <c r="B2" s="143"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="144"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -5030,12 +5030,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="143" t="s">
+      <c r="A4" s="142" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="144"/>
-      <c r="C4" s="144"/>
-      <c r="D4" s="145"/>
+      <c r="B4" s="143"/>
+      <c r="C4" s="143"/>
+      <c r="D4" s="144"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -5075,10 +5075,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="146" t="s">
+      <c r="A7" s="145" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="149">
+      <c r="B7" s="148">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -5092,8 +5092,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="147"/>
-      <c r="B8" s="150"/>
+      <c r="A8" s="146"/>
+      <c r="B8" s="149"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -5105,8 +5105,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="147"/>
-      <c r="B9" s="150"/>
+      <c r="A9" s="146"/>
+      <c r="B9" s="149"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -5118,8 +5118,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="147"/>
-      <c r="B10" s="150"/>
+      <c r="A10" s="146"/>
+      <c r="B10" s="149"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -5131,8 +5131,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="147"/>
-      <c r="B11" s="150"/>
+      <c r="A11" s="146"/>
+      <c r="B11" s="149"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -5144,8 +5144,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="148"/>
-      <c r="B12" s="151"/>
+      <c r="A12" s="147"/>
+      <c r="B12" s="150"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -5157,10 +5157,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="154" t="s">
+      <c r="A13" s="153" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="149">
+      <c r="B13" s="148">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -5174,8 +5174,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="155"/>
-      <c r="B14" s="151"/>
+      <c r="A14" s="154"/>
+      <c r="B14" s="150"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -5221,12 +5221,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="143" t="s">
+      <c r="A17" s="142" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="144"/>
-      <c r="C17" s="144"/>
-      <c r="D17" s="145"/>
+      <c r="B17" s="143"/>
+      <c r="C17" s="143"/>
+      <c r="D17" s="144"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -5266,21 +5266,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="143" t="s">
+      <c r="A20" s="142" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="144"/>
-      <c r="C20" s="144"/>
-      <c r="D20" s="145"/>
+      <c r="B20" s="143"/>
+      <c r="C20" s="143"/>
+      <c r="D20" s="144"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="156" t="s">
+      <c r="A21" s="155" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="153">
+      <c r="B21" s="152">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -5294,8 +5294,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="157"/>
-      <c r="B22" s="151"/>
+      <c r="A22" s="156"/>
+      <c r="B22" s="150"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -5318,18 +5318,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="143" t="s">
+      <c r="A24" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="144"/>
-      <c r="C24" s="144"/>
-      <c r="D24" s="145"/>
+      <c r="B24" s="143"/>
+      <c r="C24" s="143"/>
+      <c r="D24" s="144"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="152" t="s">
+      <c r="A25" s="151" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="153">
+      <c r="B25" s="152">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -5343,8 +5343,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="147"/>
-      <c r="B26" s="150"/>
+      <c r="A26" s="146"/>
+      <c r="B26" s="149"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -5356,8 +5356,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="147"/>
-      <c r="B27" s="150"/>
+      <c r="A27" s="146"/>
+      <c r="B27" s="149"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -5369,8 +5369,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="147"/>
-      <c r="B28" s="150"/>
+      <c r="A28" s="146"/>
+      <c r="B28" s="149"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -5382,8 +5382,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="147"/>
-      <c r="B29" s="150"/>
+      <c r="A29" s="146"/>
+      <c r="B29" s="149"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -5395,8 +5395,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="147"/>
-      <c r="B30" s="150"/>
+      <c r="A30" s="146"/>
+      <c r="B30" s="149"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -5408,8 +5408,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="147"/>
-      <c r="B31" s="150"/>
+      <c r="A31" s="146"/>
+      <c r="B31" s="149"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -5421,8 +5421,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="148"/>
-      <c r="B32" s="151"/>
+      <c r="A32" s="147"/>
+      <c r="B32" s="150"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -5546,12 +5546,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="143" t="s">
+      <c r="A41" s="142" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="144"/>
-      <c r="C41" s="144"/>
-      <c r="D41" s="145"/>
+      <c r="B41" s="143"/>
+      <c r="C41" s="143"/>
+      <c r="D41" s="144"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -5731,10 +5731,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="158" t="s">
+      <c r="A7" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="159" t="s">
+      <c r="B7" s="158" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5745,8 +5745,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="158"/>
-      <c r="B8" s="159"/>
+      <c r="A8" s="157"/>
+      <c r="B8" s="158"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5755,8 +5755,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="158"/>
-      <c r="B9" s="159"/>
+      <c r="A9" s="157"/>
+      <c r="B9" s="158"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5765,8 +5765,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="158"/>
-      <c r="B10" s="159"/>
+      <c r="A10" s="157"/>
+      <c r="B10" s="158"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5775,8 +5775,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="158"/>
-      <c r="B11" s="159"/>
+      <c r="A11" s="157"/>
+      <c r="B11" s="158"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5785,8 +5785,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="158"/>
-      <c r="B12" s="159"/>
+      <c r="A12" s="157"/>
+      <c r="B12" s="158"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5795,10 +5795,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="161" t="s">
+      <c r="A13" s="160" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="159" t="s">
+      <c r="B13" s="158" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5809,8 +5809,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="161"/>
-      <c r="B14" s="159"/>
+      <c r="A14" s="160"/>
+      <c r="B14" s="158"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5819,8 +5819,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="161"/>
-      <c r="B15" s="159"/>
+      <c r="A15" s="160"/>
+      <c r="B15" s="158"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5829,10 +5829,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="162" t="s">
+      <c r="A16" s="161" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="163" t="s">
+      <c r="B16" s="162" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5843,8 +5843,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="162"/>
-      <c r="B17" s="163"/>
+      <c r="A17" s="161"/>
+      <c r="B17" s="162"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5853,8 +5853,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="162"/>
-      <c r="B18" s="163"/>
+      <c r="A18" s="161"/>
+      <c r="B18" s="162"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5863,8 +5863,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="162"/>
-      <c r="B19" s="163"/>
+      <c r="A19" s="161"/>
+      <c r="B19" s="162"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5873,8 +5873,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="162"/>
-      <c r="B20" s="163"/>
+      <c r="A20" s="161"/>
+      <c r="B20" s="162"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5883,8 +5883,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="162"/>
-      <c r="B21" s="163"/>
+      <c r="A21" s="161"/>
+      <c r="B21" s="162"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5893,8 +5893,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="162"/>
-      <c r="B22" s="163"/>
+      <c r="A22" s="161"/>
+      <c r="B22" s="162"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5903,8 +5903,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="162"/>
-      <c r="B23" s="163"/>
+      <c r="A23" s="161"/>
+      <c r="B23" s="162"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5913,26 +5913,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="162"/>
-      <c r="B24" s="163"/>
-      <c r="C24" s="162" t="s">
+      <c r="A24" s="161"/>
+      <c r="B24" s="162"/>
+      <c r="C24" s="161" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="169" t="s">
+      <c r="D24" s="168" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="162"/>
-      <c r="B25" s="163"/>
-      <c r="C25" s="162"/>
-      <c r="D25" s="169"/>
+      <c r="A25" s="161"/>
+      <c r="B25" s="162"/>
+      <c r="C25" s="161"/>
+      <c r="D25" s="168"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="158" t="s">
+      <c r="A26" s="157" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="159" t="s">
+      <c r="B26" s="158" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5943,8 +5943,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="158"/>
-      <c r="B27" s="159"/>
+      <c r="A27" s="157"/>
+      <c r="B27" s="158"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5971,28 +5971,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="160" t="s">
+      <c r="A30" s="159" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="159" t="s">
+      <c r="B30" s="158" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="162" t="s">
+      <c r="C30" s="161" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="172" t="s">
+      <c r="D30" s="171" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="160"/>
-      <c r="B31" s="159"/>
-      <c r="C31" s="162"/>
-      <c r="D31" s="172"/>
+      <c r="A31" s="159"/>
+      <c r="B31" s="158"/>
+      <c r="C31" s="161"/>
+      <c r="D31" s="171"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="160"/>
-      <c r="B32" s="159"/>
+      <c r="A32" s="159"/>
+      <c r="B32" s="158"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -6001,8 +6001,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="160"/>
-      <c r="B33" s="159"/>
+      <c r="A33" s="159"/>
+      <c r="B33" s="158"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -6011,8 +6011,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="160"/>
-      <c r="B34" s="159"/>
+      <c r="A34" s="159"/>
+      <c r="B34" s="158"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -6021,8 +6021,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="160"/>
-      <c r="B35" s="159"/>
+      <c r="A35" s="159"/>
+      <c r="B35" s="158"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -6031,8 +6031,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="160"/>
-      <c r="B36" s="159"/>
+      <c r="A36" s="159"/>
+      <c r="B36" s="158"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -6041,26 +6041,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="160"/>
-      <c r="B37" s="159"/>
-      <c r="C37" s="173" t="s">
+      <c r="A37" s="159"/>
+      <c r="B37" s="158"/>
+      <c r="C37" s="172" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="175" t="s">
+      <c r="D37" s="174" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="160"/>
-      <c r="B38" s="159"/>
-      <c r="C38" s="174"/>
-      <c r="D38" s="175"/>
+      <c r="A38" s="159"/>
+      <c r="B38" s="158"/>
+      <c r="C38" s="173"/>
+      <c r="D38" s="174"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="158" t="s">
+      <c r="A39" s="157" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="159" t="s">
+      <c r="B39" s="158" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -6071,8 +6071,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="158"/>
-      <c r="B40" s="159"/>
+      <c r="A40" s="157"/>
+      <c r="B40" s="158"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -6099,10 +6099,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="160" t="s">
+      <c r="A43" s="159" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="159" t="s">
+      <c r="B43" s="158" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -6111,8 +6111,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="160"/>
-      <c r="B44" s="159"/>
+      <c r="A44" s="159"/>
+      <c r="B44" s="158"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -6121,10 +6121,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="166" t="s">
+      <c r="A45" s="165" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="159" t="s">
+      <c r="B45" s="158" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -6133,8 +6133,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="167"/>
-      <c r="B46" s="159"/>
+      <c r="A46" s="166"/>
+      <c r="B46" s="158"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -6143,8 +6143,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="167"/>
-      <c r="B47" s="159"/>
+      <c r="A47" s="166"/>
+      <c r="B47" s="158"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -6153,8 +6153,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="168"/>
-      <c r="B48" s="159"/>
+      <c r="A48" s="167"/>
+      <c r="B48" s="158"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -6163,10 +6163,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="163" t="s">
+      <c r="A49" s="162" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="163" t="s">
+      <c r="B49" s="162" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -10270,8 +10270,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="163"/>
-      <c r="B50" s="163"/>
+      <c r="A50" s="162"/>
+      <c r="B50" s="162"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -14375,8 +14375,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="163"/>
-      <c r="B51" s="163"/>
+      <c r="A51" s="162"/>
+      <c r="B51" s="162"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -18480,8 +18480,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="163"/>
-      <c r="B52" s="163"/>
+      <c r="A52" s="162"/>
+      <c r="B52" s="162"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -22585,12 +22585,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="163"/>
-      <c r="B53" s="163"/>
-      <c r="C53" s="171" t="s">
+      <c r="A53" s="162"/>
+      <c r="B53" s="162"/>
+      <c r="C53" s="170" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="172" t="s">
+      <c r="D53" s="171" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26690,10 +26690,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="163"/>
-      <c r="B54" s="163"/>
-      <c r="C54" s="171"/>
-      <c r="D54" s="172"/>
+      <c r="A54" s="162"/>
+      <c r="B54" s="162"/>
+      <c r="C54" s="170"/>
+      <c r="D54" s="171"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30811,10 +30811,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="164" t="s">
+      <c r="A57" s="163" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="163" t="s">
+      <c r="B57" s="162" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30825,8 +30825,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="164"/>
-      <c r="B58" s="163"/>
+      <c r="A58" s="163"/>
+      <c r="B58" s="162"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30835,8 +30835,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="164"/>
-      <c r="B59" s="163"/>
+      <c r="A59" s="163"/>
+      <c r="B59" s="162"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30845,8 +30845,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="164"/>
-      <c r="B60" s="163"/>
+      <c r="A60" s="163"/>
+      <c r="B60" s="162"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30855,8 +30855,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="164"/>
-      <c r="B61" s="163"/>
+      <c r="A61" s="163"/>
+      <c r="B61" s="162"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30865,8 +30865,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="164"/>
-      <c r="B62" s="163"/>
+      <c r="A62" s="163"/>
+      <c r="B62" s="162"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30875,8 +30875,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="164"/>
-      <c r="B63" s="163"/>
+      <c r="A63" s="163"/>
+      <c r="B63" s="162"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30885,16 +30885,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="164"/>
-      <c r="B64" s="163"/>
+      <c r="A64" s="163"/>
+      <c r="B64" s="162"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="164"/>
-      <c r="B65" s="163"/>
+      <c r="A65" s="163"/>
+      <c r="B65" s="162"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30903,16 +30903,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="164"/>
-      <c r="B66" s="163"/>
+      <c r="A66" s="163"/>
+      <c r="B66" s="162"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="164"/>
-      <c r="B67" s="163"/>
+      <c r="A67" s="163"/>
+      <c r="B67" s="162"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30921,8 +30921,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="164"/>
-      <c r="B68" s="163"/>
+      <c r="A68" s="163"/>
+      <c r="B68" s="162"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30931,8 +30931,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="164"/>
-      <c r="B69" s="163"/>
+      <c r="A69" s="163"/>
+      <c r="B69" s="162"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30941,8 +30941,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="164"/>
-      <c r="B70" s="163"/>
+      <c r="A70" s="163"/>
+      <c r="B70" s="162"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30951,8 +30951,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="164"/>
-      <c r="B71" s="163"/>
+      <c r="A71" s="163"/>
+      <c r="B71" s="162"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30961,8 +30961,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="164"/>
-      <c r="B72" s="163"/>
+      <c r="A72" s="163"/>
+      <c r="B72" s="162"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30971,16 +30971,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="164"/>
-      <c r="B73" s="163"/>
+      <c r="A73" s="163"/>
+      <c r="B73" s="162"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="164"/>
-      <c r="B74" s="163"/>
+      <c r="A74" s="163"/>
+      <c r="B74" s="162"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30989,18 +30989,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="164"/>
-      <c r="B75" s="163"/>
-      <c r="C75" s="170"/>
-      <c r="D75" s="165" t="s">
+      <c r="A75" s="163"/>
+      <c r="B75" s="162"/>
+      <c r="C75" s="169"/>
+      <c r="D75" s="164" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="164"/>
-      <c r="B76" s="163"/>
-      <c r="C76" s="170"/>
-      <c r="D76" s="165"/>
+      <c r="A76" s="163"/>
+      <c r="B76" s="162"/>
+      <c r="C76" s="169"/>
+      <c r="D76" s="164"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -31124,10 +31124,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="158" t="s">
+      <c r="A4" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="159" t="s">
+      <c r="B4" s="158" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -31138,133 +31138,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="158"/>
-      <c r="B5" s="159"/>
-      <c r="C5" s="185" t="s">
+      <c r="A5" s="157"/>
+      <c r="B5" s="158"/>
+      <c r="C5" s="184" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="184" t="s">
+      <c r="D5" s="183" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="158"/>
-      <c r="B6" s="159"/>
-      <c r="C6" s="185"/>
-      <c r="D6" s="184"/>
+      <c r="A6" s="157"/>
+      <c r="B6" s="158"/>
+      <c r="C6" s="184"/>
+      <c r="D6" s="183"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="158"/>
-      <c r="B7" s="159"/>
+      <c r="A7" s="157"/>
+      <c r="B7" s="158"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="158"/>
-      <c r="B8" s="159"/>
+      <c r="A8" s="157"/>
+      <c r="B8" s="158"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="158"/>
-      <c r="B9" s="159"/>
+      <c r="A9" s="157"/>
+      <c r="B9" s="158"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="161" t="s">
+      <c r="A10" s="160" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="159" t="s">
+      <c r="B10" s="158" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="183"/>
-      <c r="D10" s="184" t="s">
+      <c r="C10" s="182"/>
+      <c r="D10" s="183" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="161"/>
-      <c r="B11" s="159"/>
-      <c r="C11" s="183"/>
-      <c r="D11" s="184"/>
+      <c r="A11" s="160"/>
+      <c r="B11" s="158"/>
+      <c r="C11" s="182"/>
+      <c r="D11" s="183"/>
     </row>
     <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="161"/>
-      <c r="B12" s="159"/>
-      <c r="C12" s="183"/>
-      <c r="D12" s="184"/>
+      <c r="A12" s="160"/>
+      <c r="B12" s="158"/>
+      <c r="C12" s="182"/>
+      <c r="D12" s="183"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="162" t="s">
+      <c r="A13" s="161" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="163" t="s">
+      <c r="B13" s="162" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="186"/>
-      <c r="D13" s="184" t="s">
+      <c r="C13" s="185"/>
+      <c r="D13" s="183" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="162"/>
-      <c r="B14" s="163"/>
-      <c r="C14" s="186"/>
-      <c r="D14" s="184"/>
+      <c r="A14" s="161"/>
+      <c r="B14" s="162"/>
+      <c r="C14" s="185"/>
+      <c r="D14" s="183"/>
     </row>
     <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="162"/>
-      <c r="B15" s="163"/>
-      <c r="C15" s="186"/>
+      <c r="A15" s="161"/>
+      <c r="B15" s="162"/>
+      <c r="C15" s="185"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="162"/>
-      <c r="B16" s="163"/>
-      <c r="C16" s="186"/>
+      <c r="A16" s="161"/>
+      <c r="B16" s="162"/>
+      <c r="C16" s="185"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="162"/>
-      <c r="B17" s="163"/>
-      <c r="C17" s="186"/>
+      <c r="A17" s="161"/>
+      <c r="B17" s="162"/>
+      <c r="C17" s="185"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="162"/>
-      <c r="B18" s="163"/>
-      <c r="C18" s="186"/>
+      <c r="A18" s="161"/>
+      <c r="B18" s="162"/>
+      <c r="C18" s="185"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="162"/>
-      <c r="B19" s="163"/>
-      <c r="C19" s="186"/>
+      <c r="A19" s="161"/>
+      <c r="B19" s="162"/>
+      <c r="C19" s="185"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="162"/>
-      <c r="B20" s="163"/>
-      <c r="C20" s="186"/>
+      <c r="A20" s="161"/>
+      <c r="B20" s="162"/>
+      <c r="C20" s="185"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="162"/>
-      <c r="B21" s="163"/>
-      <c r="C21" s="186"/>
+      <c r="A21" s="161"/>
+      <c r="B21" s="162"/>
+      <c r="C21" s="185"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="162"/>
-      <c r="B22" s="163"/>
-      <c r="C22" s="186"/>
+      <c r="A22" s="161"/>
+      <c r="B22" s="162"/>
+      <c r="C22" s="185"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="162"/>
-      <c r="B23" s="163"/>
-      <c r="C23" s="186"/>
+      <c r="A23" s="161"/>
+      <c r="B23" s="162"/>
+      <c r="C23" s="185"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -31362,10 +31362,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="187" t="s">
+      <c r="A32" s="186" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="190" t="s">
+      <c r="B32" s="189" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -31376,26 +31376,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="188"/>
-      <c r="B33" s="191"/>
+      <c r="A33" s="187"/>
+      <c r="B33" s="190"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="188"/>
-      <c r="B34" s="191"/>
+      <c r="A34" s="187"/>
+      <c r="B34" s="190"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="188"/>
-      <c r="B35" s="191"/>
+      <c r="A35" s="187"/>
+      <c r="B35" s="190"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="189"/>
-      <c r="B36" s="192"/>
+      <c r="A36" s="188"/>
+      <c r="B36" s="191"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -31424,10 +31424,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="160" t="s">
+      <c r="A39" s="159" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="159" t="s">
+      <c r="B39" s="158" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -31438,8 +31438,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="160"/>
-      <c r="B40" s="159"/>
+      <c r="A40" s="159"/>
+      <c r="B40" s="158"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -31448,84 +31448,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="158" t="s">
+      <c r="A41" s="157" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="159" t="s">
+      <c r="B41" s="158" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="183" t="s">
+      <c r="C41" s="182" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="162" t="s">
+      <c r="D41" s="161" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="158"/>
-      <c r="B42" s="159"/>
-      <c r="C42" s="183"/>
-      <c r="D42" s="162"/>
+      <c r="A42" s="157"/>
+      <c r="B42" s="158"/>
+      <c r="C42" s="182"/>
+      <c r="D42" s="161"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="158"/>
-      <c r="B43" s="159"/>
-      <c r="C43" s="183" t="s">
+      <c r="A43" s="157"/>
+      <c r="B43" s="158"/>
+      <c r="C43" s="182" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="165" t="s">
+      <c r="D43" s="164" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="158"/>
-      <c r="B44" s="159"/>
-      <c r="C44" s="183"/>
-      <c r="D44" s="165"/>
+      <c r="A44" s="157"/>
+      <c r="B44" s="158"/>
+      <c r="C44" s="182"/>
+      <c r="D44" s="164"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="164" t="s">
+      <c r="A45" s="163" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="163" t="s">
+      <c r="B45" s="162" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="179"/>
+      <c r="C45" s="178"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="164"/>
-      <c r="B46" s="163"/>
-      <c r="C46" s="180"/>
-      <c r="D46" s="176" t="s">
+      <c r="A46" s="163"/>
+      <c r="B46" s="162"/>
+      <c r="C46" s="179"/>
+      <c r="D46" s="175" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="164"/>
-      <c r="B47" s="163"/>
-      <c r="C47" s="180"/>
-      <c r="D47" s="177"/>
+      <c r="A47" s="163"/>
+      <c r="B47" s="162"/>
+      <c r="C47" s="179"/>
+      <c r="D47" s="176"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="164"/>
-      <c r="B48" s="163"/>
-      <c r="C48" s="181"/>
-      <c r="D48" s="177"/>
+      <c r="A48" s="163"/>
+      <c r="B48" s="162"/>
+      <c r="C48" s="180"/>
+      <c r="D48" s="176"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="164"/>
-      <c r="B49" s="163"/>
-      <c r="C49" s="171"/>
-      <c r="D49" s="177"/>
+      <c r="A49" s="163"/>
+      <c r="B49" s="162"/>
+      <c r="C49" s="170"/>
+      <c r="D49" s="176"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="164"/>
-      <c r="B50" s="163"/>
-      <c r="C50" s="171"/>
-      <c r="D50" s="178"/>
+      <c r="A50" s="163"/>
+      <c r="B50" s="162"/>
+      <c r="C50" s="170"/>
+      <c r="D50" s="177"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -31548,10 +31548,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="163" t="s">
+      <c r="A53" s="162" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="163" t="s">
+      <c r="B53" s="162" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -31562,8 +31562,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="163"/>
-      <c r="B54" s="163"/>
+      <c r="A54" s="162"/>
+      <c r="B54" s="162"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -31572,8 +31572,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="163"/>
-      <c r="B55" s="163"/>
+      <c r="A55" s="162"/>
+      <c r="B55" s="162"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -31582,9 +31582,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="163"/>
-      <c r="B56" s="163"/>
-      <c r="C56" s="182" t="s">
+      <c r="A56" s="162"/>
+      <c r="B56" s="162"/>
+      <c r="C56" s="181" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -31592,16 +31592,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="163"/>
-      <c r="B57" s="163"/>
-      <c r="C57" s="182"/>
+      <c r="A57" s="162"/>
+      <c r="B57" s="162"/>
+      <c r="C57" s="181"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="163"/>
-      <c r="B58" s="163"/>
+      <c r="A58" s="162"/>
+      <c r="B58" s="162"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -31610,8 +31610,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="163"/>
-      <c r="B59" s="163"/>
+      <c r="A59" s="162"/>
+      <c r="B59" s="162"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31620,9 +31620,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="163"/>
-      <c r="B60" s="163"/>
-      <c r="C60" s="182" t="s">
+      <c r="A60" s="162"/>
+      <c r="B60" s="162"/>
+      <c r="C60" s="181" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31630,25 +31630,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="163"/>
-      <c r="B61" s="163"/>
-      <c r="C61" s="182"/>
+      <c r="A61" s="162"/>
+      <c r="B61" s="162"/>
+      <c r="C61" s="181"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="163"/>
-      <c r="B62" s="163"/>
-      <c r="C62" s="182"/>
+      <c r="A62" s="162"/>
+      <c r="B62" s="162"/>
+      <c r="C62" s="181"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="163"/>
-      <c r="B63" s="163"/>
-      <c r="C63" s="183" t="s">
+      <c r="A63" s="162"/>
+      <c r="B63" s="162"/>
+      <c r="C63" s="182" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31656,30 +31656,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="163"/>
-      <c r="B64" s="163"/>
-      <c r="C64" s="183"/>
-      <c r="D64" s="165" t="s">
+      <c r="A64" s="162"/>
+      <c r="B64" s="162"/>
+      <c r="C64" s="182"/>
+      <c r="D64" s="164" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="163"/>
-      <c r="B65" s="163"/>
-      <c r="C65" s="183"/>
-      <c r="D65" s="165"/>
+      <c r="A65" s="162"/>
+      <c r="B65" s="162"/>
+      <c r="C65" s="182"/>
+      <c r="D65" s="164"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="163"/>
-      <c r="B66" s="163"/>
-      <c r="C66" s="183"/>
-      <c r="D66" s="165"/>
+      <c r="A66" s="162"/>
+      <c r="B66" s="162"/>
+      <c r="C66" s="182"/>
+      <c r="D66" s="164"/>
     </row>
     <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="163"/>
-      <c r="B67" s="163"/>
-      <c r="C67" s="183"/>
-      <c r="D67" s="165"/>
+      <c r="A67" s="162"/>
+      <c r="B67" s="162"/>
+      <c r="C67" s="182"/>
+      <c r="D67" s="164"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31776,10 +31776,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D206"/>
+  <dimension ref="A1:D207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="C169" sqref="C169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31813,10 +31813,10 @@
       <c r="D2" s="104"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="195" t="s">
+      <c r="A3" s="198" t="s">
         <v>433</v>
       </c>
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="196" t="s">
         <v>434</v>
       </c>
       <c r="C3" s="101" t="s">
@@ -31827,8 +31827,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="196"/>
-      <c r="B4" s="194"/>
+      <c r="A4" s="199"/>
+      <c r="B4" s="197"/>
       <c r="C4" s="100" t="s">
         <v>437</v>
       </c>
@@ -31837,10 +31837,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="195" t="s">
+      <c r="A5" s="198" t="s">
         <v>439</v>
       </c>
-      <c r="B5" s="199" t="s">
+      <c r="B5" s="192" t="s">
         <v>440</v>
       </c>
       <c r="C5" s="100"/>
@@ -31849,8 +31849,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="196"/>
-      <c r="B6" s="200"/>
+      <c r="A6" s="199"/>
+      <c r="B6" s="193"/>
       <c r="C6" s="100"/>
       <c r="D6" t="s">
         <v>490</v>
@@ -31865,44 +31865,44 @@
       <c r="D7" s="104"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="131" t="s">
+      <c r="A8" s="130" t="s">
         <v>442</v>
       </c>
       <c r="B8" s="107" t="s">
         <v>440</v>
       </c>
       <c r="C8" s="100"/>
-      <c r="D8" s="127" t="s">
+      <c r="D8" s="126" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="195" t="s">
+      <c r="A9" s="198" t="s">
         <v>280</v>
       </c>
-      <c r="B9" s="199" t="s">
+      <c r="B9" s="192" t="s">
         <v>440</v>
       </c>
       <c r="C9" s="100" t="s">
         <v>435</v>
       </c>
-      <c r="D9" s="127" t="s">
+      <c r="D9" s="126" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="220"/>
-      <c r="B10" s="207"/>
+      <c r="A10" s="219"/>
+      <c r="B10" s="208"/>
       <c r="C10" s="100" t="s">
         <v>445</v>
       </c>
-      <c r="D10" s="127" t="s">
+      <c r="D10" s="126" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="220"/>
-      <c r="B11" s="207"/>
+      <c r="A11" s="219"/>
+      <c r="B11" s="208"/>
       <c r="C11" s="100" t="s">
         <v>447</v>
       </c>
@@ -31911,8 +31911,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="196"/>
-      <c r="B12" s="200"/>
+      <c r="A12" s="199"/>
+      <c r="B12" s="193"/>
       <c r="C12" s="100" t="s">
         <v>435</v>
       </c>
@@ -31921,10 +31921,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="193" t="s">
+      <c r="A13" s="196" t="s">
         <v>453</v>
       </c>
-      <c r="B13" s="199" t="s">
+      <c r="B13" s="192" t="s">
         <v>440</v>
       </c>
       <c r="C13" s="100" t="s">
@@ -31935,8 +31935,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="221"/>
-      <c r="B14" s="207"/>
+      <c r="A14" s="220"/>
+      <c r="B14" s="208"/>
       <c r="C14" s="100" t="s">
         <v>454</v>
       </c>
@@ -31945,8 +31945,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="194"/>
-      <c r="B15" s="200"/>
+      <c r="A15" s="197"/>
+      <c r="B15" s="193"/>
       <c r="C15" s="100">
         <v>3.3</v>
       </c>
@@ -31955,14 +31955,14 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="131" t="s">
+      <c r="A16" s="130" t="s">
         <v>458</v>
       </c>
       <c r="B16" s="107" t="s">
         <v>440</v>
       </c>
       <c r="C16" s="100"/>
-      <c r="D16" s="132" t="s">
+      <c r="D16" s="131" t="s">
         <v>459</v>
       </c>
     </row>
@@ -31975,10 +31975,10 @@
       <c r="D17" s="104"/>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="201" t="s">
+      <c r="A18" s="202" t="s">
         <v>337</v>
       </c>
-      <c r="B18" s="202" t="s">
+      <c r="B18" s="203" t="s">
         <v>440</v>
       </c>
       <c r="C18" s="100" t="s">
@@ -31989,8 +31989,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="201"/>
-      <c r="B19" s="202"/>
+      <c r="A19" s="202"/>
+      <c r="B19" s="203"/>
       <c r="C19" s="100" t="s">
         <v>342</v>
       </c>
@@ -31999,8 +31999,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="201"/>
-      <c r="B20" s="202"/>
+      <c r="A20" s="202"/>
+      <c r="B20" s="203"/>
       <c r="C20" s="100" t="s">
         <v>338</v>
       </c>
@@ -32017,10 +32017,10 @@
       <c r="D21" s="104"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="208" t="s">
+      <c r="A22" s="209" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="203" t="s">
+      <c r="B22" s="204" t="s">
         <v>440</v>
       </c>
       <c r="C22" s="106"/>
@@ -32029,9 +32029,9 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="208"/>
-      <c r="B23" s="203"/>
-      <c r="C23" s="139" t="s">
+      <c r="A23" s="209"/>
+      <c r="B23" s="204"/>
+      <c r="C23" s="138" t="s">
         <v>234</v>
       </c>
       <c r="D23" s="108" t="s">
@@ -32039,9 +32039,9 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="208"/>
-      <c r="B24" s="203"/>
-      <c r="C24" s="142" t="s">
+      <c r="A24" s="209"/>
+      <c r="B24" s="204"/>
+      <c r="C24" s="141" t="s">
         <v>486</v>
       </c>
       <c r="D24" s="108" t="s">
@@ -32049,9 +32049,9 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="208"/>
-      <c r="B25" s="203"/>
-      <c r="C25" s="142" t="s">
+      <c r="A25" s="209"/>
+      <c r="B25" s="204"/>
+      <c r="C25" s="141" t="s">
         <v>486</v>
       </c>
       <c r="D25" s="108" t="s">
@@ -32059,10 +32059,10 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="215" t="s">
+      <c r="A26" s="214" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="199" t="s">
+      <c r="B26" s="192" t="s">
         <v>440</v>
       </c>
       <c r="C26" s="107" t="s">
@@ -32073,19 +32073,19 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="216"/>
-      <c r="B27" s="207"/>
-      <c r="C27" s="139" t="s">
+      <c r="A27" s="215"/>
+      <c r="B27" s="208"/>
+      <c r="C27" s="138" t="s">
         <v>464</v>
       </c>
-      <c r="D27" s="138" t="s">
+      <c r="D27" s="137" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="217"/>
-      <c r="B28" s="200"/>
-      <c r="C28" s="140" t="s">
+      <c r="A28" s="216"/>
+      <c r="B28" s="193"/>
+      <c r="C28" s="139" t="s">
         <v>483</v>
       </c>
       <c r="D28" s="110" t="s">
@@ -32133,10 +32133,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="208" t="s">
+      <c r="A32" s="209" t="s">
         <v>270</v>
       </c>
-      <c r="B32" s="203" t="s">
+      <c r="B32" s="204" t="s">
         <v>440</v>
       </c>
       <c r="C32" s="106"/>
@@ -32145,16 +32145,16 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="208"/>
-      <c r="B33" s="203"/>
+      <c r="A33" s="209"/>
+      <c r="B33" s="204"/>
       <c r="C33" s="106"/>
       <c r="D33" s="106" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="208"/>
-      <c r="B34" s="203"/>
+      <c r="A34" s="209"/>
+      <c r="B34" s="204"/>
       <c r="C34" s="111" t="s">
         <v>320</v>
       </c>
@@ -32163,8 +32163,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="208"/>
-      <c r="B35" s="203"/>
+      <c r="A35" s="209"/>
+      <c r="B35" s="204"/>
       <c r="C35" s="112" t="s">
         <v>399</v>
       </c>
@@ -32185,10 +32185,10 @@
       <c r="D36" s="106"/>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="204" t="s">
+      <c r="A37" s="205" t="s">
         <v>165</v>
       </c>
-      <c r="B37" s="199" t="s">
+      <c r="B37" s="192" t="s">
         <v>440</v>
       </c>
       <c r="C37" s="106"/>
@@ -32197,8 +32197,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="205"/>
-      <c r="B38" s="207"/>
+      <c r="A38" s="206"/>
+      <c r="B38" s="208"/>
       <c r="C38" s="112" t="s">
         <v>356</v>
       </c>
@@ -32207,8 +32207,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="205"/>
-      <c r="B39" s="207"/>
+      <c r="A39" s="206"/>
+      <c r="B39" s="208"/>
       <c r="C39" s="112" t="s">
         <v>354</v>
       </c>
@@ -32217,8 +32217,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="205"/>
-      <c r="B40" s="207"/>
+      <c r="A40" s="206"/>
+      <c r="B40" s="208"/>
       <c r="C40" s="115" t="s">
         <v>362</v>
       </c>
@@ -32227,8 +32227,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="205"/>
-      <c r="B41" s="207"/>
+      <c r="A41" s="206"/>
+      <c r="B41" s="208"/>
       <c r="C41" s="112" t="s">
         <v>354</v>
       </c>
@@ -32237,8 +32237,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="205"/>
-      <c r="B42" s="207"/>
+      <c r="A42" s="206"/>
+      <c r="B42" s="208"/>
       <c r="C42" s="112" t="s">
         <v>366</v>
       </c>
@@ -32247,8 +32247,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="205"/>
-      <c r="B43" s="207"/>
+      <c r="A43" s="206"/>
+      <c r="B43" s="208"/>
       <c r="C43" s="112" t="s">
         <v>354</v>
       </c>
@@ -32257,8 +32257,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="205"/>
-      <c r="B44" s="207"/>
+      <c r="A44" s="206"/>
+      <c r="B44" s="208"/>
       <c r="C44" s="112" t="s">
         <v>465</v>
       </c>
@@ -32267,9 +32267,9 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="205"/>
-      <c r="B45" s="207"/>
-      <c r="C45" s="136" t="s">
+      <c r="A45" s="206"/>
+      <c r="B45" s="208"/>
+      <c r="C45" s="135" t="s">
         <v>467</v>
       </c>
       <c r="D45" s="58" t="s">
@@ -32277,9 +32277,9 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="205"/>
-      <c r="B46" s="207"/>
-      <c r="C46" s="136" t="s">
+      <c r="A46" s="206"/>
+      <c r="B46" s="208"/>
+      <c r="C46" s="135" t="s">
         <v>354</v>
       </c>
       <c r="D46" s="58" t="s">
@@ -32287,9 +32287,9 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="205"/>
-      <c r="B47" s="207"/>
-      <c r="C47" s="141" t="s">
+      <c r="A47" s="206"/>
+      <c r="B47" s="208"/>
+      <c r="C47" s="140" t="s">
         <v>467</v>
       </c>
       <c r="D47" s="61" t="s">
@@ -32297,8 +32297,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="206"/>
-      <c r="B48" s="200"/>
+      <c r="A48" s="207"/>
+      <c r="B48" s="193"/>
       <c r="C48" s="112" t="s">
         <v>354</v>
       </c>
@@ -32347,10 +32347,10 @@
       <c r="D51" s="113"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="212" t="s">
+      <c r="A52" s="211" t="s">
         <v>364</v>
       </c>
-      <c r="B52" s="199" t="s">
+      <c r="B52" s="192" t="s">
         <v>440</v>
       </c>
       <c r="C52" s="112" t="s">
@@ -32359,8 +32359,8 @@
       <c r="D52" s="113"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="222"/>
-      <c r="B53" s="200"/>
+      <c r="A53" s="221"/>
+      <c r="B53" s="193"/>
       <c r="C53" s="112" t="s">
         <v>399</v>
       </c>
@@ -32377,10 +32377,10 @@
       <c r="D54" s="103"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="212" t="s">
+      <c r="A55" s="211" t="s">
         <v>236</v>
       </c>
-      <c r="B55" s="199" t="s">
+      <c r="B55" s="192" t="s">
         <v>440</v>
       </c>
       <c r="C55" s="106"/>
@@ -32389,24 +32389,24 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="213"/>
-      <c r="B56" s="207"/>
+      <c r="A56" s="212"/>
+      <c r="B56" s="208"/>
       <c r="C56" s="106"/>
       <c r="D56" s="106" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="213"/>
-      <c r="B57" s="207"/>
+      <c r="A57" s="212"/>
+      <c r="B57" s="208"/>
       <c r="C57" s="106"/>
       <c r="D57" s="106" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="213"/>
-      <c r="B58" s="207"/>
+      <c r="A58" s="212"/>
+      <c r="B58" s="208"/>
       <c r="C58" s="106" t="s">
         <v>295</v>
       </c>
@@ -32415,8 +32415,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="213"/>
-      <c r="B59" s="207"/>
+      <c r="A59" s="212"/>
+      <c r="B59" s="208"/>
       <c r="C59" s="106" t="s">
         <v>323</v>
       </c>
@@ -32425,8 +32425,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="213"/>
-      <c r="B60" s="207"/>
+      <c r="A60" s="212"/>
+      <c r="B60" s="208"/>
       <c r="C60" s="106" t="s">
         <v>368</v>
       </c>
@@ -32435,8 +32435,8 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="213"/>
-      <c r="B61" s="207"/>
+      <c r="A61" s="212"/>
+      <c r="B61" s="208"/>
       <c r="C61" s="119" t="s">
         <v>469</v>
       </c>
@@ -32445,8 +32445,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="213"/>
-      <c r="B62" s="207"/>
+      <c r="A62" s="212"/>
+      <c r="B62" s="208"/>
       <c r="C62" s="58" t="s">
         <v>37</v>
       </c>
@@ -32455,9 +32455,9 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="213"/>
-      <c r="B63" s="207"/>
-      <c r="C63" s="133" t="s">
+      <c r="A63" s="212"/>
+      <c r="B63" s="208"/>
+      <c r="C63" s="132" t="s">
         <v>354</v>
       </c>
       <c r="D63" s="58" t="s">
@@ -32465,9 +32465,9 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="213"/>
-      <c r="B64" s="207"/>
-      <c r="C64" s="133" t="s">
+      <c r="A64" s="212"/>
+      <c r="B64" s="208"/>
+      <c r="C64" s="132" t="s">
         <v>467</v>
       </c>
       <c r="D64" s="58" t="s">
@@ -32475,9 +32475,9 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="213"/>
-      <c r="B65" s="207"/>
-      <c r="C65" s="133" t="s">
+      <c r="A65" s="212"/>
+      <c r="B65" s="208"/>
+      <c r="C65" s="132" t="s">
         <v>368</v>
       </c>
       <c r="D65" s="58" t="s">
@@ -32485,9 +32485,9 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="222"/>
-      <c r="B66" s="200"/>
-      <c r="C66" s="133" t="s">
+      <c r="A66" s="221"/>
+      <c r="B66" s="193"/>
+      <c r="C66" s="132" t="s">
         <v>354</v>
       </c>
       <c r="D66" s="108" t="s">
@@ -32495,10 +32495,10 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="209" t="s">
+      <c r="A67" s="194" t="s">
         <v>27</v>
       </c>
-      <c r="B67" s="199" t="s">
+      <c r="B67" s="192" t="s">
         <v>440</v>
       </c>
       <c r="C67" s="106" t="s">
@@ -32510,7 +32510,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="210"/>
-      <c r="B68" s="207"/>
+      <c r="B68" s="208"/>
       <c r="C68" s="106"/>
       <c r="D68" s="106" t="s">
         <v>237</v>
@@ -32518,7 +32518,7 @@
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="210"/>
-      <c r="B69" s="207"/>
+      <c r="B69" s="208"/>
       <c r="C69" s="117" t="s">
         <v>324</v>
       </c>
@@ -32528,7 +32528,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="210"/>
-      <c r="B70" s="207"/>
+      <c r="B70" s="208"/>
       <c r="C70" s="117" t="s">
         <v>354</v>
       </c>
@@ -32538,7 +32538,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="210"/>
-      <c r="B71" s="207"/>
+      <c r="B71" s="208"/>
       <c r="C71" s="117" t="s">
         <v>362</v>
       </c>
@@ -32548,7 +32548,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="210"/>
-      <c r="B72" s="207"/>
+      <c r="B72" s="208"/>
       <c r="C72" s="117" t="s">
         <v>366</v>
       </c>
@@ -32558,7 +32558,7 @@
     </row>
     <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="210"/>
-      <c r="B73" s="207"/>
+      <c r="B73" s="208"/>
       <c r="C73" s="117" t="s">
         <v>376</v>
       </c>
@@ -32568,7 +32568,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="210"/>
-      <c r="B74" s="207"/>
+      <c r="B74" s="208"/>
       <c r="C74" s="109" t="s">
         <v>354</v>
       </c>
@@ -32578,7 +32578,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="210"/>
-      <c r="B75" s="207"/>
+      <c r="B75" s="208"/>
       <c r="C75" s="109" t="s">
         <v>465</v>
       </c>
@@ -32588,8 +32588,8 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="210"/>
-      <c r="B76" s="207"/>
-      <c r="C76" s="133" t="s">
+      <c r="B76" s="208"/>
+      <c r="C76" s="132" t="s">
         <v>467</v>
       </c>
       <c r="D76" s="58" t="s">
@@ -32598,8 +32598,8 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="210"/>
-      <c r="B77" s="207"/>
-      <c r="C77" s="133" t="s">
+      <c r="B77" s="208"/>
+      <c r="C77" s="132" t="s">
         <v>354</v>
       </c>
       <c r="D77" s="58" t="s">
@@ -32608,8 +32608,8 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="210"/>
-      <c r="B78" s="207"/>
-      <c r="C78" s="133" t="s">
+      <c r="B78" s="208"/>
+      <c r="C78" s="132" t="s">
         <v>467</v>
       </c>
       <c r="D78" s="58" t="s">
@@ -32618,8 +32618,8 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="210"/>
-      <c r="B79" s="207"/>
-      <c r="C79" s="133" t="s">
+      <c r="B79" s="208"/>
+      <c r="C79" s="132" t="s">
         <v>368</v>
       </c>
       <c r="D79" s="58" t="s">
@@ -32627,9 +32627,9 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="211"/>
-      <c r="B80" s="200"/>
-      <c r="C80" s="133" t="s">
+      <c r="A80" s="195"/>
+      <c r="B80" s="193"/>
+      <c r="C80" s="132" t="s">
         <v>354</v>
       </c>
       <c r="D80" s="108" t="s">
@@ -32637,13 +32637,13 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="215" t="s">
+      <c r="A81" s="214" t="s">
         <v>222</v>
       </c>
-      <c r="B81" s="199" t="s">
+      <c r="B81" s="192" t="s">
         <v>440</v>
       </c>
-      <c r="C81" s="223" t="s">
+      <c r="C81" s="222" t="s">
         <v>238</v>
       </c>
       <c r="D81" s="96" t="s">
@@ -32651,17 +32651,17 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="216"/>
-      <c r="B82" s="207"/>
-      <c r="C82" s="224"/>
+      <c r="A82" s="215"/>
+      <c r="B82" s="208"/>
+      <c r="C82" s="223"/>
       <c r="D82" s="113" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="216"/>
-      <c r="B83" s="207"/>
-      <c r="C83" s="214" t="s">
+      <c r="A83" s="215"/>
+      <c r="B83" s="208"/>
+      <c r="C83" s="213" t="s">
         <v>239</v>
       </c>
       <c r="D83" s="106" t="s">
@@ -32669,16 +32669,16 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A84" s="216"/>
-      <c r="B84" s="207"/>
-      <c r="C84" s="214"/>
+      <c r="A84" s="215"/>
+      <c r="B84" s="208"/>
+      <c r="C84" s="213"/>
       <c r="D84" s="119" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="216"/>
-      <c r="B85" s="207"/>
+      <c r="A85" s="215"/>
+      <c r="B85" s="208"/>
       <c r="C85" s="112" t="s">
         <v>302</v>
       </c>
@@ -32687,8 +32687,8 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="216"/>
-      <c r="B86" s="207"/>
+      <c r="A86" s="215"/>
+      <c r="B86" s="208"/>
       <c r="C86" s="112">
         <v>2.1</v>
       </c>
@@ -32697,8 +32697,8 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="216"/>
-      <c r="B87" s="207"/>
+      <c r="A87" s="215"/>
+      <c r="B87" s="208"/>
       <c r="C87" s="112" t="s">
         <v>238</v>
       </c>
@@ -32707,8 +32707,8 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="216"/>
-      <c r="B88" s="207"/>
+      <c r="A88" s="215"/>
+      <c r="B88" s="208"/>
       <c r="C88" s="112" t="s">
         <v>238</v>
       </c>
@@ -32717,8 +32717,8 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="216"/>
-      <c r="B89" s="207"/>
+      <c r="A89" s="215"/>
+      <c r="B89" s="208"/>
       <c r="C89" s="112" t="s">
         <v>238</v>
       </c>
@@ -32727,8 +32727,8 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="216"/>
-      <c r="B90" s="207"/>
+      <c r="A90" s="215"/>
+      <c r="B90" s="208"/>
       <c r="C90" s="120" t="s">
         <v>373</v>
       </c>
@@ -32737,8 +32737,8 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="216"/>
-      <c r="B91" s="207"/>
+      <c r="A91" s="215"/>
+      <c r="B91" s="208"/>
       <c r="C91" s="112">
         <v>2.1</v>
       </c>
@@ -32747,8 +32747,8 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="216"/>
-      <c r="B92" s="207"/>
+      <c r="A92" s="215"/>
+      <c r="B92" s="208"/>
       <c r="C92" s="112" t="s">
         <v>238</v>
       </c>
@@ -32757,8 +32757,8 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="216"/>
-      <c r="B93" s="207"/>
+      <c r="A93" s="215"/>
+      <c r="B93" s="208"/>
       <c r="C93" s="112" t="s">
         <v>238</v>
       </c>
@@ -32767,8 +32767,8 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="216"/>
-      <c r="B94" s="207"/>
+      <c r="A94" s="215"/>
+      <c r="B94" s="208"/>
       <c r="C94" s="112">
         <v>2.1</v>
       </c>
@@ -32777,10 +32777,10 @@
       </c>
     </row>
     <row r="95" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="209" t="s">
+      <c r="A95" s="194" t="s">
         <v>291</v>
       </c>
-      <c r="B95" s="199" t="s">
+      <c r="B95" s="192" t="s">
         <v>440</v>
       </c>
       <c r="C95" s="106" t="s">
@@ -32792,7 +32792,7 @@
     </row>
     <row r="96" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="210"/>
-      <c r="B96" s="207"/>
+      <c r="B96" s="208"/>
       <c r="C96" s="119" t="s">
         <v>276</v>
       </c>
@@ -32801,8 +32801,8 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="211"/>
-      <c r="B97" s="200"/>
+      <c r="A97" s="195"/>
+      <c r="B97" s="193"/>
       <c r="C97" s="106" t="s">
         <v>345</v>
       </c>
@@ -32811,10 +32811,10 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="212" t="s">
+      <c r="A98" s="211" t="s">
         <v>365</v>
       </c>
-      <c r="B98" s="199" t="s">
+      <c r="B98" s="192" t="s">
         <v>440</v>
       </c>
       <c r="C98" s="112" t="s">
@@ -32823,8 +32823,8 @@
       <c r="D98" s="106"/>
     </row>
     <row r="99" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="213"/>
-      <c r="B99" s="207"/>
+      <c r="A99" s="212"/>
+      <c r="B99" s="208"/>
       <c r="C99" s="112" t="s">
         <v>373</v>
       </c>
@@ -32833,8 +32833,8 @@
       </c>
     </row>
     <row r="100" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="213"/>
-      <c r="B100" s="207"/>
+      <c r="A100" s="212"/>
+      <c r="B100" s="208"/>
       <c r="C100" s="112">
         <v>2.1</v>
       </c>
@@ -32843,8 +32843,8 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="213"/>
-      <c r="B101" s="207"/>
+      <c r="A101" s="212"/>
+      <c r="B101" s="208"/>
       <c r="C101" s="112" t="s">
         <v>239</v>
       </c>
@@ -32853,8 +32853,8 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="213"/>
-      <c r="B102" s="207"/>
+      <c r="A102" s="212"/>
+      <c r="B102" s="208"/>
       <c r="C102" s="112" t="s">
         <v>238</v>
       </c>
@@ -32883,10 +32883,10 @@
       <c r="D104" s="113"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="215" t="s">
+      <c r="A105" s="214" t="s">
         <v>256</v>
       </c>
-      <c r="B105" s="199" t="s">
+      <c r="B105" s="192" t="s">
         <v>440</v>
       </c>
       <c r="C105" s="106"/>
@@ -32895,24 +32895,24 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="216"/>
-      <c r="B106" s="207"/>
+      <c r="A106" s="215"/>
+      <c r="B106" s="208"/>
       <c r="C106" s="106"/>
       <c r="D106" s="106" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="216"/>
-      <c r="B107" s="207"/>
+      <c r="A107" s="215"/>
+      <c r="B107" s="208"/>
       <c r="C107" s="106"/>
       <c r="D107" s="113" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="216"/>
-      <c r="B108" s="207"/>
+      <c r="A108" s="215"/>
+      <c r="B108" s="208"/>
       <c r="C108" s="106" t="s">
         <v>419</v>
       </c>
@@ -32921,8 +32921,8 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="216"/>
-      <c r="B109" s="207"/>
+      <c r="A109" s="215"/>
+      <c r="B109" s="208"/>
       <c r="C109" s="106" t="s">
         <v>424</v>
       </c>
@@ -32931,8 +32931,8 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="216"/>
-      <c r="B110" s="207"/>
+      <c r="A110" s="215"/>
+      <c r="B110" s="208"/>
       <c r="C110" s="106" t="s">
         <v>486</v>
       </c>
@@ -32941,10 +32941,10 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="208" t="s">
+      <c r="A111" s="209" t="s">
         <v>329</v>
       </c>
-      <c r="B111" s="203" t="s">
+      <c r="B111" s="204" t="s">
         <v>440</v>
       </c>
       <c r="C111" s="80" t="s">
@@ -32955,8 +32955,8 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="208"/>
-      <c r="B112" s="203"/>
+      <c r="A112" s="209"/>
+      <c r="B112" s="204"/>
       <c r="C112" s="106" t="s">
         <v>406</v>
       </c>
@@ -32965,46 +32965,46 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="208"/>
-      <c r="B113" s="203"/>
+      <c r="A113" s="209"/>
+      <c r="B113" s="204"/>
       <c r="C113" s="122" t="s">
         <v>409</v>
       </c>
-      <c r="D113" s="218" t="s">
+      <c r="D113" s="217" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="208"/>
-      <c r="B114" s="203"/>
+      <c r="A114" s="209"/>
+      <c r="B114" s="204"/>
       <c r="C114" s="122" t="s">
         <v>410</v>
       </c>
-      <c r="D114" s="219"/>
+      <c r="D114" s="218"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="208"/>
-      <c r="B115" s="203"/>
+      <c r="A115" s="209"/>
+      <c r="B115" s="204"/>
       <c r="C115" s="122" t="s">
         <v>411</v>
       </c>
-      <c r="D115" s="219"/>
+      <c r="D115" s="218"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="208"/>
-      <c r="B116" s="203"/>
+      <c r="A116" s="209"/>
+      <c r="B116" s="204"/>
       <c r="C116" s="122" t="s">
         <v>412</v>
       </c>
-      <c r="D116" s="219"/>
+      <c r="D116" s="218"/>
     </row>
     <row r="117" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="208"/>
-      <c r="B117" s="203"/>
+      <c r="A117" s="209"/>
+      <c r="B117" s="204"/>
       <c r="C117" s="122" t="s">
         <v>471</v>
       </c>
-      <c r="D117" s="134" t="s">
+      <c r="D117" s="133" t="s">
         <v>375</v>
       </c>
     </row>
@@ -33023,10 +33023,10 @@
       </c>
     </row>
     <row r="119" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="209" t="s">
+      <c r="A119" s="194" t="s">
         <v>32</v>
       </c>
-      <c r="B119" s="199" t="s">
+      <c r="B119" s="192" t="s">
         <v>440</v>
       </c>
       <c r="C119" s="106" t="s">
@@ -33038,7 +33038,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="210"/>
-      <c r="B120" s="207"/>
+      <c r="B120" s="208"/>
       <c r="C120" s="106" t="s">
         <v>265</v>
       </c>
@@ -33048,7 +33048,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="210"/>
-      <c r="B121" s="207"/>
+      <c r="B121" s="208"/>
       <c r="C121" s="106" t="s">
         <v>264</v>
       </c>
@@ -33058,7 +33058,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="210"/>
-      <c r="B122" s="207"/>
+      <c r="B122" s="208"/>
       <c r="C122" s="113" t="s">
         <v>272</v>
       </c>
@@ -33068,7 +33068,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="210"/>
-      <c r="B123" s="207"/>
+      <c r="B123" s="208"/>
       <c r="C123" s="106" t="s">
         <v>277</v>
       </c>
@@ -33078,7 +33078,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="210"/>
-      <c r="B124" s="207"/>
+      <c r="B124" s="208"/>
       <c r="C124" s="106" t="s">
         <v>278</v>
       </c>
@@ -33088,7 +33088,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="210"/>
-      <c r="B125" s="207"/>
+      <c r="B125" s="208"/>
       <c r="C125" s="113" t="s">
         <v>283</v>
       </c>
@@ -33098,7 +33098,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="210"/>
-      <c r="B126" s="207"/>
+      <c r="B126" s="208"/>
       <c r="C126" s="113" t="s">
         <v>297</v>
       </c>
@@ -33108,7 +33108,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="210"/>
-      <c r="B127" s="207"/>
+      <c r="B127" s="208"/>
       <c r="C127" s="113" t="s">
         <v>284</v>
       </c>
@@ -33118,7 +33118,7 @@
     </row>
     <row r="128" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="210"/>
-      <c r="B128" s="207"/>
+      <c r="B128" s="208"/>
       <c r="C128" s="123" t="s">
         <v>243</v>
       </c>
@@ -33128,7 +33128,7 @@
     </row>
     <row r="129" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A129" s="210"/>
-      <c r="B129" s="207"/>
+      <c r="B129" s="208"/>
       <c r="C129" s="117" t="s">
         <v>306</v>
       </c>
@@ -33138,7 +33138,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="210"/>
-      <c r="B130" s="207"/>
+      <c r="B130" s="208"/>
       <c r="C130" s="106" t="s">
         <v>307</v>
       </c>
@@ -33148,7 +33148,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="210"/>
-      <c r="B131" s="207"/>
+      <c r="B131" s="208"/>
       <c r="C131" s="113" t="s">
         <v>308</v>
       </c>
@@ -33158,7 +33158,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="210"/>
-      <c r="B132" s="207"/>
+      <c r="B132" s="208"/>
       <c r="C132" s="113" t="s">
         <v>310</v>
       </c>
@@ -33168,7 +33168,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="210"/>
-      <c r="B133" s="207"/>
+      <c r="B133" s="208"/>
       <c r="C133" s="113" t="s">
         <v>263</v>
       </c>
@@ -33178,7 +33178,7 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="210"/>
-      <c r="B134" s="207"/>
+      <c r="B134" s="208"/>
       <c r="C134" s="106" t="s">
         <v>313</v>
       </c>
@@ -33188,7 +33188,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="210"/>
-      <c r="B135" s="207"/>
+      <c r="B135" s="208"/>
       <c r="C135" s="113" t="s">
         <v>278</v>
       </c>
@@ -33198,7 +33198,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="210"/>
-      <c r="B136" s="207"/>
+      <c r="B136" s="208"/>
       <c r="C136" s="113" t="s">
         <v>314</v>
       </c>
@@ -33208,7 +33208,7 @@
     </row>
     <row r="137" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A137" s="210"/>
-      <c r="B137" s="207"/>
+      <c r="B137" s="208"/>
       <c r="C137" s="106"/>
       <c r="D137" s="97" t="s">
         <v>316</v>
@@ -33216,7 +33216,7 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="210"/>
-      <c r="B138" s="207"/>
+      <c r="B138" s="208"/>
       <c r="C138" s="113" t="s">
         <v>317</v>
       </c>
@@ -33226,7 +33226,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="210"/>
-      <c r="B139" s="207"/>
+      <c r="B139" s="208"/>
       <c r="C139" s="113" t="s">
         <v>263</v>
       </c>
@@ -33236,7 +33236,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="210"/>
-      <c r="B140" s="207"/>
+      <c r="B140" s="208"/>
       <c r="C140" s="113" t="s">
         <v>334</v>
       </c>
@@ -33246,7 +33246,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="210"/>
-      <c r="B141" s="207"/>
+      <c r="B141" s="208"/>
       <c r="C141" s="113" t="s">
         <v>335</v>
       </c>
@@ -33256,7 +33256,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="210"/>
-      <c r="B142" s="207"/>
+      <c r="B142" s="208"/>
       <c r="C142" s="113" t="s">
         <v>319</v>
       </c>
@@ -33266,7 +33266,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="210"/>
-      <c r="B143" s="207"/>
+      <c r="B143" s="208"/>
       <c r="C143" s="118" t="s">
         <v>340</v>
       </c>
@@ -33276,7 +33276,7 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="210"/>
-      <c r="B144" s="207"/>
+      <c r="B144" s="208"/>
       <c r="C144" s="113" t="s">
         <v>333</v>
       </c>
@@ -33286,7 +33286,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="210"/>
-      <c r="B145" s="207"/>
+      <c r="B145" s="208"/>
       <c r="C145" s="113" t="s">
         <v>348</v>
       </c>
@@ -33296,7 +33296,7 @@
     </row>
     <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="210"/>
-      <c r="B146" s="207"/>
+      <c r="B146" s="208"/>
       <c r="C146" s="101" t="s">
         <v>351</v>
       </c>
@@ -33306,7 +33306,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="210"/>
-      <c r="B147" s="207"/>
+      <c r="B147" s="208"/>
       <c r="C147" s="113" t="s">
         <v>352</v>
       </c>
@@ -33316,7 +33316,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="210"/>
-      <c r="B148" s="207"/>
+      <c r="B148" s="208"/>
       <c r="C148" s="113" t="s">
         <v>353</v>
       </c>
@@ -33326,7 +33326,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="210"/>
-      <c r="B149" s="207"/>
+      <c r="B149" s="208"/>
       <c r="C149" s="113" t="s">
         <v>359</v>
       </c>
@@ -33336,7 +33336,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="210"/>
-      <c r="B150" s="207"/>
+      <c r="B150" s="208"/>
       <c r="C150" s="113" t="s">
         <v>361</v>
       </c>
@@ -33346,7 +33346,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="210"/>
-      <c r="B151" s="207"/>
+      <c r="B151" s="208"/>
       <c r="C151" s="113" t="s">
         <v>367</v>
       </c>
@@ -33356,7 +33356,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="210"/>
-      <c r="B152" s="207"/>
+      <c r="B152" s="208"/>
       <c r="C152" s="113" t="s">
         <v>359</v>
       </c>
@@ -33366,7 +33366,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="210"/>
-      <c r="B153" s="207"/>
+      <c r="B153" s="208"/>
       <c r="C153" s="118" t="s">
         <v>380</v>
       </c>
@@ -33376,7 +33376,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="210"/>
-      <c r="B154" s="207"/>
+      <c r="B154" s="208"/>
       <c r="C154" s="106" t="s">
         <v>384</v>
       </c>
@@ -33386,7 +33386,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="210"/>
-      <c r="B155" s="207"/>
+      <c r="B155" s="208"/>
       <c r="C155" s="106" t="s">
         <v>387</v>
       </c>
@@ -33396,7 +33396,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="210"/>
-      <c r="B156" s="207"/>
+      <c r="B156" s="208"/>
       <c r="C156" s="106" t="s">
         <v>388</v>
       </c>
@@ -33406,7 +33406,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="210"/>
-      <c r="B157" s="207"/>
+      <c r="B157" s="208"/>
       <c r="C157" s="106" t="s">
         <v>389</v>
       </c>
@@ -33416,7 +33416,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="210"/>
-      <c r="B158" s="207"/>
+      <c r="B158" s="208"/>
       <c r="C158" s="106" t="s">
         <v>390</v>
       </c>
@@ -33426,7 +33426,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="210"/>
-      <c r="B159" s="207"/>
+      <c r="B159" s="208"/>
       <c r="C159" s="106" t="s">
         <v>391</v>
       </c>
@@ -33436,7 +33436,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="210"/>
-      <c r="B160" s="207"/>
+      <c r="B160" s="208"/>
       <c r="C160" s="106" t="s">
         <v>394</v>
       </c>
@@ -33446,7 +33446,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="210"/>
-      <c r="B161" s="207"/>
+      <c r="B161" s="208"/>
       <c r="C161" s="106" t="s">
         <v>404</v>
       </c>
@@ -33456,7 +33456,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="210"/>
-      <c r="B162" s="207"/>
+      <c r="B162" s="208"/>
       <c r="C162" s="106" t="s">
         <v>405</v>
       </c>
@@ -33466,7 +33466,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="210"/>
-      <c r="B163" s="207"/>
+      <c r="B163" s="208"/>
       <c r="C163" s="106" t="s">
         <v>422</v>
       </c>
@@ -33476,7 +33476,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="210"/>
-      <c r="B164" s="207"/>
+      <c r="B164" s="208"/>
       <c r="C164" s="106" t="s">
         <v>423</v>
       </c>
@@ -33486,7 +33486,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="210"/>
-      <c r="B165" s="207"/>
+      <c r="B165" s="208"/>
       <c r="C165" s="106" t="s">
         <v>426</v>
       </c>
@@ -33495,8 +33495,8 @@
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="211"/>
-      <c r="B166" s="200"/>
+      <c r="A166" s="195"/>
+      <c r="B166" s="193"/>
       <c r="C166" s="58" t="s">
         <v>472</v>
       </c>
@@ -33505,10 +33505,10 @@
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="125" t="s">
+      <c r="A167" s="194" t="s">
         <v>416</v>
       </c>
-      <c r="B167" s="107" t="s">
+      <c r="B167" s="192" t="s">
         <v>440</v>
       </c>
       <c r="C167" s="106" t="s">
@@ -33519,22 +33519,18 @@
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="109" t="s">
+      <c r="A168" s="195"/>
+      <c r="B168" s="193"/>
+      <c r="C168" s="118" t="s">
+        <v>493</v>
+      </c>
+      <c r="D168" s="118" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="109" t="s">
         <v>304</v>
-      </c>
-      <c r="B168" s="107" t="s">
-        <v>440</v>
-      </c>
-      <c r="C168" s="106" t="s">
-        <v>30</v>
-      </c>
-      <c r="D168" s="113" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="109" t="s">
-        <v>305</v>
       </c>
       <c r="B169" s="107" t="s">
         <v>440</v>
@@ -33546,402 +33542,412 @@
         <v>269</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="103" t="s">
+    <row r="170" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="109" t="s">
+        <v>305</v>
+      </c>
+      <c r="B170" s="107" t="s">
+        <v>440</v>
+      </c>
+      <c r="C170" s="106" t="s">
+        <v>30</v>
+      </c>
+      <c r="D170" s="113" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B170" s="103"/>
-      <c r="C170" s="103"/>
-      <c r="D170" s="104"/>
-    </row>
-    <row r="171" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="215" t="s">
+      <c r="B171" s="103"/>
+      <c r="C171" s="103"/>
+      <c r="D171" s="104"/>
+    </row>
+    <row r="172" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="214" t="s">
         <v>84</v>
       </c>
-      <c r="B171" s="199" t="s">
+      <c r="B172" s="192" t="s">
         <v>440</v>
       </c>
-      <c r="C171" s="106"/>
-      <c r="D171" s="80" t="s">
+      <c r="C172" s="106"/>
+      <c r="D172" s="80" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="216"/>
-      <c r="B172" s="207"/>
-      <c r="C172" s="107" t="s">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="215"/>
+      <c r="B173" s="208"/>
+      <c r="C173" s="107" t="s">
         <v>245</v>
       </c>
-      <c r="D172" s="106" t="s">
+      <c r="D173" s="106" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="216"/>
-      <c r="B173" s="207"/>
-      <c r="C173" s="107">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="215"/>
+      <c r="B174" s="208"/>
+      <c r="C174" s="107">
         <v>10.1</v>
-      </c>
-      <c r="D173" s="106" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="216"/>
-      <c r="B174" s="207"/>
-      <c r="C174" s="107">
-        <v>10.199999999999999</v>
       </c>
       <c r="D174" s="106" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="216"/>
-      <c r="B175" s="207"/>
-      <c r="C175" s="98" t="s">
+      <c r="A175" s="215"/>
+      <c r="B175" s="208"/>
+      <c r="C175" s="107">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D175" s="106" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="215"/>
+      <c r="B176" s="208"/>
+      <c r="C176" s="98" t="s">
         <v>288</v>
       </c>
-      <c r="D175" s="95" t="s">
+      <c r="D176" s="95" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="216"/>
-      <c r="B176" s="207"/>
-      <c r="C176" s="98" t="s">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="215"/>
+      <c r="B177" s="208"/>
+      <c r="C177" s="98" t="s">
         <v>370</v>
       </c>
-      <c r="D176" s="95" t="s">
+      <c r="D177" s="95" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="216"/>
-      <c r="B177" s="207"/>
-      <c r="C177" s="98" t="s">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="215"/>
+      <c r="B178" s="208"/>
+      <c r="C178" s="98" t="s">
         <v>117</v>
       </c>
-      <c r="D177" s="95" t="s">
+      <c r="D178" s="95" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="216"/>
-      <c r="B178" s="207"/>
-      <c r="C178" s="98" t="s">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="215"/>
+      <c r="B179" s="208"/>
+      <c r="C179" s="98" t="s">
         <v>417</v>
       </c>
-      <c r="D178" s="95" t="s">
+      <c r="D179" s="95" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="216"/>
-      <c r="B179" s="207"/>
-      <c r="C179" s="98" t="s">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="215"/>
+      <c r="B180" s="208"/>
+      <c r="C180" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="D179" s="95" t="s">
+      <c r="D180" s="95" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A180" s="217"/>
-      <c r="B180" s="200"/>
-      <c r="C180" s="98" t="s">
+    <row r="181" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A181" s="216"/>
+      <c r="B181" s="193"/>
+      <c r="C181" s="98" t="s">
         <v>473</v>
       </c>
-      <c r="D180" s="135" t="s">
+      <c r="D181" s="134" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="199" t="s">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="192" t="s">
         <v>246</v>
       </c>
-      <c r="B181" s="199" t="s">
+      <c r="B182" s="192" t="s">
         <v>440</v>
       </c>
-      <c r="C181" s="98"/>
-      <c r="D181" s="126" t="s">
+      <c r="C182" s="98"/>
+      <c r="D182" s="125" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="207"/>
-      <c r="B182" s="207"/>
-      <c r="C182" s="127" t="s">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="208"/>
+      <c r="B183" s="208"/>
+      <c r="C183" s="126" t="s">
         <v>428</v>
       </c>
-      <c r="D182" s="102" t="s">
+      <c r="D183" s="102" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="110" t="s">
+    <row r="184" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="110" t="s">
         <v>257</v>
       </c>
-      <c r="B183" s="107" t="s">
+      <c r="B184" s="107" t="s">
         <v>440</v>
       </c>
-      <c r="C183" s="107" t="s">
+      <c r="C184" s="107" t="s">
         <v>249</v>
       </c>
-      <c r="D183" s="113" t="s">
+      <c r="D184" s="113" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="128" t="s">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="127" t="s">
         <v>247</v>
       </c>
-      <c r="B184" s="103"/>
-      <c r="C184" s="129"/>
-      <c r="D184" s="129"/>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="215" t="s">
+      <c r="B185" s="103"/>
+      <c r="C185" s="128"/>
+      <c r="D185" s="128"/>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="214" t="s">
         <v>248</v>
       </c>
-      <c r="B185" s="199" t="s">
+      <c r="B186" s="192" t="s">
         <v>440</v>
       </c>
-      <c r="C185" s="130" t="s">
+      <c r="C186" s="129" t="s">
         <v>260</v>
       </c>
-      <c r="D185" s="106" t="s">
+      <c r="D186" s="106" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="217"/>
-      <c r="B186" s="200"/>
-      <c r="C186" s="130" t="s">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="216"/>
+      <c r="B187" s="193"/>
+      <c r="C187" s="129" t="s">
         <v>476</v>
       </c>
-      <c r="D186" s="106" t="s">
+      <c r="D187" s="106" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="215" t="s">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="214" t="s">
         <v>280</v>
       </c>
-      <c r="B187" s="199" t="s">
+      <c r="B188" s="192" t="s">
         <v>440</v>
       </c>
-      <c r="C187" s="95" t="s">
+      <c r="C188" s="95" t="s">
         <v>290</v>
       </c>
-      <c r="D187" s="106" t="s">
+      <c r="D188" s="106" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="216"/>
-      <c r="B188" s="207"/>
-      <c r="C188" s="106" t="s">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="215"/>
+      <c r="B189" s="208"/>
+      <c r="C189" s="106" t="s">
         <v>300</v>
       </c>
-      <c r="D188" s="113" t="s">
+      <c r="D189" s="113" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A189" s="216"/>
-      <c r="B189" s="207"/>
-      <c r="C189" s="130" t="s">
+    <row r="190" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A190" s="215"/>
+      <c r="B190" s="208"/>
+      <c r="C190" s="129" t="s">
         <v>281</v>
       </c>
-      <c r="D189" s="106" t="s">
+      <c r="D190" s="106" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="217"/>
-      <c r="B190" s="200"/>
-      <c r="C190" s="130" t="s">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="216"/>
+      <c r="B191" s="193"/>
+      <c r="C191" s="129" t="s">
         <v>21</v>
       </c>
-      <c r="D190" s="106" t="s">
+      <c r="D191" s="106" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A191" s="137" t="s">
+    <row r="192" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A192" s="136" t="s">
         <v>479</v>
       </c>
-      <c r="B191" s="139" t="s">
+      <c r="B192" s="138" t="s">
         <v>440</v>
       </c>
-      <c r="C191" s="130" t="s">
+      <c r="C192" s="129" t="s">
         <v>480</v>
       </c>
-      <c r="D191" s="109" t="s">
+      <c r="D192" s="109" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="129" t="s">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="128" t="s">
         <v>56</v>
       </c>
-      <c r="B192" s="129"/>
-      <c r="C192" s="129"/>
-      <c r="D192" s="129"/>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="215" t="s">
+      <c r="B193" s="128"/>
+      <c r="C193" s="128"/>
+      <c r="D193" s="128"/>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="214" t="s">
         <v>58</v>
       </c>
-      <c r="B193" s="199" t="s">
+      <c r="B194" s="192" t="s">
         <v>266</v>
       </c>
-      <c r="C193" s="130" t="s">
+      <c r="C194" s="129" t="s">
         <v>260</v>
       </c>
-      <c r="D193" s="106" t="s">
+      <c r="D194" s="106" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="216"/>
-      <c r="B194" s="207"/>
-      <c r="C194" s="130" t="s">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="215"/>
+      <c r="B195" s="208"/>
+      <c r="C195" s="129" t="s">
         <v>260</v>
       </c>
-      <c r="D194" s="106" t="s">
+      <c r="D195" s="106" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="217"/>
-      <c r="B195" s="200"/>
-      <c r="C195" s="106"/>
-      <c r="D195" s="106" t="s">
+    <row r="196" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="216"/>
+      <c r="B196" s="193"/>
+      <c r="C196" s="106"/>
+      <c r="D196" s="106" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A196" s="197" t="s">
+    <row r="197" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A197" s="200" t="s">
         <v>59</v>
       </c>
-      <c r="B196" s="199" t="s">
+      <c r="B197" s="192" t="s">
         <v>266</v>
       </c>
-      <c r="C196" s="119" t="s">
+      <c r="C197" s="119" t="s">
         <v>259</v>
       </c>
-      <c r="D196" s="106" t="s">
+      <c r="D197" s="106" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="198"/>
-      <c r="B197" s="200"/>
-      <c r="C197" s="119"/>
-      <c r="D197" s="106" t="s">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="201"/>
+      <c r="B198" s="193"/>
+      <c r="C198" s="119"/>
+      <c r="D198" s="106" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A198" s="197" t="s">
+    <row r="199" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A199" s="200" t="s">
         <v>286</v>
       </c>
-      <c r="B198" s="199" t="s">
+      <c r="B199" s="192" t="s">
         <v>266</v>
       </c>
-      <c r="C198" s="119"/>
-      <c r="D198" s="119" t="s">
+      <c r="C199" s="119"/>
+      <c r="D199" s="119" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="198"/>
-      <c r="B199" s="200"/>
-      <c r="C199" s="106"/>
-      <c r="D199" s="106" t="s">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="201"/>
+      <c r="B200" s="193"/>
+      <c r="C200" s="106"/>
+      <c r="D200" s="106" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A200" s="197" t="s">
+    <row r="201" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A201" s="200" t="s">
         <v>60</v>
       </c>
-      <c r="B200" s="199" t="s">
+      <c r="B201" s="192" t="s">
         <v>266</v>
       </c>
-      <c r="C200" s="119" t="s">
+      <c r="C201" s="119" t="s">
         <v>259</v>
       </c>
-      <c r="D200" s="106" t="s">
+      <c r="D201" s="106" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="198"/>
-      <c r="B201" s="200"/>
-      <c r="C201" s="106"/>
-      <c r="D201" s="106" t="s">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="201"/>
+      <c r="B202" s="193"/>
+      <c r="C202" s="106"/>
+      <c r="D202" s="106" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="129" t="s">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="128" t="s">
         <v>268</v>
       </c>
-      <c r="B202" s="129"/>
-      <c r="C202" s="129"/>
-      <c r="D202" s="129"/>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="106"/>
-      <c r="B203" s="107" t="s">
+      <c r="B203" s="128"/>
+      <c r="C203" s="128"/>
+      <c r="D203" s="128"/>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="106"/>
+      <c r="B204" s="107" t="s">
         <v>440</v>
       </c>
-      <c r="C203" s="106" t="s">
+      <c r="C204" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="D203" s="113" t="s">
+      <c r="D204" s="113" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="129" t="s">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="128" t="s">
         <v>274</v>
       </c>
-      <c r="B204" s="129"/>
-      <c r="C204" s="129"/>
-      <c r="D204" s="129"/>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="106"/>
-      <c r="B205" s="107" t="s">
-        <v>440</v>
-      </c>
-      <c r="C205" s="106" t="s">
-        <v>30</v>
-      </c>
-      <c r="D205" s="113" t="s">
-        <v>269</v>
-      </c>
+      <c r="B205" s="128"/>
+      <c r="C205" s="128"/>
+      <c r="D205" s="128"/>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="106"/>
-      <c r="B206" s="107"/>
+      <c r="B206" s="107" t="s">
+        <v>440</v>
+      </c>
       <c r="C206" s="106" t="s">
+        <v>30</v>
+      </c>
+      <c r="D206" s="113" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="106"/>
+      <c r="B207" s="107"/>
+      <c r="C207" s="106" t="s">
         <v>396</v>
       </c>
-      <c r="D206" s="113" t="s">
+      <c r="D207" s="113" t="s">
         <v>397</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="55">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
+  <mergeCells count="57">
     <mergeCell ref="D113:D116"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
@@ -33954,45 +33960,51 @@
     <mergeCell ref="A67:A80"/>
     <mergeCell ref="B67:B80"/>
     <mergeCell ref="C81:C82"/>
-    <mergeCell ref="C83:C84"/>
-    <mergeCell ref="A105:A110"/>
-    <mergeCell ref="A193:A195"/>
-    <mergeCell ref="B193:B195"/>
-    <mergeCell ref="A171:A180"/>
-    <mergeCell ref="B171:B180"/>
-    <mergeCell ref="A187:A190"/>
-    <mergeCell ref="B187:B190"/>
-    <mergeCell ref="A181:A182"/>
-    <mergeCell ref="B181:B182"/>
-    <mergeCell ref="A185:A186"/>
-    <mergeCell ref="B185:B186"/>
-    <mergeCell ref="B105:B110"/>
     <mergeCell ref="A119:A166"/>
     <mergeCell ref="B119:B166"/>
     <mergeCell ref="A81:A94"/>
-    <mergeCell ref="B81:B94"/>
-    <mergeCell ref="A95:A97"/>
-    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A194:A196"/>
+    <mergeCell ref="B194:B196"/>
+    <mergeCell ref="A172:A181"/>
+    <mergeCell ref="B172:B181"/>
+    <mergeCell ref="A188:A191"/>
+    <mergeCell ref="B188:B191"/>
+    <mergeCell ref="A182:A183"/>
+    <mergeCell ref="B182:B183"/>
+    <mergeCell ref="A186:A187"/>
+    <mergeCell ref="B186:B187"/>
     <mergeCell ref="A111:A117"/>
     <mergeCell ref="B111:B117"/>
     <mergeCell ref="A98:A102"/>
     <mergeCell ref="B98:B102"/>
+    <mergeCell ref="C83:C84"/>
+    <mergeCell ref="A105:A110"/>
+    <mergeCell ref="B105:B110"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="B81:B94"/>
+    <mergeCell ref="A95:A97"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="B167:B168"/>
+    <mergeCell ref="A167:A168"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A200:A201"/>
-    <mergeCell ref="B200:B201"/>
-    <mergeCell ref="A196:A197"/>
-    <mergeCell ref="B196:B197"/>
-    <mergeCell ref="A198:A199"/>
-    <mergeCell ref="B198:B199"/>
+    <mergeCell ref="A201:A202"/>
+    <mergeCell ref="B201:B202"/>
+    <mergeCell ref="A197:A198"/>
+    <mergeCell ref="B197:B198"/>
+    <mergeCell ref="A199:A200"/>
+    <mergeCell ref="B199:B200"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="A37:A48"/>
     <mergeCell ref="B37:B48"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A32:A35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ERR Updated Schema Publication Changelog
</commit_message>
<xml_diff>
--- a/PIT4/Schema Publication Changelog.xlsx
+++ b/PIT4/Schema Publication Changelog.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ademps03\IdeaProjects\paye-employers-documentation\src\main\resources\PIT4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\paye-employers-documentation\src\main\resources\PIT4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444F1246-0151-4B76-9731-F8DB4FBBBB00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F36D8E-6A4F-485B-B797-C59900BB7009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28485" windowHeight="14535" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v0.10" sheetId="1" r:id="rId1"/>
     <sheet name="v1.0 Milestone 1" sheetId="2" r:id="rId2"/>
     <sheet name="v1.0Milestone 2" sheetId="3" r:id="rId3"/>
     <sheet name="1.0 Release Candidate 2" sheetId="4" r:id="rId4"/>
+    <sheet name="ERR Milestone 1" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_Toc520203303" localSheetId="3">'1.0 Release Candidate 2'!$C$53</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="554">
   <si>
     <t>Document</t>
   </si>
@@ -3483,6 +3484,67 @@
   </si>
   <si>
     <t>Added note re. upper limit</t>
+  </si>
+  <si>
+    <t>1, 2.1, 3.1, 3.7</t>
+  </si>
+  <si>
+    <t>Added Enhanced Reporting Submission web
+service</t>
+  </si>
+  <si>
+    <t>Enhanced Reporting Submission Request: Data Items</t>
+  </si>
+  <si>
+    <t>EnhancedReportingSubmission</t>
+  </si>
+  <si>
+    <t>WarningExpenseBenefit</t>
+  </si>
+  <si>
+    <t>InvalidExpenseBenefit</t>
+  </si>
+  <si>
+    <t>EnhancedReportingAddress</t>
+  </si>
+  <si>
+    <t>EnhancedReportingEmployeeID</t>
+  </si>
+  <si>
+    <t>EnhancedReportingError</t>
+  </si>
+  <si>
+    <t>EnhancedReportingName</t>
+  </si>
+  <si>
+    <t>EnhancedReportingSubmissionResult</t>
+  </si>
+  <si>
+    <t>ExpenseBenefit</t>
+  </si>
+  <si>
+    <t>ExpenseBenefitSubmissionStatus</t>
+  </si>
+  <si>
+    <t>ExpenseBenefitSubmissionSummary</t>
+  </si>
+  <si>
+    <t>ExpenseBenefitSummary</t>
+  </si>
+  <si>
+    <t>Added definition</t>
+  </si>
+  <si>
+    <t>/enhanced_reporting</t>
+  </si>
+  <si>
+    <t>Added Enhanced Reporting endpoint for submissions</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>Updated "description": "List of validation warnings related to the payslip." to "description": "Details of validation check warning."</t>
   </si>
 </sst>
 </file>
@@ -4106,7 +4168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="244">
+  <cellXfs count="250">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -4514,6 +4576,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4775,11 +4851,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5154,7 +5230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -5184,12 +5260,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="161" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="156"/>
-      <c r="C2" s="156"/>
-      <c r="D2" s="157"/>
+      <c r="B2" s="162"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="163"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -5212,12 +5288,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="155" t="s">
+      <c r="A4" s="161" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="156"/>
-      <c r="C4" s="156"/>
-      <c r="D4" s="157"/>
+      <c r="B4" s="162"/>
+      <c r="C4" s="162"/>
+      <c r="D4" s="163"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -5257,10 +5333,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="158" t="s">
+      <c r="A7" s="164" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="161">
+      <c r="B7" s="167">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -5274,8 +5350,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="159"/>
-      <c r="B8" s="162"/>
+      <c r="A8" s="165"/>
+      <c r="B8" s="168"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -5287,8 +5363,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="159"/>
-      <c r="B9" s="162"/>
+      <c r="A9" s="165"/>
+      <c r="B9" s="168"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -5300,8 +5376,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="159"/>
-      <c r="B10" s="162"/>
+      <c r="A10" s="165"/>
+      <c r="B10" s="168"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -5313,8 +5389,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="159"/>
-      <c r="B11" s="162"/>
+      <c r="A11" s="165"/>
+      <c r="B11" s="168"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -5326,8 +5402,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="160"/>
-      <c r="B12" s="163"/>
+      <c r="A12" s="166"/>
+      <c r="B12" s="169"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -5339,10 +5415,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="166" t="s">
+      <c r="A13" s="172" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="161">
+      <c r="B13" s="167">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -5356,8 +5432,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="167"/>
-      <c r="B14" s="163"/>
+      <c r="A14" s="173"/>
+      <c r="B14" s="169"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -5403,12 +5479,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="155" t="s">
+      <c r="A17" s="161" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="156"/>
-      <c r="C17" s="156"/>
-      <c r="D17" s="157"/>
+      <c r="B17" s="162"/>
+      <c r="C17" s="162"/>
+      <c r="D17" s="163"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -5448,21 +5524,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="155" t="s">
+      <c r="A20" s="161" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="156"/>
-      <c r="C20" s="156"/>
-      <c r="D20" s="157"/>
+      <c r="B20" s="162"/>
+      <c r="C20" s="162"/>
+      <c r="D20" s="163"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="168" t="s">
+      <c r="A21" s="174" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="165">
+      <c r="B21" s="171">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -5476,8 +5552,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="169"/>
-      <c r="B22" s="163"/>
+      <c r="A22" s="175"/>
+      <c r="B22" s="169"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -5500,18 +5576,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="155" t="s">
+      <c r="A24" s="161" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="156"/>
-      <c r="C24" s="156"/>
-      <c r="D24" s="157"/>
+      <c r="B24" s="162"/>
+      <c r="C24" s="162"/>
+      <c r="D24" s="163"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="164" t="s">
+      <c r="A25" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="165">
+      <c r="B25" s="171">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -5525,8 +5601,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="159"/>
-      <c r="B26" s="162"/>
+      <c r="A26" s="165"/>
+      <c r="B26" s="168"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -5538,8 +5614,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="159"/>
-      <c r="B27" s="162"/>
+      <c r="A27" s="165"/>
+      <c r="B27" s="168"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -5551,8 +5627,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="159"/>
-      <c r="B28" s="162"/>
+      <c r="A28" s="165"/>
+      <c r="B28" s="168"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -5564,8 +5640,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="159"/>
-      <c r="B29" s="162"/>
+      <c r="A29" s="165"/>
+      <c r="B29" s="168"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -5577,8 +5653,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="159"/>
-      <c r="B30" s="162"/>
+      <c r="A30" s="165"/>
+      <c r="B30" s="168"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -5590,8 +5666,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="159"/>
-      <c r="B31" s="162"/>
+      <c r="A31" s="165"/>
+      <c r="B31" s="168"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -5603,8 +5679,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="160"/>
-      <c r="B32" s="163"/>
+      <c r="A32" s="166"/>
+      <c r="B32" s="169"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -5728,12 +5804,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="155" t="s">
+      <c r="A41" s="161" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="156"/>
-      <c r="C41" s="156"/>
-      <c r="D41" s="157"/>
+      <c r="B41" s="162"/>
+      <c r="C41" s="162"/>
+      <c r="D41" s="163"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -5834,7 +5910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFC79"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A30" sqref="A30:A38"/>
     </sheetView>
   </sheetViews>
@@ -5913,10 +5989,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="185" t="s">
+      <c r="A7" s="191" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="184" t="s">
+      <c r="B7" s="190" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5927,8 +6003,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="185"/>
-      <c r="B8" s="184"/>
+      <c r="A8" s="191"/>
+      <c r="B8" s="190"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5937,8 +6013,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="185"/>
-      <c r="B9" s="184"/>
+      <c r="A9" s="191"/>
+      <c r="B9" s="190"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5947,8 +6023,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="185"/>
-      <c r="B10" s="184"/>
+      <c r="A10" s="191"/>
+      <c r="B10" s="190"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5957,8 +6033,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="185"/>
-      <c r="B11" s="184"/>
+      <c r="A11" s="191"/>
+      <c r="B11" s="190"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5967,8 +6043,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="185"/>
-      <c r="B12" s="184"/>
+      <c r="A12" s="191"/>
+      <c r="B12" s="190"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5977,10 +6053,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="187" t="s">
+      <c r="A13" s="193" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="184" t="s">
+      <c r="B13" s="190" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5991,8 +6067,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="187"/>
-      <c r="B14" s="184"/>
+      <c r="A14" s="193"/>
+      <c r="B14" s="190"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -6001,8 +6077,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="187"/>
-      <c r="B15" s="184"/>
+      <c r="A15" s="193"/>
+      <c r="B15" s="190"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -6011,10 +6087,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="170" t="s">
+      <c r="A16" s="176" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="179" t="s">
+      <c r="B16" s="185" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -6025,8 +6101,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="170"/>
-      <c r="B17" s="179"/>
+      <c r="A17" s="176"/>
+      <c r="B17" s="185"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -6035,8 +6111,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="170"/>
-      <c r="B18" s="179"/>
+      <c r="A18" s="176"/>
+      <c r="B18" s="185"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -6045,8 +6121,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="170"/>
-      <c r="B19" s="179"/>
+      <c r="A19" s="176"/>
+      <c r="B19" s="185"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -6055,8 +6131,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="170"/>
-      <c r="B20" s="179"/>
+      <c r="A20" s="176"/>
+      <c r="B20" s="185"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -6065,8 +6141,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="170"/>
-      <c r="B21" s="179"/>
+      <c r="A21" s="176"/>
+      <c r="B21" s="185"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -6075,8 +6151,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="170"/>
-      <c r="B22" s="179"/>
+      <c r="A22" s="176"/>
+      <c r="B22" s="185"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -6085,8 +6161,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="170"/>
-      <c r="B23" s="179"/>
+      <c r="A23" s="176"/>
+      <c r="B23" s="185"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -6095,26 +6171,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="170"/>
-      <c r="B24" s="179"/>
-      <c r="C24" s="170" t="s">
+      <c r="A24" s="176"/>
+      <c r="B24" s="185"/>
+      <c r="C24" s="176" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="171" t="s">
+      <c r="D24" s="177" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="170"/>
-      <c r="B25" s="179"/>
-      <c r="C25" s="170"/>
-      <c r="D25" s="171"/>
+      <c r="A25" s="176"/>
+      <c r="B25" s="185"/>
+      <c r="C25" s="176"/>
+      <c r="D25" s="177"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="185" t="s">
+      <c r="A26" s="191" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="184" t="s">
+      <c r="B26" s="190" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -6125,8 +6201,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="185"/>
-      <c r="B27" s="184"/>
+      <c r="A27" s="191"/>
+      <c r="B27" s="190"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -6153,28 +6229,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="186" t="s">
+      <c r="A30" s="192" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="184" t="s">
+      <c r="B30" s="190" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="170" t="s">
+      <c r="C30" s="176" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="174" t="s">
+      <c r="D30" s="180" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="186"/>
-      <c r="B31" s="184"/>
-      <c r="C31" s="170"/>
-      <c r="D31" s="174"/>
+      <c r="A31" s="192"/>
+      <c r="B31" s="190"/>
+      <c r="C31" s="176"/>
+      <c r="D31" s="180"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="186"/>
-      <c r="B32" s="184"/>
+      <c r="A32" s="192"/>
+      <c r="B32" s="190"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -6183,8 +6259,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="186"/>
-      <c r="B33" s="184"/>
+      <c r="A33" s="192"/>
+      <c r="B33" s="190"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -6193,8 +6269,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="186"/>
-      <c r="B34" s="184"/>
+      <c r="A34" s="192"/>
+      <c r="B34" s="190"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -6203,8 +6279,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="186"/>
-      <c r="B35" s="184"/>
+      <c r="A35" s="192"/>
+      <c r="B35" s="190"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -6213,8 +6289,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="186"/>
-      <c r="B36" s="184"/>
+      <c r="A36" s="192"/>
+      <c r="B36" s="190"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -6223,26 +6299,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="186"/>
-      <c r="B37" s="184"/>
-      <c r="C37" s="175" t="s">
+      <c r="A37" s="192"/>
+      <c r="B37" s="190"/>
+      <c r="C37" s="181" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="177" t="s">
+      <c r="D37" s="183" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="186"/>
-      <c r="B38" s="184"/>
-      <c r="C38" s="176"/>
-      <c r="D38" s="177"/>
+      <c r="A38" s="192"/>
+      <c r="B38" s="190"/>
+      <c r="C38" s="182"/>
+      <c r="D38" s="183"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="185" t="s">
+      <c r="A39" s="191" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="184" t="s">
+      <c r="B39" s="190" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -6253,8 +6329,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="185"/>
-      <c r="B40" s="184"/>
+      <c r="A40" s="191"/>
+      <c r="B40" s="190"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -6281,10 +6357,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="186" t="s">
+      <c r="A43" s="192" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="184" t="s">
+      <c r="B43" s="190" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -6293,8 +6369,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="186"/>
-      <c r="B44" s="184"/>
+      <c r="A44" s="192"/>
+      <c r="B44" s="190"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -6303,10 +6379,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="181" t="s">
+      <c r="A45" s="187" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="184" t="s">
+      <c r="B45" s="190" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -6315,8 +6391,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="182"/>
-      <c r="B46" s="184"/>
+      <c r="A46" s="188"/>
+      <c r="B46" s="190"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -6325,8 +6401,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="182"/>
-      <c r="B47" s="184"/>
+      <c r="A47" s="188"/>
+      <c r="B47" s="190"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -6335,8 +6411,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="183"/>
-      <c r="B48" s="184"/>
+      <c r="A48" s="189"/>
+      <c r="B48" s="190"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -6345,10 +6421,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="179" t="s">
+      <c r="A49" s="185" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="179" t="s">
+      <c r="B49" s="185" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -10452,8 +10528,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="179"/>
-      <c r="B50" s="179"/>
+      <c r="A50" s="185"/>
+      <c r="B50" s="185"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -14557,8 +14633,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="179"/>
-      <c r="B51" s="179"/>
+      <c r="A51" s="185"/>
+      <c r="B51" s="185"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -18662,8 +18738,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="179"/>
-      <c r="B52" s="179"/>
+      <c r="A52" s="185"/>
+      <c r="B52" s="185"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -22767,12 +22843,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="179"/>
-      <c r="B53" s="179"/>
-      <c r="C53" s="173" t="s">
+      <c r="A53" s="185"/>
+      <c r="B53" s="185"/>
+      <c r="C53" s="179" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="174" t="s">
+      <c r="D53" s="180" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26872,10 +26948,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="179"/>
-      <c r="B54" s="179"/>
-      <c r="C54" s="173"/>
-      <c r="D54" s="174"/>
+      <c r="A54" s="185"/>
+      <c r="B54" s="185"/>
+      <c r="C54" s="179"/>
+      <c r="D54" s="180"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30993,10 +31069,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="178" t="s">
+      <c r="A57" s="184" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="179" t="s">
+      <c r="B57" s="185" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -31007,8 +31083,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="178"/>
-      <c r="B58" s="179"/>
+      <c r="A58" s="184"/>
+      <c r="B58" s="185"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -31017,8 +31093,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="178"/>
-      <c r="B59" s="179"/>
+      <c r="A59" s="184"/>
+      <c r="B59" s="185"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -31027,8 +31103,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="178"/>
-      <c r="B60" s="179"/>
+      <c r="A60" s="184"/>
+      <c r="B60" s="185"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -31037,8 +31113,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="178"/>
-      <c r="B61" s="179"/>
+      <c r="A61" s="184"/>
+      <c r="B61" s="185"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -31047,8 +31123,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="178"/>
-      <c r="B62" s="179"/>
+      <c r="A62" s="184"/>
+      <c r="B62" s="185"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -31057,8 +31133,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="178"/>
-      <c r="B63" s="179"/>
+      <c r="A63" s="184"/>
+      <c r="B63" s="185"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -31067,16 +31143,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="178"/>
-      <c r="B64" s="179"/>
+      <c r="A64" s="184"/>
+      <c r="B64" s="185"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="178"/>
-      <c r="B65" s="179"/>
+      <c r="A65" s="184"/>
+      <c r="B65" s="185"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -31085,16 +31161,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="178"/>
-      <c r="B66" s="179"/>
+      <c r="A66" s="184"/>
+      <c r="B66" s="185"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="178"/>
-      <c r="B67" s="179"/>
+      <c r="A67" s="184"/>
+      <c r="B67" s="185"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -31103,8 +31179,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="178"/>
-      <c r="B68" s="179"/>
+      <c r="A68" s="184"/>
+      <c r="B68" s="185"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -31113,8 +31189,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="178"/>
-      <c r="B69" s="179"/>
+      <c r="A69" s="184"/>
+      <c r="B69" s="185"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -31123,8 +31199,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="178"/>
-      <c r="B70" s="179"/>
+      <c r="A70" s="184"/>
+      <c r="B70" s="185"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -31133,8 +31209,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="178"/>
-      <c r="B71" s="179"/>
+      <c r="A71" s="184"/>
+      <c r="B71" s="185"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -31143,8 +31219,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="178"/>
-      <c r="B72" s="179"/>
+      <c r="A72" s="184"/>
+      <c r="B72" s="185"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -31153,16 +31229,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="178"/>
-      <c r="B73" s="179"/>
+      <c r="A73" s="184"/>
+      <c r="B73" s="185"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="178"/>
-      <c r="B74" s="179"/>
+      <c r="A74" s="184"/>
+      <c r="B74" s="185"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -31171,18 +31247,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="178"/>
-      <c r="B75" s="179"/>
-      <c r="C75" s="172"/>
-      <c r="D75" s="180" t="s">
+      <c r="A75" s="184"/>
+      <c r="B75" s="185"/>
+      <c r="C75" s="178"/>
+      <c r="D75" s="186" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="178"/>
-      <c r="B76" s="179"/>
-      <c r="C76" s="172"/>
-      <c r="D76" s="180"/>
+      <c r="A76" s="184"/>
+      <c r="B76" s="185"/>
+      <c r="C76" s="178"/>
+      <c r="D76" s="186"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -31306,10 +31382,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="185" t="s">
+      <c r="A4" s="191" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="184" t="s">
+      <c r="B4" s="190" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -31320,133 +31396,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="185"/>
-      <c r="B5" s="184"/>
-      <c r="C5" s="195" t="s">
+      <c r="A5" s="191"/>
+      <c r="B5" s="190"/>
+      <c r="C5" s="201" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="194" t="s">
+      <c r="D5" s="200" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="185"/>
-      <c r="B6" s="184"/>
-      <c r="C6" s="195"/>
-      <c r="D6" s="194"/>
+      <c r="A6" s="191"/>
+      <c r="B6" s="190"/>
+      <c r="C6" s="201"/>
+      <c r="D6" s="200"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="185"/>
-      <c r="B7" s="184"/>
+      <c r="A7" s="191"/>
+      <c r="B7" s="190"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="185"/>
-      <c r="B8" s="184"/>
+      <c r="A8" s="191"/>
+      <c r="B8" s="190"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="185"/>
-      <c r="B9" s="184"/>
+      <c r="A9" s="191"/>
+      <c r="B9" s="190"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="187" t="s">
+      <c r="A10" s="193" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="184" t="s">
+      <c r="B10" s="190" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="197"/>
-      <c r="D10" s="194" t="s">
+      <c r="C10" s="203"/>
+      <c r="D10" s="200" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="187"/>
-      <c r="B11" s="184"/>
-      <c r="C11" s="197"/>
-      <c r="D11" s="194"/>
+      <c r="A11" s="193"/>
+      <c r="B11" s="190"/>
+      <c r="C11" s="203"/>
+      <c r="D11" s="200"/>
     </row>
     <row r="12" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="187"/>
-      <c r="B12" s="184"/>
-      <c r="C12" s="197"/>
-      <c r="D12" s="194"/>
+      <c r="A12" s="193"/>
+      <c r="B12" s="190"/>
+      <c r="C12" s="203"/>
+      <c r="D12" s="200"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="170" t="s">
+      <c r="A13" s="176" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="179" t="s">
+      <c r="B13" s="185" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="196"/>
-      <c r="D13" s="194" t="s">
+      <c r="C13" s="202"/>
+      <c r="D13" s="200" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="170"/>
-      <c r="B14" s="179"/>
-      <c r="C14" s="196"/>
-      <c r="D14" s="194"/>
+      <c r="A14" s="176"/>
+      <c r="B14" s="185"/>
+      <c r="C14" s="202"/>
+      <c r="D14" s="200"/>
     </row>
     <row r="15" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="170"/>
-      <c r="B15" s="179"/>
-      <c r="C15" s="196"/>
+      <c r="A15" s="176"/>
+      <c r="B15" s="185"/>
+      <c r="C15" s="202"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="170"/>
-      <c r="B16" s="179"/>
-      <c r="C16" s="196"/>
+      <c r="A16" s="176"/>
+      <c r="B16" s="185"/>
+      <c r="C16" s="202"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="170"/>
-      <c r="B17" s="179"/>
-      <c r="C17" s="196"/>
+      <c r="A17" s="176"/>
+      <c r="B17" s="185"/>
+      <c r="C17" s="202"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="170"/>
-      <c r="B18" s="179"/>
-      <c r="C18" s="196"/>
+      <c r="A18" s="176"/>
+      <c r="B18" s="185"/>
+      <c r="C18" s="202"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="170"/>
-      <c r="B19" s="179"/>
-      <c r="C19" s="196"/>
+      <c r="A19" s="176"/>
+      <c r="B19" s="185"/>
+      <c r="C19" s="202"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="170"/>
-      <c r="B20" s="179"/>
-      <c r="C20" s="196"/>
+      <c r="A20" s="176"/>
+      <c r="B20" s="185"/>
+      <c r="C20" s="202"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="170"/>
-      <c r="B21" s="179"/>
-      <c r="C21" s="196"/>
+      <c r="A21" s="176"/>
+      <c r="B21" s="185"/>
+      <c r="C21" s="202"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="170"/>
-      <c r="B22" s="179"/>
-      <c r="C22" s="196"/>
+      <c r="A22" s="176"/>
+      <c r="B22" s="185"/>
+      <c r="C22" s="202"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="170"/>
-      <c r="B23" s="179"/>
-      <c r="C23" s="196"/>
+      <c r="A23" s="176"/>
+      <c r="B23" s="185"/>
+      <c r="C23" s="202"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -31544,10 +31620,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="188" t="s">
+      <c r="A32" s="194" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="191" t="s">
+      <c r="B32" s="197" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -31558,26 +31634,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="189"/>
-      <c r="B33" s="192"/>
+      <c r="A33" s="195"/>
+      <c r="B33" s="198"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="189"/>
-      <c r="B34" s="192"/>
+      <c r="A34" s="195"/>
+      <c r="B34" s="198"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="189"/>
-      <c r="B35" s="192"/>
+      <c r="A35" s="195"/>
+      <c r="B35" s="198"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="190"/>
-      <c r="B36" s="193"/>
+      <c r="A36" s="196"/>
+      <c r="B36" s="199"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -31606,10 +31682,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="186" t="s">
+      <c r="A39" s="192" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="184" t="s">
+      <c r="B39" s="190" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -31620,8 +31696,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="186"/>
-      <c r="B40" s="184"/>
+      <c r="A40" s="192"/>
+      <c r="B40" s="190"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -31630,84 +31706,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="185" t="s">
+      <c r="A41" s="191" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="184" t="s">
+      <c r="B41" s="190" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="197" t="s">
+      <c r="C41" s="203" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="170" t="s">
+      <c r="D41" s="176" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="185"/>
-      <c r="B42" s="184"/>
-      <c r="C42" s="197"/>
-      <c r="D42" s="170"/>
+      <c r="A42" s="191"/>
+      <c r="B42" s="190"/>
+      <c r="C42" s="203"/>
+      <c r="D42" s="176"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="185"/>
-      <c r="B43" s="184"/>
-      <c r="C43" s="197" t="s">
+      <c r="A43" s="191"/>
+      <c r="B43" s="190"/>
+      <c r="C43" s="203" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="180" t="s">
+      <c r="D43" s="186" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="185"/>
-      <c r="B44" s="184"/>
-      <c r="C44" s="197"/>
-      <c r="D44" s="180"/>
+      <c r="A44" s="191"/>
+      <c r="B44" s="190"/>
+      <c r="C44" s="203"/>
+      <c r="D44" s="186"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="178" t="s">
+      <c r="A45" s="184" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="179" t="s">
+      <c r="B45" s="185" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="201"/>
+      <c r="C45" s="207"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="178"/>
-      <c r="B46" s="179"/>
-      <c r="C46" s="202"/>
-      <c r="D46" s="198" t="s">
+      <c r="A46" s="184"/>
+      <c r="B46" s="185"/>
+      <c r="C46" s="208"/>
+      <c r="D46" s="204" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="178"/>
-      <c r="B47" s="179"/>
-      <c r="C47" s="202"/>
-      <c r="D47" s="199"/>
+      <c r="A47" s="184"/>
+      <c r="B47" s="185"/>
+      <c r="C47" s="208"/>
+      <c r="D47" s="205"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="178"/>
-      <c r="B48" s="179"/>
-      <c r="C48" s="203"/>
-      <c r="D48" s="199"/>
+      <c r="A48" s="184"/>
+      <c r="B48" s="185"/>
+      <c r="C48" s="209"/>
+      <c r="D48" s="205"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="178"/>
-      <c r="B49" s="179"/>
-      <c r="C49" s="173"/>
-      <c r="D49" s="199"/>
+      <c r="A49" s="184"/>
+      <c r="B49" s="185"/>
+      <c r="C49" s="179"/>
+      <c r="D49" s="205"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="178"/>
-      <c r="B50" s="179"/>
-      <c r="C50" s="173"/>
-      <c r="D50" s="200"/>
+      <c r="A50" s="184"/>
+      <c r="B50" s="185"/>
+      <c r="C50" s="179"/>
+      <c r="D50" s="206"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -31730,10 +31806,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="179" t="s">
+      <c r="A53" s="185" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="179" t="s">
+      <c r="B53" s="185" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -31744,8 +31820,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="179"/>
-      <c r="B54" s="179"/>
+      <c r="A54" s="185"/>
+      <c r="B54" s="185"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -31754,8 +31830,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="179"/>
-      <c r="B55" s="179"/>
+      <c r="A55" s="185"/>
+      <c r="B55" s="185"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -31764,9 +31840,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="179"/>
-      <c r="B56" s="179"/>
-      <c r="C56" s="204" t="s">
+      <c r="A56" s="185"/>
+      <c r="B56" s="185"/>
+      <c r="C56" s="210" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -31774,16 +31850,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="179"/>
-      <c r="B57" s="179"/>
-      <c r="C57" s="204"/>
+      <c r="A57" s="185"/>
+      <c r="B57" s="185"/>
+      <c r="C57" s="210"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="179"/>
-      <c r="B58" s="179"/>
+      <c r="A58" s="185"/>
+      <c r="B58" s="185"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -31792,8 +31868,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="179"/>
-      <c r="B59" s="179"/>
+      <c r="A59" s="185"/>
+      <c r="B59" s="185"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31802,9 +31878,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="179"/>
-      <c r="B60" s="179"/>
-      <c r="C60" s="204" t="s">
+      <c r="A60" s="185"/>
+      <c r="B60" s="185"/>
+      <c r="C60" s="210" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31812,25 +31888,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="179"/>
-      <c r="B61" s="179"/>
-      <c r="C61" s="204"/>
+      <c r="A61" s="185"/>
+      <c r="B61" s="185"/>
+      <c r="C61" s="210"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="179"/>
-      <c r="B62" s="179"/>
-      <c r="C62" s="204"/>
+      <c r="A62" s="185"/>
+      <c r="B62" s="185"/>
+      <c r="C62" s="210"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="179"/>
-      <c r="B63" s="179"/>
-      <c r="C63" s="197" t="s">
+      <c r="A63" s="185"/>
+      <c r="B63" s="185"/>
+      <c r="C63" s="203" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31838,30 +31914,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="179"/>
-      <c r="B64" s="179"/>
-      <c r="C64" s="197"/>
-      <c r="D64" s="180" t="s">
+      <c r="A64" s="185"/>
+      <c r="B64" s="185"/>
+      <c r="C64" s="203"/>
+      <c r="D64" s="186" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="179"/>
-      <c r="B65" s="179"/>
-      <c r="C65" s="197"/>
-      <c r="D65" s="180"/>
+      <c r="A65" s="185"/>
+      <c r="B65" s="185"/>
+      <c r="C65" s="203"/>
+      <c r="D65" s="186"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="179"/>
-      <c r="B66" s="179"/>
-      <c r="C66" s="197"/>
-      <c r="D66" s="180"/>
+      <c r="A66" s="185"/>
+      <c r="B66" s="185"/>
+      <c r="C66" s="203"/>
+      <c r="D66" s="186"/>
     </row>
     <row r="67" spans="1:4" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="179"/>
-      <c r="B67" s="179"/>
-      <c r="C67" s="197"/>
-      <c r="D67" s="180"/>
+      <c r="A67" s="185"/>
+      <c r="B67" s="185"/>
+      <c r="C67" s="203"/>
+      <c r="D67" s="186"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31960,8 +32036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111:A129"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95:A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31995,10 +32071,10 @@
       <c r="D2" s="104"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="205" t="s">
+      <c r="A3" s="211" t="s">
         <v>432</v>
       </c>
-      <c r="B3" s="205" t="s">
+      <c r="B3" s="211" t="s">
         <v>433</v>
       </c>
       <c r="C3" s="101" t="s">
@@ -32009,8 +32085,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="206"/>
-      <c r="B4" s="206"/>
+      <c r="A4" s="212"/>
+      <c r="B4" s="212"/>
       <c r="C4" s="100" t="s">
         <v>436</v>
       </c>
@@ -32019,8 +32095,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="207"/>
-      <c r="B5" s="207"/>
+      <c r="A5" s="213"/>
+      <c r="B5" s="213"/>
       <c r="C5" s="100" t="s">
         <v>436</v>
       </c>
@@ -32029,10 +32105,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="213" t="s">
+      <c r="A6" s="219" t="s">
         <v>438</v>
       </c>
-      <c r="B6" s="208" t="s">
+      <c r="B6" s="214" t="s">
         <v>439</v>
       </c>
       <c r="C6" s="100"/>
@@ -32041,32 +32117,32 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="214"/>
-      <c r="B7" s="209"/>
+      <c r="A7" s="220"/>
+      <c r="B7" s="215"/>
       <c r="C7" s="100"/>
       <c r="D7" s="58" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="214"/>
-      <c r="B8" s="209"/>
+      <c r="A8" s="220"/>
+      <c r="B8" s="215"/>
       <c r="C8" s="100"/>
       <c r="D8" s="140" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="214"/>
-      <c r="B9" s="209"/>
+      <c r="A9" s="220"/>
+      <c r="B9" s="215"/>
       <c r="C9" s="100"/>
       <c r="D9" s="140" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="215"/>
-      <c r="B10" s="210"/>
+      <c r="A10" s="221"/>
+      <c r="B10" s="216"/>
       <c r="C10" s="100" t="s">
         <v>498</v>
       </c>
@@ -32075,10 +32151,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="205" t="s">
+      <c r="A11" s="211" t="s">
         <v>525</v>
       </c>
-      <c r="B11" s="208" t="s">
+      <c r="B11" s="214" t="s">
         <v>433</v>
       </c>
       <c r="C11" s="100" t="s">
@@ -32089,8 +32165,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="206"/>
-      <c r="B12" s="209"/>
+      <c r="A12" s="212"/>
+      <c r="B12" s="215"/>
       <c r="C12" s="100" t="s">
         <v>526</v>
       </c>
@@ -32099,8 +32175,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="207"/>
-      <c r="B13" s="210"/>
+      <c r="A13" s="213"/>
+      <c r="B13" s="216"/>
       <c r="C13" s="100" t="s">
         <v>529</v>
       </c>
@@ -32117,10 +32193,10 @@
       <c r="D14" s="104"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="225" t="s">
+      <c r="A15" s="231" t="s">
         <v>247</v>
       </c>
-      <c r="B15" s="208" t="s">
+      <c r="B15" s="214" t="s">
         <v>439</v>
       </c>
       <c r="C15" s="128" t="s">
@@ -32131,8 +32207,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="227"/>
-      <c r="B16" s="210"/>
+      <c r="A16" s="233"/>
+      <c r="B16" s="216"/>
       <c r="C16" s="128" t="s">
         <v>474</v>
       </c>
@@ -32167,10 +32243,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="205" t="s">
+      <c r="A19" s="211" t="s">
         <v>279</v>
       </c>
-      <c r="B19" s="208" t="s">
+      <c r="B19" s="214" t="s">
         <v>439</v>
       </c>
       <c r="C19" s="95" t="s">
@@ -32181,8 +32257,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="206"/>
-      <c r="B20" s="209"/>
+      <c r="A20" s="212"/>
+      <c r="B20" s="215"/>
       <c r="C20" s="106" t="s">
         <v>299</v>
       </c>
@@ -32191,8 +32267,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="206"/>
-      <c r="B21" s="209"/>
+      <c r="A21" s="212"/>
+      <c r="B21" s="215"/>
       <c r="C21" s="128" t="s">
         <v>280</v>
       </c>
@@ -32201,8 +32277,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="206"/>
-      <c r="B22" s="209"/>
+      <c r="A22" s="212"/>
+      <c r="B22" s="215"/>
       <c r="C22" s="128" t="s">
         <v>21</v>
       </c>
@@ -32211,8 +32287,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="206"/>
-      <c r="B23" s="209"/>
+      <c r="A23" s="212"/>
+      <c r="B23" s="215"/>
       <c r="C23" s="100" t="s">
         <v>434</v>
       </c>
@@ -32221,8 +32297,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="206"/>
-      <c r="B24" s="209"/>
+      <c r="A24" s="212"/>
+      <c r="B24" s="215"/>
       <c r="C24" s="100" t="s">
         <v>444</v>
       </c>
@@ -32231,8 +32307,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="206"/>
-      <c r="B25" s="209"/>
+      <c r="A25" s="212"/>
+      <c r="B25" s="215"/>
       <c r="C25" s="100" t="s">
         <v>446</v>
       </c>
@@ -32241,8 +32317,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="206"/>
-      <c r="B26" s="209"/>
+      <c r="A26" s="212"/>
+      <c r="B26" s="215"/>
       <c r="C26" s="100" t="s">
         <v>434</v>
       </c>
@@ -32251,8 +32327,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="206"/>
-      <c r="B27" s="209"/>
+      <c r="A27" s="212"/>
+      <c r="B27" s="215"/>
       <c r="C27" s="142" t="s">
         <v>453</v>
       </c>
@@ -32261,8 +32337,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="207"/>
-      <c r="B28" s="210"/>
+      <c r="A28" s="213"/>
+      <c r="B28" s="216"/>
       <c r="C28" s="142">
         <v>1.1000000000000001</v>
       </c>
@@ -32271,10 +32347,10 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="213" t="s">
+      <c r="A29" s="219" t="s">
         <v>452</v>
       </c>
-      <c r="B29" s="208" t="s">
+      <c r="B29" s="214" t="s">
         <v>439</v>
       </c>
       <c r="C29" s="100" t="s">
@@ -32285,8 +32361,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="214"/>
-      <c r="B30" s="209"/>
+      <c r="A30" s="220"/>
+      <c r="B30" s="215"/>
       <c r="C30" s="100" t="s">
         <v>453</v>
       </c>
@@ -32295,8 +32371,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="214"/>
-      <c r="B31" s="209"/>
+      <c r="A31" s="220"/>
+      <c r="B31" s="215"/>
       <c r="C31" s="100">
         <v>3.3</v>
       </c>
@@ -32305,8 +32381,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="214"/>
-      <c r="B32" s="209"/>
+      <c r="A32" s="220"/>
+      <c r="B32" s="215"/>
       <c r="C32" s="130">
         <v>3</v>
       </c>
@@ -32315,8 +32391,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="215"/>
-      <c r="B33" s="210"/>
+      <c r="A33" s="221"/>
+      <c r="B33" s="216"/>
       <c r="C33" s="130">
         <v>3.5</v>
       </c>
@@ -32325,10 +32401,10 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="213" t="s">
+      <c r="A34" s="219" t="s">
         <v>457</v>
       </c>
-      <c r="B34" s="208" t="s">
+      <c r="B34" s="214" t="s">
         <v>439</v>
       </c>
       <c r="C34" s="130"/>
@@ -32337,18 +32413,18 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="215"/>
-      <c r="B35" s="210"/>
+      <c r="A35" s="221"/>
+      <c r="B35" s="216"/>
       <c r="C35" s="100"/>
       <c r="D35" s="67" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="237" t="s">
+      <c r="A36" s="243" t="s">
         <v>501</v>
       </c>
-      <c r="B36" s="208" t="s">
+      <c r="B36" s="214" t="s">
         <v>439</v>
       </c>
       <c r="D36" s="67" t="s">
@@ -32356,8 +32432,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="237"/>
-      <c r="B37" s="209"/>
+      <c r="A37" s="243"/>
+      <c r="B37" s="215"/>
       <c r="C37" s="144" t="s">
         <v>508</v>
       </c>
@@ -32366,8 +32442,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="237"/>
-      <c r="B38" s="209"/>
+      <c r="A38" s="243"/>
+      <c r="B38" s="215"/>
       <c r="C38" s="58" t="s">
         <v>506</v>
       </c>
@@ -32376,8 +32452,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="237"/>
-      <c r="B39" s="209"/>
+      <c r="A39" s="243"/>
+      <c r="B39" s="215"/>
       <c r="C39" s="61" t="s">
         <v>509</v>
       </c>
@@ -32389,7 +32465,7 @@
       <c r="A40" s="146" t="s">
         <v>511</v>
       </c>
-      <c r="B40" s="208" t="s">
+      <c r="B40" s="214" t="s">
         <v>439</v>
       </c>
       <c r="C40" s="100"/>
@@ -32399,7 +32475,7 @@
     </row>
     <row r="41" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="147"/>
-      <c r="B41" s="209"/>
+      <c r="B41" s="215"/>
       <c r="C41" s="100" t="s">
         <v>512</v>
       </c>
@@ -32409,7 +32485,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="148"/>
-      <c r="B42" s="210"/>
+      <c r="B42" s="216"/>
       <c r="C42" s="100"/>
       <c r="D42" s="145" t="s">
         <v>514</v>
@@ -32419,7 +32495,7 @@
       <c r="A43" s="146" t="s">
         <v>502</v>
       </c>
-      <c r="B43" s="208" t="s">
+      <c r="B43" s="214" t="s">
         <v>439</v>
       </c>
       <c r="C43" s="100"/>
@@ -32429,28 +32505,28 @@
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="148"/>
-      <c r="B44" s="210"/>
+      <c r="B44" s="216"/>
       <c r="C44" s="100"/>
       <c r="D44" s="145" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="205" t="s">
+      <c r="A45" s="211" t="s">
         <v>517</v>
       </c>
-      <c r="B45" s="208" t="s">
+      <c r="B45" s="214" t="s">
         <v>439</v>
       </c>
-      <c r="C45" s="232"/>
+      <c r="C45" s="238"/>
       <c r="D45" s="145" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="207"/>
-      <c r="B46" s="210"/>
-      <c r="C46" s="233"/>
+      <c r="A46" s="213"/>
+      <c r="B46" s="216"/>
+      <c r="C46" s="239"/>
       <c r="D46" s="145" t="s">
         <v>518</v>
       </c>
@@ -32500,10 +32576,10 @@
       <c r="D50" s="104"/>
     </row>
     <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="237" t="s">
+      <c r="A51" s="243" t="s">
         <v>336</v>
       </c>
-      <c r="B51" s="238" t="s">
+      <c r="B51" s="244" t="s">
         <v>439</v>
       </c>
       <c r="C51" s="100" t="s">
@@ -32514,8 +32590,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="237"/>
-      <c r="B52" s="238"/>
+      <c r="A52" s="243"/>
+      <c r="B52" s="244"/>
       <c r="C52" s="100" t="s">
         <v>341</v>
       </c>
@@ -32524,8 +32600,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="237"/>
-      <c r="B53" s="238"/>
+      <c r="A53" s="243"/>
+      <c r="B53" s="244"/>
       <c r="C53" s="100" t="s">
         <v>337</v>
       </c>
@@ -32542,10 +32618,10 @@
       <c r="D54" s="104"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="228" t="s">
+      <c r="A55" s="234" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="229" t="s">
+      <c r="B55" s="235" t="s">
         <v>439</v>
       </c>
       <c r="C55" s="106"/>
@@ -32554,8 +32630,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="228"/>
-      <c r="B56" s="229"/>
+      <c r="A56" s="234"/>
+      <c r="B56" s="235"/>
       <c r="C56" s="136" t="s">
         <v>234</v>
       </c>
@@ -32564,8 +32640,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="228"/>
-      <c r="B57" s="229"/>
+      <c r="A57" s="234"/>
+      <c r="B57" s="235"/>
       <c r="C57" s="139" t="s">
         <v>484</v>
       </c>
@@ -32574,8 +32650,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="228"/>
-      <c r="B58" s="229"/>
+      <c r="A58" s="234"/>
+      <c r="B58" s="235"/>
       <c r="C58" s="141" t="s">
         <v>484</v>
       </c>
@@ -32584,8 +32660,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="228"/>
-      <c r="B59" s="229"/>
+      <c r="A59" s="234"/>
+      <c r="B59" s="235"/>
       <c r="C59" s="139" t="s">
         <v>498</v>
       </c>
@@ -32594,8 +32670,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="228"/>
-      <c r="B60" s="229"/>
+      <c r="A60" s="234"/>
+      <c r="B60" s="235"/>
       <c r="C60" s="112" t="s">
         <v>498</v>
       </c>
@@ -32604,10 +32680,10 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="225" t="s">
+      <c r="A61" s="231" t="s">
         <v>74</v>
       </c>
-      <c r="B61" s="208" t="s">
+      <c r="B61" s="214" t="s">
         <v>439</v>
       </c>
       <c r="C61" s="107" t="s">
@@ -32618,8 +32694,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="226"/>
-      <c r="B62" s="209"/>
+      <c r="A62" s="232"/>
+      <c r="B62" s="215"/>
       <c r="C62" s="136" t="s">
         <v>463</v>
       </c>
@@ -32628,8 +32704,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="227"/>
-      <c r="B63" s="210"/>
+      <c r="A63" s="233"/>
+      <c r="B63" s="216"/>
       <c r="C63" s="137" t="s">
         <v>481</v>
       </c>
@@ -32678,10 +32754,10 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="228" t="s">
+      <c r="A67" s="234" t="s">
         <v>269</v>
       </c>
-      <c r="B67" s="229" t="s">
+      <c r="B67" s="235" t="s">
         <v>439</v>
       </c>
       <c r="C67" s="106" t="s">
@@ -32692,24 +32768,24 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="228"/>
-      <c r="B68" s="229"/>
+      <c r="A68" s="234"/>
+      <c r="B68" s="235"/>
       <c r="C68" s="106"/>
       <c r="D68" s="80" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="228"/>
-      <c r="B69" s="229"/>
+      <c r="A69" s="234"/>
+      <c r="B69" s="235"/>
       <c r="C69" s="106"/>
       <c r="D69" s="106" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="228"/>
-      <c r="B70" s="229"/>
+      <c r="A70" s="234"/>
+      <c r="B70" s="235"/>
       <c r="C70" s="111" t="s">
         <v>319</v>
       </c>
@@ -32718,8 +32794,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="228"/>
-      <c r="B71" s="229"/>
+      <c r="A71" s="234"/>
+      <c r="B71" s="235"/>
       <c r="C71" s="112" t="s">
         <v>398</v>
       </c>
@@ -32740,10 +32816,10 @@
       <c r="D72" s="106"/>
     </row>
     <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="234" t="s">
+      <c r="A73" s="240" t="s">
         <v>165</v>
       </c>
-      <c r="B73" s="208" t="s">
+      <c r="B73" s="214" t="s">
         <v>439</v>
       </c>
       <c r="C73" s="106"/>
@@ -32752,8 +32828,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="235"/>
-      <c r="B74" s="209"/>
+      <c r="A74" s="241"/>
+      <c r="B74" s="215"/>
       <c r="C74" s="112" t="s">
         <v>355</v>
       </c>
@@ -32762,8 +32838,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="235"/>
-      <c r="B75" s="209"/>
+      <c r="A75" s="241"/>
+      <c r="B75" s="215"/>
       <c r="C75" s="112" t="s">
         <v>353</v>
       </c>
@@ -32772,8 +32848,8 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="235"/>
-      <c r="B76" s="209"/>
+      <c r="A76" s="241"/>
+      <c r="B76" s="215"/>
       <c r="C76" s="115" t="s">
         <v>361</v>
       </c>
@@ -32782,8 +32858,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="235"/>
-      <c r="B77" s="209"/>
+      <c r="A77" s="241"/>
+      <c r="B77" s="215"/>
       <c r="C77" s="112" t="s">
         <v>353</v>
       </c>
@@ -32792,8 +32868,8 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="235"/>
-      <c r="B78" s="209"/>
+      <c r="A78" s="241"/>
+      <c r="B78" s="215"/>
       <c r="C78" s="112" t="s">
         <v>365</v>
       </c>
@@ -32802,8 +32878,8 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="235"/>
-      <c r="B79" s="209"/>
+      <c r="A79" s="241"/>
+      <c r="B79" s="215"/>
       <c r="C79" s="112" t="s">
         <v>353</v>
       </c>
@@ -32812,8 +32888,8 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="235"/>
-      <c r="B80" s="209"/>
+      <c r="A80" s="241"/>
+      <c r="B80" s="215"/>
       <c r="C80" s="112" t="s">
         <v>464</v>
       </c>
@@ -32822,8 +32898,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="235"/>
-      <c r="B81" s="209"/>
+      <c r="A81" s="241"/>
+      <c r="B81" s="215"/>
       <c r="C81" s="133" t="s">
         <v>466</v>
       </c>
@@ -32832,8 +32908,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="235"/>
-      <c r="B82" s="209"/>
+      <c r="A82" s="241"/>
+      <c r="B82" s="215"/>
       <c r="C82" s="133" t="s">
         <v>353</v>
       </c>
@@ -32842,8 +32918,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="235"/>
-      <c r="B83" s="209"/>
+      <c r="A83" s="241"/>
+      <c r="B83" s="215"/>
       <c r="C83" s="138" t="s">
         <v>466</v>
       </c>
@@ -32852,8 +32928,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="235"/>
-      <c r="B84" s="209"/>
+      <c r="A84" s="241"/>
+      <c r="B84" s="215"/>
       <c r="C84" s="112" t="s">
         <v>353</v>
       </c>
@@ -32862,8 +32938,8 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="235"/>
-      <c r="B85" s="209"/>
+      <c r="A85" s="241"/>
+      <c r="B85" s="215"/>
       <c r="C85" s="112" t="s">
         <v>498</v>
       </c>
@@ -32872,8 +32948,8 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="235"/>
-      <c r="B86" s="209"/>
+      <c r="A86" s="241"/>
+      <c r="B86" s="215"/>
       <c r="C86" s="112" t="s">
         <v>498</v>
       </c>
@@ -32882,8 +32958,8 @@
       </c>
     </row>
     <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="235"/>
-      <c r="B87" s="209"/>
+      <c r="A87" s="241"/>
+      <c r="B87" s="215"/>
       <c r="C87" s="151" t="s">
         <v>520</v>
       </c>
@@ -32892,8 +32968,8 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="236"/>
-      <c r="B88" s="210"/>
+      <c r="A88" s="242"/>
+      <c r="B88" s="216"/>
       <c r="C88" s="112" t="s">
         <v>498</v>
       </c>
@@ -32942,10 +33018,10 @@
       <c r="D91" s="113"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="216" t="s">
+      <c r="A92" s="222" t="s">
         <v>363</v>
       </c>
-      <c r="B92" s="208" t="s">
+      <c r="B92" s="214" t="s">
         <v>439</v>
       </c>
       <c r="C92" s="112" t="s">
@@ -32954,8 +33030,8 @@
       <c r="D92" s="113"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="217"/>
-      <c r="B93" s="210"/>
+      <c r="A93" s="223"/>
+      <c r="B93" s="216"/>
       <c r="C93" s="112" t="s">
         <v>398</v>
       </c>
@@ -32972,10 +33048,10 @@
       <c r="D94" s="103"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="216" t="s">
+      <c r="A95" s="222" t="s">
         <v>236</v>
       </c>
-      <c r="B95" s="208" t="s">
+      <c r="B95" s="214" t="s">
         <v>439</v>
       </c>
       <c r="C95" s="106"/>
@@ -32984,24 +33060,24 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="218"/>
-      <c r="B96" s="209"/>
+      <c r="A96" s="224"/>
+      <c r="B96" s="215"/>
       <c r="C96" s="106"/>
       <c r="D96" s="106" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="218"/>
-      <c r="B97" s="209"/>
+      <c r="A97" s="224"/>
+      <c r="B97" s="215"/>
       <c r="C97" s="106"/>
       <c r="D97" s="106" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="218"/>
-      <c r="B98" s="209"/>
+      <c r="A98" s="224"/>
+      <c r="B98" s="215"/>
       <c r="C98" s="106" t="s">
         <v>294</v>
       </c>
@@ -33010,8 +33086,8 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="218"/>
-      <c r="B99" s="209"/>
+      <c r="A99" s="224"/>
+      <c r="B99" s="215"/>
       <c r="C99" s="106" t="s">
         <v>322</v>
       </c>
@@ -33020,8 +33096,8 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="218"/>
-      <c r="B100" s="209"/>
+      <c r="A100" s="224"/>
+      <c r="B100" s="215"/>
       <c r="C100" s="106" t="s">
         <v>367</v>
       </c>
@@ -33030,8 +33106,8 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="218"/>
-      <c r="B101" s="209"/>
+      <c r="A101" s="224"/>
+      <c r="B101" s="215"/>
       <c r="C101" s="119" t="s">
         <v>468</v>
       </c>
@@ -33040,8 +33116,8 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="218"/>
-      <c r="B102" s="209"/>
+      <c r="A102" s="224"/>
+      <c r="B102" s="215"/>
       <c r="C102" s="58" t="s">
         <v>37</v>
       </c>
@@ -33050,8 +33126,8 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="218"/>
-      <c r="B103" s="209"/>
+      <c r="A103" s="224"/>
+      <c r="B103" s="215"/>
       <c r="C103" s="130" t="s">
         <v>353</v>
       </c>
@@ -33060,8 +33136,8 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="218"/>
-      <c r="B104" s="209"/>
+      <c r="A104" s="224"/>
+      <c r="B104" s="215"/>
       <c r="C104" s="130" t="s">
         <v>466</v>
       </c>
@@ -33070,8 +33146,8 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="218"/>
-      <c r="B105" s="209"/>
+      <c r="A105" s="224"/>
+      <c r="B105" s="215"/>
       <c r="C105" s="130" t="s">
         <v>367</v>
       </c>
@@ -33080,8 +33156,8 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="218"/>
-      <c r="B106" s="209"/>
+      <c r="A106" s="224"/>
+      <c r="B106" s="215"/>
       <c r="C106" s="130" t="s">
         <v>353</v>
       </c>
@@ -33090,8 +33166,8 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="218"/>
-      <c r="B107" s="209"/>
+      <c r="A107" s="224"/>
+      <c r="B107" s="215"/>
       <c r="C107" s="130" t="s">
         <v>498</v>
       </c>
@@ -33100,8 +33176,8 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="218"/>
-      <c r="B108" s="209"/>
+      <c r="A108" s="224"/>
+      <c r="B108" s="215"/>
       <c r="C108" s="109" t="s">
         <v>498</v>
       </c>
@@ -33110,8 +33186,8 @@
       </c>
     </row>
     <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="218"/>
-      <c r="B109" s="209"/>
+      <c r="A109" s="224"/>
+      <c r="B109" s="215"/>
       <c r="C109" s="151" t="s">
         <v>520</v>
       </c>
@@ -33120,8 +33196,8 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="217"/>
-      <c r="B110" s="210"/>
+      <c r="A110" s="223"/>
+      <c r="B110" s="216"/>
       <c r="C110" s="109" t="s">
         <v>498</v>
       </c>
@@ -33130,22 +33206,22 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="219" t="s">
+      <c r="A111" s="225" t="s">
         <v>27</v>
       </c>
-      <c r="B111" s="208" t="s">
+      <c r="B111" s="214" t="s">
         <v>439</v>
       </c>
-      <c r="C111" s="242" t="s">
+      <c r="C111" s="157" t="s">
         <v>532</v>
       </c>
-      <c r="D111" s="243" t="s">
+      <c r="D111" s="158" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="220"/>
-      <c r="B112" s="209"/>
+      <c r="A112" s="226"/>
+      <c r="B112" s="215"/>
       <c r="C112" s="106" t="s">
         <v>297</v>
       </c>
@@ -33154,16 +33230,16 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="220"/>
-      <c r="B113" s="209"/>
+      <c r="A113" s="226"/>
+      <c r="B113" s="215"/>
       <c r="C113" s="106"/>
       <c r="D113" s="106" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="220"/>
-      <c r="B114" s="209"/>
+      <c r="A114" s="226"/>
+      <c r="B114" s="215"/>
       <c r="C114" s="117" t="s">
         <v>323</v>
       </c>
@@ -33172,8 +33248,8 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="220"/>
-      <c r="B115" s="209"/>
+      <c r="A115" s="226"/>
+      <c r="B115" s="215"/>
       <c r="C115" s="117" t="s">
         <v>353</v>
       </c>
@@ -33182,8 +33258,8 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="220"/>
-      <c r="B116" s="209"/>
+      <c r="A116" s="226"/>
+      <c r="B116" s="215"/>
       <c r="C116" s="117" t="s">
         <v>361</v>
       </c>
@@ -33192,8 +33268,8 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="220"/>
-      <c r="B117" s="209"/>
+      <c r="A117" s="226"/>
+      <c r="B117" s="215"/>
       <c r="C117" s="117" t="s">
         <v>365</v>
       </c>
@@ -33202,8 +33278,8 @@
       </c>
     </row>
     <row r="118" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="220"/>
-      <c r="B118" s="209"/>
+      <c r="A118" s="226"/>
+      <c r="B118" s="215"/>
       <c r="C118" s="117" t="s">
         <v>375</v>
       </c>
@@ -33212,8 +33288,8 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="220"/>
-      <c r="B119" s="209"/>
+      <c r="A119" s="226"/>
+      <c r="B119" s="215"/>
       <c r="C119" s="109" t="s">
         <v>353</v>
       </c>
@@ -33222,8 +33298,8 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="220"/>
-      <c r="B120" s="209"/>
+      <c r="A120" s="226"/>
+      <c r="B120" s="215"/>
       <c r="C120" s="109" t="s">
         <v>464</v>
       </c>
@@ -33232,8 +33308,8 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="220"/>
-      <c r="B121" s="209"/>
+      <c r="A121" s="226"/>
+      <c r="B121" s="215"/>
       <c r="C121" s="130" t="s">
         <v>466</v>
       </c>
@@ -33242,8 +33318,8 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="220"/>
-      <c r="B122" s="209"/>
+      <c r="A122" s="226"/>
+      <c r="B122" s="215"/>
       <c r="C122" s="130" t="s">
         <v>353</v>
       </c>
@@ -33252,8 +33328,8 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="220"/>
-      <c r="B123" s="209"/>
+      <c r="A123" s="226"/>
+      <c r="B123" s="215"/>
       <c r="C123" s="130" t="s">
         <v>466</v>
       </c>
@@ -33262,8 +33338,8 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="220"/>
-      <c r="B124" s="209"/>
+      <c r="A124" s="226"/>
+      <c r="B124" s="215"/>
       <c r="C124" s="130" t="s">
         <v>367</v>
       </c>
@@ -33272,8 +33348,8 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="220"/>
-      <c r="B125" s="209"/>
+      <c r="A125" s="226"/>
+      <c r="B125" s="215"/>
       <c r="C125" s="130" t="s">
         <v>353</v>
       </c>
@@ -33282,8 +33358,8 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="220"/>
-      <c r="B126" s="209"/>
+      <c r="A126" s="226"/>
+      <c r="B126" s="215"/>
       <c r="C126" s="130" t="s">
         <v>498</v>
       </c>
@@ -33292,8 +33368,8 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="220"/>
-      <c r="B127" s="209"/>
+      <c r="A127" s="226"/>
+      <c r="B127" s="215"/>
       <c r="C127" s="109" t="s">
         <v>498</v>
       </c>
@@ -33302,8 +33378,8 @@
       </c>
     </row>
     <row r="128" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A128" s="220"/>
-      <c r="B128" s="209"/>
+      <c r="A128" s="226"/>
+      <c r="B128" s="215"/>
       <c r="C128" s="151" t="s">
         <v>520</v>
       </c>
@@ -33312,8 +33388,8 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="221"/>
-      <c r="B129" s="210"/>
+      <c r="A129" s="227"/>
+      <c r="B129" s="216"/>
       <c r="C129" s="109" t="s">
         <v>498</v>
       </c>
@@ -33322,13 +33398,13 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="225" t="s">
+      <c r="A130" s="231" t="s">
         <v>222</v>
       </c>
-      <c r="B130" s="208" t="s">
+      <c r="B130" s="214" t="s">
         <v>439</v>
       </c>
-      <c r="C130" s="222" t="s">
+      <c r="C130" s="228" t="s">
         <v>238</v>
       </c>
       <c r="D130" s="96" t="s">
@@ -33336,17 +33412,17 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="226"/>
-      <c r="B131" s="209"/>
-      <c r="C131" s="223"/>
+      <c r="A131" s="232"/>
+      <c r="B131" s="215"/>
+      <c r="C131" s="229"/>
       <c r="D131" s="113" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="226"/>
-      <c r="B132" s="209"/>
-      <c r="C132" s="224" t="s">
+      <c r="A132" s="232"/>
+      <c r="B132" s="215"/>
+      <c r="C132" s="230" t="s">
         <v>239</v>
       </c>
       <c r="D132" s="106" t="s">
@@ -33354,16 +33430,16 @@
       </c>
     </row>
     <row r="133" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A133" s="226"/>
-      <c r="B133" s="209"/>
-      <c r="C133" s="224"/>
+      <c r="A133" s="232"/>
+      <c r="B133" s="215"/>
+      <c r="C133" s="230"/>
       <c r="D133" s="119" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="226"/>
-      <c r="B134" s="209"/>
+      <c r="A134" s="232"/>
+      <c r="B134" s="215"/>
       <c r="C134" s="112" t="s">
         <v>301</v>
       </c>
@@ -33372,8 +33448,8 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="226"/>
-      <c r="B135" s="209"/>
+      <c r="A135" s="232"/>
+      <c r="B135" s="215"/>
       <c r="C135" s="112">
         <v>2.1</v>
       </c>
@@ -33382,8 +33458,8 @@
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="226"/>
-      <c r="B136" s="209"/>
+      <c r="A136" s="232"/>
+      <c r="B136" s="215"/>
       <c r="C136" s="112" t="s">
         <v>238</v>
       </c>
@@ -33392,8 +33468,8 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="226"/>
-      <c r="B137" s="209"/>
+      <c r="A137" s="232"/>
+      <c r="B137" s="215"/>
       <c r="C137" s="112" t="s">
         <v>238</v>
       </c>
@@ -33402,8 +33478,8 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="226"/>
-      <c r="B138" s="209"/>
+      <c r="A138" s="232"/>
+      <c r="B138" s="215"/>
       <c r="C138" s="112" t="s">
         <v>238</v>
       </c>
@@ -33412,8 +33488,8 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="226"/>
-      <c r="B139" s="209"/>
+      <c r="A139" s="232"/>
+      <c r="B139" s="215"/>
       <c r="C139" s="120" t="s">
         <v>372</v>
       </c>
@@ -33422,8 +33498,8 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="226"/>
-      <c r="B140" s="209"/>
+      <c r="A140" s="232"/>
+      <c r="B140" s="215"/>
       <c r="C140" s="112">
         <v>2.1</v>
       </c>
@@ -33432,8 +33508,8 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="226"/>
-      <c r="B141" s="209"/>
+      <c r="A141" s="232"/>
+      <c r="B141" s="215"/>
       <c r="C141" s="112" t="s">
         <v>238</v>
       </c>
@@ -33442,8 +33518,8 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="226"/>
-      <c r="B142" s="209"/>
+      <c r="A142" s="232"/>
+      <c r="B142" s="215"/>
       <c r="C142" s="112" t="s">
         <v>238</v>
       </c>
@@ -33452,8 +33528,8 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="226"/>
-      <c r="B143" s="209"/>
+      <c r="A143" s="232"/>
+      <c r="B143" s="215"/>
       <c r="C143" s="112">
         <v>2.1</v>
       </c>
@@ -33462,10 +33538,10 @@
       </c>
     </row>
     <row r="144" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="219" t="s">
+      <c r="A144" s="225" t="s">
         <v>290</v>
       </c>
-      <c r="B144" s="208" t="s">
+      <c r="B144" s="214" t="s">
         <v>439</v>
       </c>
       <c r="C144" s="106" t="s">
@@ -33476,8 +33552,8 @@
       </c>
     </row>
     <row r="145" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A145" s="220"/>
-      <c r="B145" s="209"/>
+      <c r="A145" s="226"/>
+      <c r="B145" s="215"/>
       <c r="C145" s="119" t="s">
         <v>275</v>
       </c>
@@ -33486,8 +33562,8 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="221"/>
-      <c r="B146" s="210"/>
+      <c r="A146" s="227"/>
+      <c r="B146" s="216"/>
       <c r="C146" s="106" t="s">
         <v>344</v>
       </c>
@@ -33496,10 +33572,10 @@
       </c>
     </row>
     <row r="147" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="216" t="s">
+      <c r="A147" s="222" t="s">
         <v>364</v>
       </c>
-      <c r="B147" s="208" t="s">
+      <c r="B147" s="214" t="s">
         <v>439</v>
       </c>
       <c r="C147" s="112" t="s">
@@ -33508,8 +33584,8 @@
       <c r="D147" s="106"/>
     </row>
     <row r="148" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="218"/>
-      <c r="B148" s="209"/>
+      <c r="A148" s="224"/>
+      <c r="B148" s="215"/>
       <c r="C148" s="112" t="s">
         <v>372</v>
       </c>
@@ -33518,8 +33594,8 @@
       </c>
     </row>
     <row r="149" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="218"/>
-      <c r="B149" s="209"/>
+      <c r="A149" s="224"/>
+      <c r="B149" s="215"/>
       <c r="C149" s="112">
         <v>2.1</v>
       </c>
@@ -33528,8 +33604,8 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="218"/>
-      <c r="B150" s="209"/>
+      <c r="A150" s="224"/>
+      <c r="B150" s="215"/>
       <c r="C150" s="112" t="s">
         <v>239</v>
       </c>
@@ -33538,8 +33614,8 @@
       </c>
     </row>
     <row r="151" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="218"/>
-      <c r="B151" s="209"/>
+      <c r="A151" s="224"/>
+      <c r="B151" s="215"/>
       <c r="C151" s="112" t="s">
         <v>238</v>
       </c>
@@ -33568,10 +33644,10 @@
       <c r="D153" s="113"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="225" t="s">
+      <c r="A154" s="231" t="s">
         <v>255</v>
       </c>
-      <c r="B154" s="208" t="s">
+      <c r="B154" s="214" t="s">
         <v>439</v>
       </c>
       <c r="C154" s="106"/>
@@ -33580,24 +33656,24 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="226"/>
-      <c r="B155" s="209"/>
+      <c r="A155" s="232"/>
+      <c r="B155" s="215"/>
       <c r="C155" s="106"/>
       <c r="D155" s="106" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="226"/>
-      <c r="B156" s="209"/>
+      <c r="A156" s="232"/>
+      <c r="B156" s="215"/>
       <c r="C156" s="106"/>
       <c r="D156" s="113" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="226"/>
-      <c r="B157" s="209"/>
+      <c r="A157" s="232"/>
+      <c r="B157" s="215"/>
       <c r="C157" s="106" t="s">
         <v>418</v>
       </c>
@@ -33606,8 +33682,8 @@
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="226"/>
-      <c r="B158" s="209"/>
+      <c r="A158" s="232"/>
+      <c r="B158" s="215"/>
       <c r="C158" s="106" t="s">
         <v>423</v>
       </c>
@@ -33616,8 +33692,8 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="226"/>
-      <c r="B159" s="209"/>
+      <c r="A159" s="232"/>
+      <c r="B159" s="215"/>
       <c r="C159" s="106" t="s">
         <v>484</v>
       </c>
@@ -33626,8 +33702,8 @@
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="226"/>
-      <c r="B160" s="209"/>
+      <c r="A160" s="232"/>
+      <c r="B160" s="215"/>
       <c r="C160" s="106" t="s">
         <v>498</v>
       </c>
@@ -33636,10 +33712,10 @@
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="228" t="s">
+      <c r="A161" s="234" t="s">
         <v>328</v>
       </c>
-      <c r="B161" s="229" t="s">
+      <c r="B161" s="235" t="s">
         <v>439</v>
       </c>
       <c r="C161" s="80" t="s">
@@ -33650,8 +33726,8 @@
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="228"/>
-      <c r="B162" s="229"/>
+      <c r="A162" s="234"/>
+      <c r="B162" s="235"/>
       <c r="C162" s="106" t="s">
         <v>405</v>
       </c>
@@ -33660,42 +33736,42 @@
       </c>
     </row>
     <row r="163" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A163" s="228"/>
-      <c r="B163" s="229"/>
+      <c r="A163" s="234"/>
+      <c r="B163" s="235"/>
       <c r="C163" s="122" t="s">
         <v>408</v>
       </c>
-      <c r="D163" s="211" t="s">
+      <c r="D163" s="217" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A164" s="228"/>
-      <c r="B164" s="229"/>
+      <c r="A164" s="234"/>
+      <c r="B164" s="235"/>
       <c r="C164" s="122" t="s">
         <v>409</v>
       </c>
-      <c r="D164" s="212"/>
+      <c r="D164" s="218"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="228"/>
-      <c r="B165" s="229"/>
+      <c r="A165" s="234"/>
+      <c r="B165" s="235"/>
       <c r="C165" s="122" t="s">
         <v>410</v>
       </c>
-      <c r="D165" s="212"/>
+      <c r="D165" s="218"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="228"/>
-      <c r="B166" s="229"/>
+      <c r="A166" s="234"/>
+      <c r="B166" s="235"/>
       <c r="C166" s="122" t="s">
         <v>411</v>
       </c>
-      <c r="D166" s="212"/>
+      <c r="D166" s="218"/>
     </row>
     <row r="167" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A167" s="228"/>
-      <c r="B167" s="229"/>
+      <c r="A167" s="234"/>
+      <c r="B167" s="235"/>
       <c r="C167" s="122" t="s">
         <v>470</v>
       </c>
@@ -33718,10 +33794,10 @@
       </c>
     </row>
     <row r="169" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="239" t="s">
+      <c r="A169" s="245" t="s">
         <v>32</v>
       </c>
-      <c r="B169" s="208" t="s">
+      <c r="B169" s="214" t="s">
         <v>439</v>
       </c>
       <c r="C169" s="106" t="s">
@@ -33732,8 +33808,8 @@
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="240"/>
-      <c r="B170" s="209"/>
+      <c r="A170" s="246"/>
+      <c r="B170" s="215"/>
       <c r="C170" s="106" t="s">
         <v>264</v>
       </c>
@@ -33742,8 +33818,8 @@
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="240"/>
-      <c r="B171" s="209"/>
+      <c r="A171" s="246"/>
+      <c r="B171" s="215"/>
       <c r="C171" s="106" t="s">
         <v>263</v>
       </c>
@@ -33752,8 +33828,8 @@
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="240"/>
-      <c r="B172" s="209"/>
+      <c r="A172" s="246"/>
+      <c r="B172" s="215"/>
       <c r="C172" s="113" t="s">
         <v>271</v>
       </c>
@@ -33762,8 +33838,8 @@
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="240"/>
-      <c r="B173" s="209"/>
+      <c r="A173" s="246"/>
+      <c r="B173" s="215"/>
       <c r="C173" s="106" t="s">
         <v>276</v>
       </c>
@@ -33772,8 +33848,8 @@
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="240"/>
-      <c r="B174" s="209"/>
+      <c r="A174" s="246"/>
+      <c r="B174" s="215"/>
       <c r="C174" s="106" t="s">
         <v>277</v>
       </c>
@@ -33782,8 +33858,8 @@
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="240"/>
-      <c r="B175" s="209"/>
+      <c r="A175" s="246"/>
+      <c r="B175" s="215"/>
       <c r="C175" s="113" t="s">
         <v>282</v>
       </c>
@@ -33792,8 +33868,8 @@
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="240"/>
-      <c r="B176" s="209"/>
+      <c r="A176" s="246"/>
+      <c r="B176" s="215"/>
       <c r="C176" s="113" t="s">
         <v>296</v>
       </c>
@@ -33802,8 +33878,8 @@
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="240"/>
-      <c r="B177" s="209"/>
+      <c r="A177" s="246"/>
+      <c r="B177" s="215"/>
       <c r="C177" s="113" t="s">
         <v>283</v>
       </c>
@@ -33812,8 +33888,8 @@
       </c>
     </row>
     <row r="178" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A178" s="240"/>
-      <c r="B178" s="209"/>
+      <c r="A178" s="246"/>
+      <c r="B178" s="215"/>
       <c r="C178" s="123" t="s">
         <v>243</v>
       </c>
@@ -33822,8 +33898,8 @@
       </c>
     </row>
     <row r="179" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A179" s="240"/>
-      <c r="B179" s="209"/>
+      <c r="A179" s="246"/>
+      <c r="B179" s="215"/>
       <c r="C179" s="117" t="s">
         <v>305</v>
       </c>
@@ -33832,8 +33908,8 @@
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="240"/>
-      <c r="B180" s="209"/>
+      <c r="A180" s="246"/>
+      <c r="B180" s="215"/>
       <c r="C180" s="106" t="s">
         <v>306</v>
       </c>
@@ -33842,8 +33918,8 @@
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="240"/>
-      <c r="B181" s="209"/>
+      <c r="A181" s="246"/>
+      <c r="B181" s="215"/>
       <c r="C181" s="113" t="s">
         <v>307</v>
       </c>
@@ -33852,8 +33928,8 @@
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="240"/>
-      <c r="B182" s="209"/>
+      <c r="A182" s="246"/>
+      <c r="B182" s="215"/>
       <c r="C182" s="113" t="s">
         <v>309</v>
       </c>
@@ -33862,8 +33938,8 @@
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="240"/>
-      <c r="B183" s="209"/>
+      <c r="A183" s="246"/>
+      <c r="B183" s="215"/>
       <c r="C183" s="113" t="s">
         <v>262</v>
       </c>
@@ -33872,8 +33948,8 @@
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="240"/>
-      <c r="B184" s="209"/>
+      <c r="A184" s="246"/>
+      <c r="B184" s="215"/>
       <c r="C184" s="106" t="s">
         <v>312</v>
       </c>
@@ -33882,8 +33958,8 @@
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="240"/>
-      <c r="B185" s="209"/>
+      <c r="A185" s="246"/>
+      <c r="B185" s="215"/>
       <c r="C185" s="113" t="s">
         <v>277</v>
       </c>
@@ -33892,8 +33968,8 @@
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="240"/>
-      <c r="B186" s="209"/>
+      <c r="A186" s="246"/>
+      <c r="B186" s="215"/>
       <c r="C186" s="113" t="s">
         <v>313</v>
       </c>
@@ -33902,16 +33978,16 @@
       </c>
     </row>
     <row r="187" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A187" s="240"/>
-      <c r="B187" s="209"/>
+      <c r="A187" s="246"/>
+      <c r="B187" s="215"/>
       <c r="C187" s="106"/>
       <c r="D187" s="97" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="240"/>
-      <c r="B188" s="209"/>
+      <c r="A188" s="246"/>
+      <c r="B188" s="215"/>
       <c r="C188" s="113" t="s">
         <v>316</v>
       </c>
@@ -33920,8 +33996,8 @@
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="240"/>
-      <c r="B189" s="209"/>
+      <c r="A189" s="246"/>
+      <c r="B189" s="215"/>
       <c r="C189" s="113" t="s">
         <v>262</v>
       </c>
@@ -33930,8 +34006,8 @@
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="240"/>
-      <c r="B190" s="209"/>
+      <c r="A190" s="246"/>
+      <c r="B190" s="215"/>
       <c r="C190" s="113" t="s">
         <v>333</v>
       </c>
@@ -33940,8 +34016,8 @@
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="240"/>
-      <c r="B191" s="209"/>
+      <c r="A191" s="246"/>
+      <c r="B191" s="215"/>
       <c r="C191" s="113" t="s">
         <v>334</v>
       </c>
@@ -33950,8 +34026,8 @@
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="240"/>
-      <c r="B192" s="209"/>
+      <c r="A192" s="246"/>
+      <c r="B192" s="215"/>
       <c r="C192" s="113" t="s">
         <v>318</v>
       </c>
@@ -33960,8 +34036,8 @@
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="240"/>
-      <c r="B193" s="209"/>
+      <c r="A193" s="246"/>
+      <c r="B193" s="215"/>
       <c r="C193" s="113" t="s">
         <v>339</v>
       </c>
@@ -33970,8 +34046,8 @@
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="240"/>
-      <c r="B194" s="209"/>
+      <c r="A194" s="246"/>
+      <c r="B194" s="215"/>
       <c r="C194" s="113" t="s">
         <v>332</v>
       </c>
@@ -33980,8 +34056,8 @@
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="240"/>
-      <c r="B195" s="209"/>
+      <c r="A195" s="246"/>
+      <c r="B195" s="215"/>
       <c r="C195" s="113" t="s">
         <v>347</v>
       </c>
@@ -33990,8 +34066,8 @@
       </c>
     </row>
     <row r="196" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A196" s="240"/>
-      <c r="B196" s="209"/>
+      <c r="A196" s="246"/>
+      <c r="B196" s="215"/>
       <c r="C196" s="101" t="s">
         <v>350</v>
       </c>
@@ -34000,8 +34076,8 @@
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="240"/>
-      <c r="B197" s="209"/>
+      <c r="A197" s="246"/>
+      <c r="B197" s="215"/>
       <c r="C197" s="113" t="s">
         <v>351</v>
       </c>
@@ -34010,8 +34086,8 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="240"/>
-      <c r="B198" s="209"/>
+      <c r="A198" s="246"/>
+      <c r="B198" s="215"/>
       <c r="C198" s="113" t="s">
         <v>352</v>
       </c>
@@ -34020,8 +34096,8 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="240"/>
-      <c r="B199" s="209"/>
+      <c r="A199" s="246"/>
+      <c r="B199" s="215"/>
       <c r="C199" s="113" t="s">
         <v>358</v>
       </c>
@@ -34030,8 +34106,8 @@
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="240"/>
-      <c r="B200" s="209"/>
+      <c r="A200" s="246"/>
+      <c r="B200" s="215"/>
       <c r="C200" s="113" t="s">
         <v>360</v>
       </c>
@@ -34040,8 +34116,8 @@
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="240"/>
-      <c r="B201" s="209"/>
+      <c r="A201" s="246"/>
+      <c r="B201" s="215"/>
       <c r="C201" s="113" t="s">
         <v>366</v>
       </c>
@@ -34050,8 +34126,8 @@
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="240"/>
-      <c r="B202" s="209"/>
+      <c r="A202" s="246"/>
+      <c r="B202" s="215"/>
       <c r="C202" s="113" t="s">
         <v>358</v>
       </c>
@@ -34060,8 +34136,8 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="240"/>
-      <c r="B203" s="209"/>
+      <c r="A203" s="246"/>
+      <c r="B203" s="215"/>
       <c r="C203" s="118" t="s">
         <v>379</v>
       </c>
@@ -34070,8 +34146,8 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="240"/>
-      <c r="B204" s="209"/>
+      <c r="A204" s="246"/>
+      <c r="B204" s="215"/>
       <c r="C204" s="106" t="s">
         <v>383</v>
       </c>
@@ -34080,8 +34156,8 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="240"/>
-      <c r="B205" s="209"/>
+      <c r="A205" s="246"/>
+      <c r="B205" s="215"/>
       <c r="C205" s="106" t="s">
         <v>386</v>
       </c>
@@ -34090,8 +34166,8 @@
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="240"/>
-      <c r="B206" s="209"/>
+      <c r="A206" s="246"/>
+      <c r="B206" s="215"/>
       <c r="C206" s="106" t="s">
         <v>387</v>
       </c>
@@ -34100,8 +34176,8 @@
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="240"/>
-      <c r="B207" s="209"/>
+      <c r="A207" s="246"/>
+      <c r="B207" s="215"/>
       <c r="C207" s="106" t="s">
         <v>388</v>
       </c>
@@ -34110,8 +34186,8 @@
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="240"/>
-      <c r="B208" s="209"/>
+      <c r="A208" s="246"/>
+      <c r="B208" s="215"/>
       <c r="C208" s="106" t="s">
         <v>389</v>
       </c>
@@ -34120,8 +34196,8 @@
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" s="240"/>
-      <c r="B209" s="209"/>
+      <c r="A209" s="246"/>
+      <c r="B209" s="215"/>
       <c r="C209" s="106" t="s">
         <v>390</v>
       </c>
@@ -34130,8 +34206,8 @@
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="240"/>
-      <c r="B210" s="209"/>
+      <c r="A210" s="246"/>
+      <c r="B210" s="215"/>
       <c r="C210" s="106" t="s">
         <v>393</v>
       </c>
@@ -34140,8 +34216,8 @@
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="240"/>
-      <c r="B211" s="209"/>
+      <c r="A211" s="246"/>
+      <c r="B211" s="215"/>
       <c r="C211" s="106" t="s">
         <v>403</v>
       </c>
@@ -34150,8 +34226,8 @@
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="240"/>
-      <c r="B212" s="209"/>
+      <c r="A212" s="246"/>
+      <c r="B212" s="215"/>
       <c r="C212" s="106" t="s">
         <v>404</v>
       </c>
@@ -34160,8 +34236,8 @@
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" s="240"/>
-      <c r="B213" s="209"/>
+      <c r="A213" s="246"/>
+      <c r="B213" s="215"/>
       <c r="C213" s="106" t="s">
         <v>421</v>
       </c>
@@ -34170,8 +34246,8 @@
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" s="240"/>
-      <c r="B214" s="209"/>
+      <c r="A214" s="246"/>
+      <c r="B214" s="215"/>
       <c r="C214" s="106" t="s">
         <v>422</v>
       </c>
@@ -34180,8 +34256,8 @@
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" s="240"/>
-      <c r="B215" s="209"/>
+      <c r="A215" s="246"/>
+      <c r="B215" s="215"/>
       <c r="C215" s="106" t="s">
         <v>425</v>
       </c>
@@ -34190,8 +34266,8 @@
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="240"/>
-      <c r="B216" s="209"/>
+      <c r="A216" s="246"/>
+      <c r="B216" s="215"/>
       <c r="C216" s="58" t="s">
         <v>471</v>
       </c>
@@ -34200,8 +34276,8 @@
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" s="240"/>
-      <c r="B217" s="209"/>
+      <c r="A217" s="246"/>
+      <c r="B217" s="215"/>
       <c r="C217" s="58" t="s">
         <v>421</v>
       </c>
@@ -34210,8 +34286,8 @@
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" s="240"/>
-      <c r="B218" s="209"/>
+      <c r="A218" s="246"/>
+      <c r="B218" s="215"/>
       <c r="C218" s="58" t="s">
         <v>497</v>
       </c>
@@ -34220,8 +34296,8 @@
       </c>
     </row>
     <row r="219" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A219" s="240"/>
-      <c r="B219" s="209"/>
+      <c r="A219" s="246"/>
+      <c r="B219" s="215"/>
       <c r="C219" s="61" t="s">
         <v>522</v>
       </c>
@@ -34230,8 +34306,8 @@
       </c>
     </row>
     <row r="220" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A220" s="241"/>
-      <c r="B220" s="210"/>
+      <c r="A220" s="247"/>
+      <c r="B220" s="216"/>
       <c r="C220" s="61" t="s">
         <v>332</v>
       </c>
@@ -34240,10 +34316,10 @@
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" s="239" t="s">
+      <c r="A221" s="245" t="s">
         <v>415</v>
       </c>
-      <c r="B221" s="208" t="s">
+      <c r="B221" s="214" t="s">
         <v>439</v>
       </c>
       <c r="C221" s="106" t="s">
@@ -34254,8 +34330,8 @@
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" s="240"/>
-      <c r="B222" s="209"/>
+      <c r="A222" s="246"/>
+      <c r="B222" s="215"/>
       <c r="C222" s="118" t="s">
         <v>491</v>
       </c>
@@ -34264,8 +34340,8 @@
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223" s="241"/>
-      <c r="B223" s="210"/>
+      <c r="A223" s="247"/>
+      <c r="B223" s="216"/>
       <c r="C223" s="113" t="s">
         <v>524</v>
       </c>
@@ -34310,10 +34386,10 @@
       <c r="D226" s="104"/>
     </row>
     <row r="227" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="225" t="s">
+      <c r="A227" s="231" t="s">
         <v>84</v>
       </c>
-      <c r="B227" s="208" t="s">
+      <c r="B227" s="214" t="s">
         <v>439</v>
       </c>
       <c r="C227" s="106"/>
@@ -34322,8 +34398,8 @@
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" s="226"/>
-      <c r="B228" s="209"/>
+      <c r="A228" s="232"/>
+      <c r="B228" s="215"/>
       <c r="C228" s="107" t="s">
         <v>245</v>
       </c>
@@ -34332,8 +34408,8 @@
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="226"/>
-      <c r="B229" s="209"/>
+      <c r="A229" s="232"/>
+      <c r="B229" s="215"/>
       <c r="C229" s="107">
         <v>10.1</v>
       </c>
@@ -34342,8 +34418,8 @@
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="226"/>
-      <c r="B230" s="209"/>
+      <c r="A230" s="232"/>
+      <c r="B230" s="215"/>
       <c r="C230" s="107">
         <v>10.199999999999999</v>
       </c>
@@ -34352,8 +34428,8 @@
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="226"/>
-      <c r="B231" s="209"/>
+      <c r="A231" s="232"/>
+      <c r="B231" s="215"/>
       <c r="C231" s="98" t="s">
         <v>287</v>
       </c>
@@ -34362,8 +34438,8 @@
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="226"/>
-      <c r="B232" s="209"/>
+      <c r="A232" s="232"/>
+      <c r="B232" s="215"/>
       <c r="C232" s="98" t="s">
         <v>369</v>
       </c>
@@ -34372,8 +34448,8 @@
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="226"/>
-      <c r="B233" s="209"/>
+      <c r="A233" s="232"/>
+      <c r="B233" s="215"/>
       <c r="C233" s="98" t="s">
         <v>117</v>
       </c>
@@ -34382,8 +34458,8 @@
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="226"/>
-      <c r="B234" s="209"/>
+      <c r="A234" s="232"/>
+      <c r="B234" s="215"/>
       <c r="C234" s="98" t="s">
         <v>416</v>
       </c>
@@ -34392,8 +34468,8 @@
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="226"/>
-      <c r="B235" s="209"/>
+      <c r="A235" s="232"/>
+      <c r="B235" s="215"/>
       <c r="C235" s="98" t="s">
         <v>17</v>
       </c>
@@ -34402,8 +34478,8 @@
       </c>
     </row>
     <row r="236" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A236" s="226"/>
-      <c r="B236" s="209"/>
+      <c r="A236" s="232"/>
+      <c r="B236" s="215"/>
       <c r="C236" s="98" t="s">
         <v>496</v>
       </c>
@@ -34412,8 +34488,8 @@
       </c>
     </row>
     <row r="237" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A237" s="227"/>
-      <c r="B237" s="210"/>
+      <c r="A237" s="233"/>
+      <c r="B237" s="216"/>
       <c r="C237" s="98" t="s">
         <v>496</v>
       </c>
@@ -34422,10 +34498,10 @@
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" s="225" t="s">
+      <c r="A238" s="231" t="s">
         <v>246</v>
       </c>
-      <c r="B238" s="208" t="s">
+      <c r="B238" s="214" t="s">
         <v>439</v>
       </c>
       <c r="C238" s="98"/>
@@ -34434,8 +34510,8 @@
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" s="226"/>
-      <c r="B239" s="209"/>
+      <c r="A239" s="232"/>
+      <c r="B239" s="215"/>
       <c r="C239" s="126" t="s">
         <v>427</v>
       </c>
@@ -34466,10 +34542,10 @@
       <c r="D241" s="127"/>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="225" t="s">
+      <c r="A242" s="231" t="s">
         <v>58</v>
       </c>
-      <c r="B242" s="208" t="s">
+      <c r="B242" s="214" t="s">
         <v>265</v>
       </c>
       <c r="C242" s="128" t="s">
@@ -34480,8 +34556,8 @@
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="226"/>
-      <c r="B243" s="209"/>
+      <c r="A243" s="232"/>
+      <c r="B243" s="215"/>
       <c r="C243" s="128" t="s">
         <v>259</v>
       </c>
@@ -34490,18 +34566,18 @@
       </c>
     </row>
     <row r="244" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A244" s="227"/>
-      <c r="B244" s="210"/>
+      <c r="A244" s="233"/>
+      <c r="B244" s="216"/>
       <c r="C244" s="106"/>
       <c r="D244" s="106" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="245" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A245" s="230" t="s">
+      <c r="A245" s="236" t="s">
         <v>59</v>
       </c>
-      <c r="B245" s="208" t="s">
+      <c r="B245" s="214" t="s">
         <v>265</v>
       </c>
       <c r="C245" s="119" t="s">
@@ -34512,18 +34588,18 @@
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A246" s="231"/>
-      <c r="B246" s="210"/>
+      <c r="A246" s="237"/>
+      <c r="B246" s="216"/>
       <c r="C246" s="119"/>
       <c r="D246" s="106" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="247" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A247" s="230" t="s">
+      <c r="A247" s="236" t="s">
         <v>285</v>
       </c>
-      <c r="B247" s="208" t="s">
+      <c r="B247" s="214" t="s">
         <v>265</v>
       </c>
       <c r="C247" s="119"/>
@@ -34532,18 +34608,18 @@
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A248" s="231"/>
-      <c r="B248" s="210"/>
+      <c r="A248" s="237"/>
+      <c r="B248" s="216"/>
       <c r="C248" s="106"/>
       <c r="D248" s="106" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="249" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A249" s="230" t="s">
+      <c r="A249" s="236" t="s">
         <v>60</v>
       </c>
-      <c r="B249" s="208" t="s">
+      <c r="B249" s="214" t="s">
         <v>265</v>
       </c>
       <c r="C249" s="119" t="s">
@@ -34554,8 +34630,8 @@
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A250" s="231"/>
-      <c r="B250" s="210"/>
+      <c r="A250" s="237"/>
+      <c r="B250" s="216"/>
       <c r="C250" s="106"/>
       <c r="D250" s="106" t="s">
         <v>407</v>
@@ -34683,4 +34759,377 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DBC65A-63D2-46B3-B8B5-A94A70B9EDFE}">
+  <dimension ref="A1:D33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30:D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>430</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="103" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="217" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="214" t="s">
+        <v>439</v>
+      </c>
+      <c r="C3" s="106" t="s">
+        <v>550</v>
+      </c>
+      <c r="D3" s="160" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="218"/>
+      <c r="B4" s="215"/>
+      <c r="C4" s="58" t="s">
+        <v>540</v>
+      </c>
+      <c r="D4" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="218"/>
+      <c r="B5" s="215"/>
+      <c r="C5" s="58" t="s">
+        <v>541</v>
+      </c>
+      <c r="D5" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="218"/>
+      <c r="B6" s="215"/>
+      <c r="C6" s="58" t="s">
+        <v>542</v>
+      </c>
+      <c r="D6" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="218"/>
+      <c r="B7" s="215"/>
+      <c r="C7" s="58" t="s">
+        <v>543</v>
+      </c>
+      <c r="D7" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="218"/>
+      <c r="B8" s="215"/>
+      <c r="C8" s="58" t="s">
+        <v>537</v>
+      </c>
+      <c r="D8" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="218"/>
+      <c r="B9" s="215"/>
+      <c r="C9" s="58" t="s">
+        <v>544</v>
+      </c>
+      <c r="D9" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="218"/>
+      <c r="B10" s="215"/>
+      <c r="C10" s="58" t="s">
+        <v>545</v>
+      </c>
+      <c r="D10" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="218"/>
+      <c r="B11" s="215"/>
+      <c r="C11" s="58" t="s">
+        <v>546</v>
+      </c>
+      <c r="D11" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="218"/>
+      <c r="B12" s="215"/>
+      <c r="C12" s="58" t="s">
+        <v>547</v>
+      </c>
+      <c r="D12" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="218"/>
+      <c r="B13" s="215"/>
+      <c r="C13" s="58" t="s">
+        <v>548</v>
+      </c>
+      <c r="D13" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="218"/>
+      <c r="B14" s="215"/>
+      <c r="C14" s="58" t="s">
+        <v>539</v>
+      </c>
+      <c r="D14" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="218"/>
+      <c r="B15" s="215"/>
+      <c r="C15" s="58" t="s">
+        <v>538</v>
+      </c>
+      <c r="D15" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="248"/>
+      <c r="B16" s="216"/>
+      <c r="C16" s="106" t="s">
+        <v>552</v>
+      </c>
+      <c r="D16" s="58" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="249" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="235" t="s">
+        <v>439</v>
+      </c>
+      <c r="C17" s="106" t="s">
+        <v>550</v>
+      </c>
+      <c r="D17" s="160" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="249"/>
+      <c r="B18" s="235"/>
+      <c r="C18" s="58" t="s">
+        <v>540</v>
+      </c>
+      <c r="D18" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="249"/>
+      <c r="B19" s="235"/>
+      <c r="C19" s="58" t="s">
+        <v>541</v>
+      </c>
+      <c r="D19" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="249"/>
+      <c r="B20" s="235"/>
+      <c r="C20" s="58" t="s">
+        <v>542</v>
+      </c>
+      <c r="D20" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="249"/>
+      <c r="B21" s="235"/>
+      <c r="C21" s="58" t="s">
+        <v>543</v>
+      </c>
+      <c r="D21" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="249"/>
+      <c r="B22" s="235"/>
+      <c r="C22" s="58" t="s">
+        <v>537</v>
+      </c>
+      <c r="D22" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="249"/>
+      <c r="B23" s="235"/>
+      <c r="C23" s="58" t="s">
+        <v>544</v>
+      </c>
+      <c r="D23" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="249"/>
+      <c r="B24" s="235"/>
+      <c r="C24" s="58" t="s">
+        <v>545</v>
+      </c>
+      <c r="D24" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="249"/>
+      <c r="B25" s="235"/>
+      <c r="C25" s="58" t="s">
+        <v>546</v>
+      </c>
+      <c r="D25" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="249"/>
+      <c r="B26" s="235"/>
+      <c r="C26" s="58" t="s">
+        <v>547</v>
+      </c>
+      <c r="D26" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="249"/>
+      <c r="B27" s="235"/>
+      <c r="C27" s="58" t="s">
+        <v>548</v>
+      </c>
+      <c r="D27" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="249"/>
+      <c r="B28" s="235"/>
+      <c r="C28" s="58" t="s">
+        <v>539</v>
+      </c>
+      <c r="D28" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="249"/>
+      <c r="B29" s="235"/>
+      <c r="C29" s="58" t="s">
+        <v>538</v>
+      </c>
+      <c r="D29" s="119" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="249"/>
+      <c r="B30" s="235"/>
+      <c r="C30" s="106" t="s">
+        <v>552</v>
+      </c>
+      <c r="D30" s="58" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="126" t="s">
+        <v>222</v>
+      </c>
+      <c r="B31" s="156" t="s">
+        <v>439</v>
+      </c>
+      <c r="C31" s="109" t="s">
+        <v>534</v>
+      </c>
+      <c r="D31" s="159" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="103" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="103"/>
+      <c r="C32" s="103"/>
+      <c r="D32" s="104"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="109" t="s">
+        <v>536</v>
+      </c>
+      <c r="B33" s="112" t="s">
+        <v>439</v>
+      </c>
+      <c r="C33" s="156" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="155" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="B3:B16"/>
+    <mergeCell ref="A17:A30"/>
+    <mergeCell ref="B17:B30"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ERR - updating changelog
</commit_message>
<xml_diff>
--- a/PIT4/Schema Publication Changelog.xlsx
+++ b/PIT4/Schema Publication Changelog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwalsh06\IdeaProjects\paye-employers-documentation\src\main\resources\PIT4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\paye-employers-documentation\src\main\resources\PIT4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF58CF23-56E8-4E81-8CE4-33ACCAD7E735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDB739B-8A3D-4160-8CFE-4492D22CFFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,9 +24,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="571">
   <si>
     <t>Document</t>
   </si>
@@ -3559,9 +3559,6 @@
     <t>New file</t>
   </si>
   <si>
-    <t xml:space="preserve">SOAP Reference </t>
-  </si>
-  <si>
     <t>Added Enhanced Reporting Check
 Run and Check Submission Web
 Services</t>
@@ -3582,9 +3579,6 @@
     <t>ERN Schema</t>
   </si>
   <si>
-    <t>Added Enhanced Reporting and ERN Web Services and Schemas</t>
-  </si>
-  <si>
     <t>1, 2.1, 3.8, 3.9</t>
   </si>
   <si>
@@ -3601,6 +3595,9 @@
   </si>
   <si>
     <t>1, 2.1, 3.10</t>
+  </si>
+  <si>
+    <t>Enhanced Reporting Validation Rules</t>
   </si>
 </sst>
 </file>
@@ -4700,38 +4697,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4754,6 +4721,66 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4775,36 +4802,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4823,14 +4820,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4841,61 +4835,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4915,6 +4861,57 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5937,7 +5934,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5947,7 +5944,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -6057,10 +6054,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="179" t="s">
+      <c r="A7" s="194" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="180" t="s">
+      <c r="B7" s="193" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -6071,8 +6068,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="179"/>
-      <c r="B8" s="180"/>
+      <c r="A8" s="194"/>
+      <c r="B8" s="193"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -6081,8 +6078,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="179"/>
-      <c r="B9" s="180"/>
+      <c r="A9" s="194"/>
+      <c r="B9" s="193"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -6091,8 +6088,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="179"/>
-      <c r="B10" s="180"/>
+      <c r="A10" s="194"/>
+      <c r="B10" s="193"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -6101,8 +6098,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="179"/>
-      <c r="B11" s="180"/>
+      <c r="A11" s="194"/>
+      <c r="B11" s="193"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -6111,8 +6108,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="179"/>
-      <c r="B12" s="180"/>
+      <c r="A12" s="194"/>
+      <c r="B12" s="193"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -6121,10 +6118,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="182" t="s">
+      <c r="A13" s="196" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="180" t="s">
+      <c r="B13" s="193" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -6135,8 +6132,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="182"/>
-      <c r="B14" s="180"/>
+      <c r="A14" s="196"/>
+      <c r="B14" s="193"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -6145,8 +6142,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="182"/>
-      <c r="B15" s="180"/>
+      <c r="A15" s="196"/>
+      <c r="B15" s="193"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -6155,10 +6152,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="183" t="s">
+      <c r="A16" s="179" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="184" t="s">
+      <c r="B16" s="188" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -6169,8 +6166,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="183"/>
-      <c r="B17" s="184"/>
+      <c r="A17" s="179"/>
+      <c r="B17" s="188"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -6179,8 +6176,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="183"/>
-      <c r="B18" s="184"/>
+      <c r="A18" s="179"/>
+      <c r="B18" s="188"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -6189,8 +6186,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="183"/>
-      <c r="B19" s="184"/>
+      <c r="A19" s="179"/>
+      <c r="B19" s="188"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -6199,8 +6196,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="183"/>
-      <c r="B20" s="184"/>
+      <c r="A20" s="179"/>
+      <c r="B20" s="188"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -6209,8 +6206,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="183"/>
-      <c r="B21" s="184"/>
+      <c r="A21" s="179"/>
+      <c r="B21" s="188"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -6219,8 +6216,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="183"/>
-      <c r="B22" s="184"/>
+      <c r="A22" s="179"/>
+      <c r="B22" s="188"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -6229,8 +6226,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="183"/>
-      <c r="B23" s="184"/>
+      <c r="A23" s="179"/>
+      <c r="B23" s="188"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -6239,26 +6236,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="183"/>
-      <c r="B24" s="184"/>
-      <c r="C24" s="183" t="s">
+      <c r="A24" s="179"/>
+      <c r="B24" s="188"/>
+      <c r="C24" s="179" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="190" t="s">
+      <c r="D24" s="180" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="183"/>
-      <c r="B25" s="184"/>
-      <c r="C25" s="183"/>
-      <c r="D25" s="190"/>
+      <c r="A25" s="179"/>
+      <c r="B25" s="188"/>
+      <c r="C25" s="179"/>
+      <c r="D25" s="180"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="179" t="s">
+      <c r="A26" s="194" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="180" t="s">
+      <c r="B26" s="193" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -6269,8 +6266,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="179"/>
-      <c r="B27" s="180"/>
+      <c r="A27" s="194"/>
+      <c r="B27" s="193"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -6297,28 +6294,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="181" t="s">
+      <c r="A30" s="195" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="180" t="s">
+      <c r="B30" s="193" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="183" t="s">
+      <c r="C30" s="179" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="193" t="s">
+      <c r="D30" s="183" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="181"/>
-      <c r="B31" s="180"/>
-      <c r="C31" s="183"/>
-      <c r="D31" s="193"/>
+      <c r="A31" s="195"/>
+      <c r="B31" s="193"/>
+      <c r="C31" s="179"/>
+      <c r="D31" s="183"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="181"/>
-      <c r="B32" s="180"/>
+      <c r="A32" s="195"/>
+      <c r="B32" s="193"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -6327,8 +6324,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="181"/>
-      <c r="B33" s="180"/>
+      <c r="A33" s="195"/>
+      <c r="B33" s="193"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -6337,8 +6334,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="181"/>
-      <c r="B34" s="180"/>
+      <c r="A34" s="195"/>
+      <c r="B34" s="193"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -6347,8 +6344,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="181"/>
-      <c r="B35" s="180"/>
+      <c r="A35" s="195"/>
+      <c r="B35" s="193"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -6357,8 +6354,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="181"/>
-      <c r="B36" s="180"/>
+      <c r="A36" s="195"/>
+      <c r="B36" s="193"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -6367,26 +6364,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="181"/>
-      <c r="B37" s="180"/>
-      <c r="C37" s="194" t="s">
+      <c r="A37" s="195"/>
+      <c r="B37" s="193"/>
+      <c r="C37" s="184" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="196" t="s">
+      <c r="D37" s="186" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="181"/>
-      <c r="B38" s="180"/>
-      <c r="C38" s="195"/>
-      <c r="D38" s="196"/>
+      <c r="A38" s="195"/>
+      <c r="B38" s="193"/>
+      <c r="C38" s="185"/>
+      <c r="D38" s="186"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="179" t="s">
+      <c r="A39" s="194" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="180" t="s">
+      <c r="B39" s="193" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -6397,8 +6394,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="179"/>
-      <c r="B40" s="180"/>
+      <c r="A40" s="194"/>
+      <c r="B40" s="193"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -6425,10 +6422,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="181" t="s">
+      <c r="A43" s="195" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="180" t="s">
+      <c r="B43" s="193" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -6437,8 +6434,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="181"/>
-      <c r="B44" s="180"/>
+      <c r="A44" s="195"/>
+      <c r="B44" s="193"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -6447,10 +6444,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="187" t="s">
+      <c r="A45" s="190" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="180" t="s">
+      <c r="B45" s="193" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -6459,8 +6456,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="188"/>
-      <c r="B46" s="180"/>
+      <c r="A46" s="191"/>
+      <c r="B46" s="193"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -6469,8 +6466,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="188"/>
-      <c r="B47" s="180"/>
+      <c r="A47" s="191"/>
+      <c r="B47" s="193"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -6479,8 +6476,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="189"/>
-      <c r="B48" s="180"/>
+      <c r="A48" s="192"/>
+      <c r="B48" s="193"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -6489,10 +6486,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="184" t="s">
+      <c r="A49" s="188" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="184" t="s">
+      <c r="B49" s="188" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -10596,8 +10593,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="184"/>
-      <c r="B50" s="184"/>
+      <c r="A50" s="188"/>
+      <c r="B50" s="188"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -14701,8 +14698,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="184"/>
-      <c r="B51" s="184"/>
+      <c r="A51" s="188"/>
+      <c r="B51" s="188"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -18806,8 +18803,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="184"/>
-      <c r="B52" s="184"/>
+      <c r="A52" s="188"/>
+      <c r="B52" s="188"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -22911,12 +22908,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="184"/>
-      <c r="B53" s="184"/>
-      <c r="C53" s="192" t="s">
+      <c r="A53" s="188"/>
+      <c r="B53" s="188"/>
+      <c r="C53" s="182" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="193" t="s">
+      <c r="D53" s="183" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -27016,10 +27013,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="184"/>
-      <c r="B54" s="184"/>
-      <c r="C54" s="192"/>
-      <c r="D54" s="193"/>
+      <c r="A54" s="188"/>
+      <c r="B54" s="188"/>
+      <c r="C54" s="182"/>
+      <c r="D54" s="183"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -31137,10 +31134,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="185" t="s">
+      <c r="A57" s="187" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="184" t="s">
+      <c r="B57" s="188" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -31151,8 +31148,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="185"/>
-      <c r="B58" s="184"/>
+      <c r="A58" s="187"/>
+      <c r="B58" s="188"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -31161,8 +31158,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="185"/>
-      <c r="B59" s="184"/>
+      <c r="A59" s="187"/>
+      <c r="B59" s="188"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -31171,8 +31168,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="185"/>
-      <c r="B60" s="184"/>
+      <c r="A60" s="187"/>
+      <c r="B60" s="188"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -31181,8 +31178,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="185"/>
-      <c r="B61" s="184"/>
+      <c r="A61" s="187"/>
+      <c r="B61" s="188"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -31191,8 +31188,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="185"/>
-      <c r="B62" s="184"/>
+      <c r="A62" s="187"/>
+      <c r="B62" s="188"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -31201,8 +31198,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="185"/>
-      <c r="B63" s="184"/>
+      <c r="A63" s="187"/>
+      <c r="B63" s="188"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -31211,16 +31208,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="185"/>
-      <c r="B64" s="184"/>
+      <c r="A64" s="187"/>
+      <c r="B64" s="188"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="185"/>
-      <c r="B65" s="184"/>
+      <c r="A65" s="187"/>
+      <c r="B65" s="188"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -31229,16 +31226,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="185"/>
-      <c r="B66" s="184"/>
+      <c r="A66" s="187"/>
+      <c r="B66" s="188"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="185"/>
-      <c r="B67" s="184"/>
+      <c r="A67" s="187"/>
+      <c r="B67" s="188"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -31247,8 +31244,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="185"/>
-      <c r="B68" s="184"/>
+      <c r="A68" s="187"/>
+      <c r="B68" s="188"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -31257,8 +31254,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="185"/>
-      <c r="B69" s="184"/>
+      <c r="A69" s="187"/>
+      <c r="B69" s="188"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -31267,8 +31264,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="185"/>
-      <c r="B70" s="184"/>
+      <c r="A70" s="187"/>
+      <c r="B70" s="188"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -31277,8 +31274,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="185"/>
-      <c r="B71" s="184"/>
+      <c r="A71" s="187"/>
+      <c r="B71" s="188"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -31287,8 +31284,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="185"/>
-      <c r="B72" s="184"/>
+      <c r="A72" s="187"/>
+      <c r="B72" s="188"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -31297,16 +31294,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="185"/>
-      <c r="B73" s="184"/>
+      <c r="A73" s="187"/>
+      <c r="B73" s="188"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="185"/>
-      <c r="B74" s="184"/>
+      <c r="A74" s="187"/>
+      <c r="B74" s="188"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -31315,18 +31312,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="185"/>
-      <c r="B75" s="184"/>
-      <c r="C75" s="191"/>
-      <c r="D75" s="186" t="s">
+      <c r="A75" s="187"/>
+      <c r="B75" s="188"/>
+      <c r="C75" s="181"/>
+      <c r="D75" s="189" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="185"/>
-      <c r="B76" s="184"/>
-      <c r="C76" s="191"/>
-      <c r="D76" s="186"/>
+      <c r="A76" s="187"/>
+      <c r="B76" s="188"/>
+      <c r="C76" s="181"/>
+      <c r="D76" s="189"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -31350,8 +31347,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -31360,29 +31357,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -31397,6 +31378,22 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -31450,10 +31447,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="179" t="s">
+      <c r="A4" s="194" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="193" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -31464,133 +31461,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="179"/>
-      <c r="B5" s="180"/>
-      <c r="C5" s="206" t="s">
+      <c r="A5" s="194"/>
+      <c r="B5" s="193"/>
+      <c r="C5" s="204" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="205" t="s">
+      <c r="D5" s="203" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="179"/>
-      <c r="B6" s="180"/>
-      <c r="C6" s="206"/>
-      <c r="D6" s="205"/>
+      <c r="A6" s="194"/>
+      <c r="B6" s="193"/>
+      <c r="C6" s="204"/>
+      <c r="D6" s="203"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="179"/>
-      <c r="B7" s="180"/>
+      <c r="A7" s="194"/>
+      <c r="B7" s="193"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="179"/>
-      <c r="B8" s="180"/>
+      <c r="A8" s="194"/>
+      <c r="B8" s="193"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="179"/>
-      <c r="B9" s="180"/>
+      <c r="A9" s="194"/>
+      <c r="B9" s="193"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="182" t="s">
+      <c r="A10" s="196" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="180" t="s">
+      <c r="B10" s="193" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="204"/>
-      <c r="D10" s="205" t="s">
+      <c r="C10" s="206"/>
+      <c r="D10" s="203" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="182"/>
-      <c r="B11" s="180"/>
-      <c r="C11" s="204"/>
-      <c r="D11" s="205"/>
+      <c r="A11" s="196"/>
+      <c r="B11" s="193"/>
+      <c r="C11" s="206"/>
+      <c r="D11" s="203"/>
     </row>
     <row r="12" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="182"/>
-      <c r="B12" s="180"/>
-      <c r="C12" s="204"/>
-      <c r="D12" s="205"/>
+      <c r="A12" s="196"/>
+      <c r="B12" s="193"/>
+      <c r="C12" s="206"/>
+      <c r="D12" s="203"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="183" t="s">
+      <c r="A13" s="179" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="184" t="s">
+      <c r="B13" s="188" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="207"/>
-      <c r="D13" s="205" t="s">
+      <c r="C13" s="205"/>
+      <c r="D13" s="203" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="183"/>
-      <c r="B14" s="184"/>
-      <c r="C14" s="207"/>
-      <c r="D14" s="205"/>
+      <c r="A14" s="179"/>
+      <c r="B14" s="188"/>
+      <c r="C14" s="205"/>
+      <c r="D14" s="203"/>
     </row>
     <row r="15" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="183"/>
-      <c r="B15" s="184"/>
-      <c r="C15" s="207"/>
+      <c r="A15" s="179"/>
+      <c r="B15" s="188"/>
+      <c r="C15" s="205"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="183"/>
-      <c r="B16" s="184"/>
-      <c r="C16" s="207"/>
+      <c r="A16" s="179"/>
+      <c r="B16" s="188"/>
+      <c r="C16" s="205"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="183"/>
-      <c r="B17" s="184"/>
-      <c r="C17" s="207"/>
+      <c r="A17" s="179"/>
+      <c r="B17" s="188"/>
+      <c r="C17" s="205"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="183"/>
-      <c r="B18" s="184"/>
-      <c r="C18" s="207"/>
+      <c r="A18" s="179"/>
+      <c r="B18" s="188"/>
+      <c r="C18" s="205"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="183"/>
-      <c r="B19" s="184"/>
-      <c r="C19" s="207"/>
+      <c r="A19" s="179"/>
+      <c r="B19" s="188"/>
+      <c r="C19" s="205"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="183"/>
-      <c r="B20" s="184"/>
-      <c r="C20" s="207"/>
+      <c r="A20" s="179"/>
+      <c r="B20" s="188"/>
+      <c r="C20" s="205"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="183"/>
-      <c r="B21" s="184"/>
-      <c r="C21" s="207"/>
+      <c r="A21" s="179"/>
+      <c r="B21" s="188"/>
+      <c r="C21" s="205"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="183"/>
-      <c r="B22" s="184"/>
-      <c r="C22" s="207"/>
+      <c r="A22" s="179"/>
+      <c r="B22" s="188"/>
+      <c r="C22" s="205"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="183"/>
-      <c r="B23" s="184"/>
-      <c r="C23" s="207"/>
+      <c r="A23" s="179"/>
+      <c r="B23" s="188"/>
+      <c r="C23" s="205"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -31688,10 +31685,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="208" t="s">
+      <c r="A32" s="197" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="211" t="s">
+      <c r="B32" s="200" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -31702,26 +31699,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="209"/>
-      <c r="B33" s="212"/>
+      <c r="A33" s="198"/>
+      <c r="B33" s="201"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="209"/>
-      <c r="B34" s="212"/>
+      <c r="A34" s="198"/>
+      <c r="B34" s="201"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="209"/>
-      <c r="B35" s="212"/>
+      <c r="A35" s="198"/>
+      <c r="B35" s="201"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="210"/>
-      <c r="B36" s="213"/>
+      <c r="A36" s="199"/>
+      <c r="B36" s="202"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -31750,10 +31747,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="181" t="s">
+      <c r="A39" s="195" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="180" t="s">
+      <c r="B39" s="193" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -31764,8 +31761,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="181"/>
-      <c r="B40" s="180"/>
+      <c r="A40" s="195"/>
+      <c r="B40" s="193"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -31774,84 +31771,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="179" t="s">
+      <c r="A41" s="194" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="180" t="s">
+      <c r="B41" s="193" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="204" t="s">
+      <c r="C41" s="206" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="183" t="s">
+      <c r="D41" s="179" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="179"/>
-      <c r="B42" s="180"/>
-      <c r="C42" s="204"/>
-      <c r="D42" s="183"/>
+      <c r="A42" s="194"/>
+      <c r="B42" s="193"/>
+      <c r="C42" s="206"/>
+      <c r="D42" s="179"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="179"/>
-      <c r="B43" s="180"/>
-      <c r="C43" s="204" t="s">
+      <c r="A43" s="194"/>
+      <c r="B43" s="193"/>
+      <c r="C43" s="206" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="186" t="s">
+      <c r="D43" s="189" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="179"/>
-      <c r="B44" s="180"/>
-      <c r="C44" s="204"/>
-      <c r="D44" s="186"/>
+      <c r="A44" s="194"/>
+      <c r="B44" s="193"/>
+      <c r="C44" s="206"/>
+      <c r="D44" s="189"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="185" t="s">
+      <c r="A45" s="187" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="184" t="s">
+      <c r="B45" s="188" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="200"/>
+      <c r="C45" s="210"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="185"/>
-      <c r="B46" s="184"/>
-      <c r="C46" s="201"/>
-      <c r="D46" s="197" t="s">
+      <c r="A46" s="187"/>
+      <c r="B46" s="188"/>
+      <c r="C46" s="211"/>
+      <c r="D46" s="207" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="185"/>
-      <c r="B47" s="184"/>
-      <c r="C47" s="201"/>
-      <c r="D47" s="198"/>
+      <c r="A47" s="187"/>
+      <c r="B47" s="188"/>
+      <c r="C47" s="211"/>
+      <c r="D47" s="208"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="185"/>
-      <c r="B48" s="184"/>
-      <c r="C48" s="202"/>
-      <c r="D48" s="198"/>
+      <c r="A48" s="187"/>
+      <c r="B48" s="188"/>
+      <c r="C48" s="212"/>
+      <c r="D48" s="208"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="185"/>
-      <c r="B49" s="184"/>
-      <c r="C49" s="192"/>
-      <c r="D49" s="198"/>
+      <c r="A49" s="187"/>
+      <c r="B49" s="188"/>
+      <c r="C49" s="182"/>
+      <c r="D49" s="208"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="185"/>
-      <c r="B50" s="184"/>
-      <c r="C50" s="192"/>
-      <c r="D50" s="199"/>
+      <c r="A50" s="187"/>
+      <c r="B50" s="188"/>
+      <c r="C50" s="182"/>
+      <c r="D50" s="209"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -31874,10 +31871,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="184" t="s">
+      <c r="A53" s="188" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="184" t="s">
+      <c r="B53" s="188" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -31888,8 +31885,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="184"/>
-      <c r="B54" s="184"/>
+      <c r="A54" s="188"/>
+      <c r="B54" s="188"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -31898,8 +31895,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="184"/>
-      <c r="B55" s="184"/>
+      <c r="A55" s="188"/>
+      <c r="B55" s="188"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -31908,9 +31905,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="184"/>
-      <c r="B56" s="184"/>
-      <c r="C56" s="203" t="s">
+      <c r="A56" s="188"/>
+      <c r="B56" s="188"/>
+      <c r="C56" s="213" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -31918,16 +31915,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="184"/>
-      <c r="B57" s="184"/>
-      <c r="C57" s="203"/>
+      <c r="A57" s="188"/>
+      <c r="B57" s="188"/>
+      <c r="C57" s="213"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="184"/>
-      <c r="B58" s="184"/>
+      <c r="A58" s="188"/>
+      <c r="B58" s="188"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -31936,8 +31933,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="184"/>
-      <c r="B59" s="184"/>
+      <c r="A59" s="188"/>
+      <c r="B59" s="188"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31946,9 +31943,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="184"/>
-      <c r="B60" s="184"/>
-      <c r="C60" s="203" t="s">
+      <c r="A60" s="188"/>
+      <c r="B60" s="188"/>
+      <c r="C60" s="213" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31956,25 +31953,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="184"/>
-      <c r="B61" s="184"/>
-      <c r="C61" s="203"/>
+      <c r="A61" s="188"/>
+      <c r="B61" s="188"/>
+      <c r="C61" s="213"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="184"/>
-      <c r="B62" s="184"/>
-      <c r="C62" s="203"/>
+      <c r="A62" s="188"/>
+      <c r="B62" s="188"/>
+      <c r="C62" s="213"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="184"/>
-      <c r="B63" s="184"/>
-      <c r="C63" s="204" t="s">
+      <c r="A63" s="188"/>
+      <c r="B63" s="188"/>
+      <c r="C63" s="206" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31982,30 +31979,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="184"/>
-      <c r="B64" s="184"/>
-      <c r="C64" s="204"/>
-      <c r="D64" s="186" t="s">
+      <c r="A64" s="188"/>
+      <c r="B64" s="188"/>
+      <c r="C64" s="206"/>
+      <c r="D64" s="189" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="184"/>
-      <c r="B65" s="184"/>
-      <c r="C65" s="204"/>
-      <c r="D65" s="186"/>
+      <c r="A65" s="188"/>
+      <c r="B65" s="188"/>
+      <c r="C65" s="206"/>
+      <c r="D65" s="189"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="184"/>
-      <c r="B66" s="184"/>
-      <c r="C66" s="204"/>
-      <c r="D66" s="186"/>
+      <c r="A66" s="188"/>
+      <c r="B66" s="188"/>
+      <c r="C66" s="206"/>
+      <c r="D66" s="189"/>
     </row>
     <row r="67" spans="1:4" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="184"/>
-      <c r="B67" s="184"/>
-      <c r="C67" s="204"/>
-      <c r="D67" s="186"/>
+      <c r="A67" s="188"/>
+      <c r="B67" s="188"/>
+      <c r="C67" s="206"/>
+      <c r="D67" s="189"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -32061,23 +32058,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -32094,6 +32074,23 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -32173,7 +32170,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="223" t="s">
+      <c r="A6" s="222" t="s">
         <v>438</v>
       </c>
       <c r="B6" s="217" t="s">
@@ -32185,7 +32182,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="224"/>
+      <c r="A7" s="223"/>
       <c r="B7" s="218"/>
       <c r="C7" s="100"/>
       <c r="D7" s="58" t="s">
@@ -32193,7 +32190,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="224"/>
+      <c r="A8" s="223"/>
       <c r="B8" s="218"/>
       <c r="C8" s="100"/>
       <c r="D8" s="140" t="s">
@@ -32201,7 +32198,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="224"/>
+      <c r="A9" s="223"/>
       <c r="B9" s="218"/>
       <c r="C9" s="100"/>
       <c r="D9" s="140" t="s">
@@ -32209,7 +32206,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="225"/>
+      <c r="A10" s="224"/>
       <c r="B10" s="219"/>
       <c r="C10" s="100" t="s">
         <v>498</v>
@@ -32261,7 +32258,7 @@
       <c r="D14" s="104"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="227" t="s">
+      <c r="A15" s="234" t="s">
         <v>247</v>
       </c>
       <c r="B15" s="217" t="s">
@@ -32275,7 +32272,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="228"/>
+      <c r="A16" s="236"/>
       <c r="B16" s="219"/>
       <c r="C16" s="128" t="s">
         <v>474</v>
@@ -32415,7 +32412,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="223" t="s">
+      <c r="A29" s="222" t="s">
         <v>452</v>
       </c>
       <c r="B29" s="217" t="s">
@@ -32429,7 +32426,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="224"/>
+      <c r="A30" s="223"/>
       <c r="B30" s="218"/>
       <c r="C30" s="100" t="s">
         <v>453</v>
@@ -32439,7 +32436,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="224"/>
+      <c r="A31" s="223"/>
       <c r="B31" s="218"/>
       <c r="C31" s="100">
         <v>3.3</v>
@@ -32449,7 +32446,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="224"/>
+      <c r="A32" s="223"/>
       <c r="B32" s="218"/>
       <c r="C32" s="130">
         <v>3</v>
@@ -32459,7 +32456,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="225"/>
+      <c r="A33" s="224"/>
       <c r="B33" s="219"/>
       <c r="C33" s="130">
         <v>3.5</v>
@@ -32469,7 +32466,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="223" t="s">
+      <c r="A34" s="222" t="s">
         <v>457</v>
       </c>
       <c r="B34" s="217" t="s">
@@ -32481,7 +32478,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="225"/>
+      <c r="A35" s="224"/>
       <c r="B35" s="219"/>
       <c r="C35" s="100"/>
       <c r="D35" s="67" t="s">
@@ -32489,7 +32486,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="226" t="s">
+      <c r="A36" s="246" t="s">
         <v>501</v>
       </c>
       <c r="B36" s="217" t="s">
@@ -32500,7 +32497,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="226"/>
+      <c r="A37" s="246"/>
       <c r="B37" s="218"/>
       <c r="C37" s="144" t="s">
         <v>508</v>
@@ -32510,7 +32507,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="226"/>
+      <c r="A38" s="246"/>
       <c r="B38" s="218"/>
       <c r="C38" s="58" t="s">
         <v>506</v>
@@ -32520,7 +32517,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="226"/>
+      <c r="A39" s="246"/>
       <c r="B39" s="218"/>
       <c r="C39" s="61" t="s">
         <v>509</v>
@@ -32586,7 +32583,7 @@
       <c r="B45" s="217" t="s">
         <v>439</v>
       </c>
-      <c r="C45" s="229"/>
+      <c r="C45" s="241"/>
       <c r="D45" s="145" t="s">
         <v>510</v>
       </c>
@@ -32594,7 +32591,7 @@
     <row r="46" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="216"/>
       <c r="B46" s="219"/>
-      <c r="C46" s="230"/>
+      <c r="C46" s="242"/>
       <c r="D46" s="145" t="s">
         <v>518</v>
       </c>
@@ -32644,10 +32641,10 @@
       <c r="D50" s="104"/>
     </row>
     <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="226" t="s">
+      <c r="A51" s="246" t="s">
         <v>336</v>
       </c>
-      <c r="B51" s="235" t="s">
+      <c r="B51" s="247" t="s">
         <v>439</v>
       </c>
       <c r="C51" s="100" t="s">
@@ -32658,8 +32655,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="226"/>
-      <c r="B52" s="235"/>
+      <c r="A52" s="246"/>
+      <c r="B52" s="247"/>
       <c r="C52" s="100" t="s">
         <v>341</v>
       </c>
@@ -32668,8 +32665,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="226"/>
-      <c r="B53" s="235"/>
+      <c r="A53" s="246"/>
+      <c r="B53" s="247"/>
       <c r="C53" s="100" t="s">
         <v>337</v>
       </c>
@@ -32686,10 +32683,10 @@
       <c r="D54" s="104"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="236" t="s">
+      <c r="A55" s="237" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="231" t="s">
+      <c r="B55" s="238" t="s">
         <v>439</v>
       </c>
       <c r="C55" s="106"/>
@@ -32698,8 +32695,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="236"/>
-      <c r="B56" s="231"/>
+      <c r="A56" s="237"/>
+      <c r="B56" s="238"/>
       <c r="C56" s="136" t="s">
         <v>234</v>
       </c>
@@ -32708,8 +32705,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="236"/>
-      <c r="B57" s="231"/>
+      <c r="A57" s="237"/>
+      <c r="B57" s="238"/>
       <c r="C57" s="139" t="s">
         <v>484</v>
       </c>
@@ -32718,8 +32715,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="236"/>
-      <c r="B58" s="231"/>
+      <c r="A58" s="237"/>
+      <c r="B58" s="238"/>
       <c r="C58" s="141" t="s">
         <v>484</v>
       </c>
@@ -32728,8 +32725,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="236"/>
-      <c r="B59" s="231"/>
+      <c r="A59" s="237"/>
+      <c r="B59" s="238"/>
       <c r="C59" s="139" t="s">
         <v>498</v>
       </c>
@@ -32738,8 +32735,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="236"/>
-      <c r="B60" s="231"/>
+      <c r="A60" s="237"/>
+      <c r="B60" s="238"/>
       <c r="C60" s="112" t="s">
         <v>498</v>
       </c>
@@ -32748,7 +32745,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="227" t="s">
+      <c r="A61" s="234" t="s">
         <v>74</v>
       </c>
       <c r="B61" s="217" t="s">
@@ -32762,7 +32759,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="239"/>
+      <c r="A62" s="235"/>
       <c r="B62" s="218"/>
       <c r="C62" s="136" t="s">
         <v>463</v>
@@ -32772,7 +32769,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="228"/>
+      <c r="A63" s="236"/>
       <c r="B63" s="219"/>
       <c r="C63" s="137" t="s">
         <v>481</v>
@@ -32822,10 +32819,10 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="236" t="s">
+      <c r="A67" s="237" t="s">
         <v>269</v>
       </c>
-      <c r="B67" s="231" t="s">
+      <c r="B67" s="238" t="s">
         <v>439</v>
       </c>
       <c r="C67" s="106" t="s">
@@ -32836,24 +32833,24 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="236"/>
-      <c r="B68" s="231"/>
+      <c r="A68" s="237"/>
+      <c r="B68" s="238"/>
       <c r="C68" s="106"/>
       <c r="D68" s="80" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="236"/>
-      <c r="B69" s="231"/>
+      <c r="A69" s="237"/>
+      <c r="B69" s="238"/>
       <c r="C69" s="106"/>
       <c r="D69" s="106" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="236"/>
-      <c r="B70" s="231"/>
+      <c r="A70" s="237"/>
+      <c r="B70" s="238"/>
       <c r="C70" s="111" t="s">
         <v>319</v>
       </c>
@@ -32862,8 +32859,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="236"/>
-      <c r="B71" s="231"/>
+      <c r="A71" s="237"/>
+      <c r="B71" s="238"/>
       <c r="C71" s="112" t="s">
         <v>398</v>
       </c>
@@ -32884,7 +32881,7 @@
       <c r="D72" s="106"/>
     </row>
     <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="232" t="s">
+      <c r="A73" s="243" t="s">
         <v>165</v>
       </c>
       <c r="B73" s="217" t="s">
@@ -32896,7 +32893,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="233"/>
+      <c r="A74" s="244"/>
       <c r="B74" s="218"/>
       <c r="C74" s="112" t="s">
         <v>355</v>
@@ -32906,7 +32903,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="233"/>
+      <c r="A75" s="244"/>
       <c r="B75" s="218"/>
       <c r="C75" s="112" t="s">
         <v>353</v>
@@ -32916,7 +32913,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="233"/>
+      <c r="A76" s="244"/>
       <c r="B76" s="218"/>
       <c r="C76" s="115" t="s">
         <v>361</v>
@@ -32926,7 +32923,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="233"/>
+      <c r="A77" s="244"/>
       <c r="B77" s="218"/>
       <c r="C77" s="112" t="s">
         <v>353</v>
@@ -32936,7 +32933,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="233"/>
+      <c r="A78" s="244"/>
       <c r="B78" s="218"/>
       <c r="C78" s="112" t="s">
         <v>365</v>
@@ -32946,7 +32943,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="233"/>
+      <c r="A79" s="244"/>
       <c r="B79" s="218"/>
       <c r="C79" s="112" t="s">
         <v>353</v>
@@ -32956,7 +32953,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="233"/>
+      <c r="A80" s="244"/>
       <c r="B80" s="218"/>
       <c r="C80" s="112" t="s">
         <v>464</v>
@@ -32966,7 +32963,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="233"/>
+      <c r="A81" s="244"/>
       <c r="B81" s="218"/>
       <c r="C81" s="133" t="s">
         <v>466</v>
@@ -32976,7 +32973,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="233"/>
+      <c r="A82" s="244"/>
       <c r="B82" s="218"/>
       <c r="C82" s="133" t="s">
         <v>353</v>
@@ -32986,7 +32983,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="233"/>
+      <c r="A83" s="244"/>
       <c r="B83" s="218"/>
       <c r="C83" s="138" t="s">
         <v>466</v>
@@ -32996,7 +32993,7 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="233"/>
+      <c r="A84" s="244"/>
       <c r="B84" s="218"/>
       <c r="C84" s="112" t="s">
         <v>353</v>
@@ -33006,7 +33003,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="233"/>
+      <c r="A85" s="244"/>
       <c r="B85" s="218"/>
       <c r="C85" s="112" t="s">
         <v>498</v>
@@ -33016,7 +33013,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="233"/>
+      <c r="A86" s="244"/>
       <c r="B86" s="218"/>
       <c r="C86" s="112" t="s">
         <v>498</v>
@@ -33026,7 +33023,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="233"/>
+      <c r="A87" s="244"/>
       <c r="B87" s="218"/>
       <c r="C87" s="151" t="s">
         <v>520</v>
@@ -33036,7 +33033,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="234"/>
+      <c r="A88" s="245"/>
       <c r="B88" s="219"/>
       <c r="C88" s="112" t="s">
         <v>498</v>
@@ -33086,7 +33083,7 @@
       <c r="D91" s="113"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="240" t="s">
+      <c r="A92" s="225" t="s">
         <v>363</v>
       </c>
       <c r="B92" s="217" t="s">
@@ -33098,7 +33095,7 @@
       <c r="D92" s="113"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="244"/>
+      <c r="A93" s="226"/>
       <c r="B93" s="219"/>
       <c r="C93" s="112" t="s">
         <v>398</v>
@@ -33116,7 +33113,7 @@
       <c r="D94" s="103"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="240" t="s">
+      <c r="A95" s="225" t="s">
         <v>236</v>
       </c>
       <c r="B95" s="217" t="s">
@@ -33128,7 +33125,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="241"/>
+      <c r="A96" s="227"/>
       <c r="B96" s="218"/>
       <c r="C96" s="106"/>
       <c r="D96" s="106" t="s">
@@ -33136,7 +33133,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="241"/>
+      <c r="A97" s="227"/>
       <c r="B97" s="218"/>
       <c r="C97" s="106"/>
       <c r="D97" s="106" t="s">
@@ -33144,7 +33141,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="241"/>
+      <c r="A98" s="227"/>
       <c r="B98" s="218"/>
       <c r="C98" s="106" t="s">
         <v>294</v>
@@ -33154,7 +33151,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="241"/>
+      <c r="A99" s="227"/>
       <c r="B99" s="218"/>
       <c r="C99" s="106" t="s">
         <v>322</v>
@@ -33164,7 +33161,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="241"/>
+      <c r="A100" s="227"/>
       <c r="B100" s="218"/>
       <c r="C100" s="106" t="s">
         <v>367</v>
@@ -33174,7 +33171,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="241"/>
+      <c r="A101" s="227"/>
       <c r="B101" s="218"/>
       <c r="C101" s="119" t="s">
         <v>468</v>
@@ -33184,7 +33181,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="241"/>
+      <c r="A102" s="227"/>
       <c r="B102" s="218"/>
       <c r="C102" s="58" t="s">
         <v>37</v>
@@ -33194,7 +33191,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="241"/>
+      <c r="A103" s="227"/>
       <c r="B103" s="218"/>
       <c r="C103" s="130" t="s">
         <v>353</v>
@@ -33204,7 +33201,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="241"/>
+      <c r="A104" s="227"/>
       <c r="B104" s="218"/>
       <c r="C104" s="130" t="s">
         <v>466</v>
@@ -33214,7 +33211,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="241"/>
+      <c r="A105" s="227"/>
       <c r="B105" s="218"/>
       <c r="C105" s="130" t="s">
         <v>367</v>
@@ -33224,7 +33221,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="241"/>
+      <c r="A106" s="227"/>
       <c r="B106" s="218"/>
       <c r="C106" s="130" t="s">
         <v>353</v>
@@ -33234,7 +33231,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="241"/>
+      <c r="A107" s="227"/>
       <c r="B107" s="218"/>
       <c r="C107" s="130" t="s">
         <v>498</v>
@@ -33244,7 +33241,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="241"/>
+      <c r="A108" s="227"/>
       <c r="B108" s="218"/>
       <c r="C108" s="109" t="s">
         <v>498</v>
@@ -33254,7 +33251,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="241"/>
+      <c r="A109" s="227"/>
       <c r="B109" s="218"/>
       <c r="C109" s="151" t="s">
         <v>520</v>
@@ -33264,7 +33261,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="244"/>
+      <c r="A110" s="226"/>
       <c r="B110" s="219"/>
       <c r="C110" s="109" t="s">
         <v>498</v>
@@ -33274,7 +33271,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="245" t="s">
+      <c r="A111" s="228" t="s">
         <v>27</v>
       </c>
       <c r="B111" s="217" t="s">
@@ -33288,7 +33285,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="246"/>
+      <c r="A112" s="229"/>
       <c r="B112" s="218"/>
       <c r="C112" s="106" t="s">
         <v>297</v>
@@ -33298,7 +33295,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="246"/>
+      <c r="A113" s="229"/>
       <c r="B113" s="218"/>
       <c r="C113" s="106"/>
       <c r="D113" s="106" t="s">
@@ -33306,7 +33303,7 @@
       </c>
     </row>
     <row r="114" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="246"/>
+      <c r="A114" s="229"/>
       <c r="B114" s="218"/>
       <c r="C114" s="117" t="s">
         <v>323</v>
@@ -33316,7 +33313,7 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="246"/>
+      <c r="A115" s="229"/>
       <c r="B115" s="218"/>
       <c r="C115" s="117" t="s">
         <v>353</v>
@@ -33326,7 +33323,7 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="246"/>
+      <c r="A116" s="229"/>
       <c r="B116" s="218"/>
       <c r="C116" s="117" t="s">
         <v>361</v>
@@ -33336,7 +33333,7 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="246"/>
+      <c r="A117" s="229"/>
       <c r="B117" s="218"/>
       <c r="C117" s="117" t="s">
         <v>365</v>
@@ -33346,7 +33343,7 @@
       </c>
     </row>
     <row r="118" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="246"/>
+      <c r="A118" s="229"/>
       <c r="B118" s="218"/>
       <c r="C118" s="117" t="s">
         <v>375</v>
@@ -33356,7 +33353,7 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="246"/>
+      <c r="A119" s="229"/>
       <c r="B119" s="218"/>
       <c r="C119" s="109" t="s">
         <v>353</v>
@@ -33366,7 +33363,7 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="246"/>
+      <c r="A120" s="229"/>
       <c r="B120" s="218"/>
       <c r="C120" s="109" t="s">
         <v>464</v>
@@ -33376,7 +33373,7 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="246"/>
+      <c r="A121" s="229"/>
       <c r="B121" s="218"/>
       <c r="C121" s="130" t="s">
         <v>466</v>
@@ -33386,7 +33383,7 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="246"/>
+      <c r="A122" s="229"/>
       <c r="B122" s="218"/>
       <c r="C122" s="130" t="s">
         <v>353</v>
@@ -33396,7 +33393,7 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="246"/>
+      <c r="A123" s="229"/>
       <c r="B123" s="218"/>
       <c r="C123" s="130" t="s">
         <v>466</v>
@@ -33406,7 +33403,7 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="246"/>
+      <c r="A124" s="229"/>
       <c r="B124" s="218"/>
       <c r="C124" s="130" t="s">
         <v>367</v>
@@ -33416,7 +33413,7 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="246"/>
+      <c r="A125" s="229"/>
       <c r="B125" s="218"/>
       <c r="C125" s="130" t="s">
         <v>353</v>
@@ -33426,7 +33423,7 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="246"/>
+      <c r="A126" s="229"/>
       <c r="B126" s="218"/>
       <c r="C126" s="130" t="s">
         <v>498</v>
@@ -33436,7 +33433,7 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="246"/>
+      <c r="A127" s="229"/>
       <c r="B127" s="218"/>
       <c r="C127" s="109" t="s">
         <v>498</v>
@@ -33446,7 +33443,7 @@
       </c>
     </row>
     <row r="128" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A128" s="246"/>
+      <c r="A128" s="229"/>
       <c r="B128" s="218"/>
       <c r="C128" s="151" t="s">
         <v>520</v>
@@ -33456,7 +33453,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="247"/>
+      <c r="A129" s="230"/>
       <c r="B129" s="219"/>
       <c r="C129" s="109" t="s">
         <v>498</v>
@@ -33466,13 +33463,13 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="227" t="s">
+      <c r="A130" s="234" t="s">
         <v>222</v>
       </c>
       <c r="B130" s="217" t="s">
         <v>439</v>
       </c>
-      <c r="C130" s="248" t="s">
+      <c r="C130" s="231" t="s">
         <v>238</v>
       </c>
       <c r="D130" s="96" t="s">
@@ -33480,17 +33477,17 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="239"/>
+      <c r="A131" s="235"/>
       <c r="B131" s="218"/>
-      <c r="C131" s="249"/>
+      <c r="C131" s="232"/>
       <c r="D131" s="113" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="239"/>
+      <c r="A132" s="235"/>
       <c r="B132" s="218"/>
-      <c r="C132" s="250" t="s">
+      <c r="C132" s="233" t="s">
         <v>239</v>
       </c>
       <c r="D132" s="106" t="s">
@@ -33498,15 +33495,15 @@
       </c>
     </row>
     <row r="133" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A133" s="239"/>
+      <c r="A133" s="235"/>
       <c r="B133" s="218"/>
-      <c r="C133" s="250"/>
+      <c r="C133" s="233"/>
       <c r="D133" s="119" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="239"/>
+      <c r="A134" s="235"/>
       <c r="B134" s="218"/>
       <c r="C134" s="112" t="s">
         <v>301</v>
@@ -33516,7 +33513,7 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="239"/>
+      <c r="A135" s="235"/>
       <c r="B135" s="218"/>
       <c r="C135" s="112">
         <v>2.1</v>
@@ -33526,7 +33523,7 @@
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="239"/>
+      <c r="A136" s="235"/>
       <c r="B136" s="218"/>
       <c r="C136" s="112" t="s">
         <v>238</v>
@@ -33536,7 +33533,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="239"/>
+      <c r="A137" s="235"/>
       <c r="B137" s="218"/>
       <c r="C137" s="112" t="s">
         <v>238</v>
@@ -33546,7 +33543,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="239"/>
+      <c r="A138" s="235"/>
       <c r="B138" s="218"/>
       <c r="C138" s="112" t="s">
         <v>238</v>
@@ -33556,7 +33553,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="239"/>
+      <c r="A139" s="235"/>
       <c r="B139" s="218"/>
       <c r="C139" s="120" t="s">
         <v>372</v>
@@ -33566,7 +33563,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="239"/>
+      <c r="A140" s="235"/>
       <c r="B140" s="218"/>
       <c r="C140" s="112">
         <v>2.1</v>
@@ -33576,7 +33573,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="239"/>
+      <c r="A141" s="235"/>
       <c r="B141" s="218"/>
       <c r="C141" s="112" t="s">
         <v>238</v>
@@ -33586,7 +33583,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="239"/>
+      <c r="A142" s="235"/>
       <c r="B142" s="218"/>
       <c r="C142" s="112" t="s">
         <v>238</v>
@@ -33596,7 +33593,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="239"/>
+      <c r="A143" s="235"/>
       <c r="B143" s="218"/>
       <c r="C143" s="112">
         <v>2.1</v>
@@ -33606,7 +33603,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="245" t="s">
+      <c r="A144" s="228" t="s">
         <v>290</v>
       </c>
       <c r="B144" s="217" t="s">
@@ -33620,7 +33617,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A145" s="246"/>
+      <c r="A145" s="229"/>
       <c r="B145" s="218"/>
       <c r="C145" s="119" t="s">
         <v>275</v>
@@ -33630,7 +33627,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="247"/>
+      <c r="A146" s="230"/>
       <c r="B146" s="219"/>
       <c r="C146" s="106" t="s">
         <v>344</v>
@@ -33640,7 +33637,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="240" t="s">
+      <c r="A147" s="225" t="s">
         <v>364</v>
       </c>
       <c r="B147" s="217" t="s">
@@ -33652,7 +33649,7 @@
       <c r="D147" s="106"/>
     </row>
     <row r="148" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="241"/>
+      <c r="A148" s="227"/>
       <c r="B148" s="218"/>
       <c r="C148" s="112" t="s">
         <v>372</v>
@@ -33662,7 +33659,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="241"/>
+      <c r="A149" s="227"/>
       <c r="B149" s="218"/>
       <c r="C149" s="112">
         <v>2.1</v>
@@ -33672,7 +33669,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="241"/>
+      <c r="A150" s="227"/>
       <c r="B150" s="218"/>
       <c r="C150" s="112" t="s">
         <v>239</v>
@@ -33682,7 +33679,7 @@
       </c>
     </row>
     <row r="151" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="241"/>
+      <c r="A151" s="227"/>
       <c r="B151" s="218"/>
       <c r="C151" s="112" t="s">
         <v>238</v>
@@ -33712,7 +33709,7 @@
       <c r="D153" s="113"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="227" t="s">
+      <c r="A154" s="234" t="s">
         <v>255</v>
       </c>
       <c r="B154" s="217" t="s">
@@ -33724,7 +33721,7 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="239"/>
+      <c r="A155" s="235"/>
       <c r="B155" s="218"/>
       <c r="C155" s="106"/>
       <c r="D155" s="106" t="s">
@@ -33732,7 +33729,7 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="239"/>
+      <c r="A156" s="235"/>
       <c r="B156" s="218"/>
       <c r="C156" s="106"/>
       <c r="D156" s="113" t="s">
@@ -33740,7 +33737,7 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="239"/>
+      <c r="A157" s="235"/>
       <c r="B157" s="218"/>
       <c r="C157" s="106" t="s">
         <v>418</v>
@@ -33750,7 +33747,7 @@
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="239"/>
+      <c r="A158" s="235"/>
       <c r="B158" s="218"/>
       <c r="C158" s="106" t="s">
         <v>423</v>
@@ -33760,7 +33757,7 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="239"/>
+      <c r="A159" s="235"/>
       <c r="B159" s="218"/>
       <c r="C159" s="106" t="s">
         <v>484</v>
@@ -33770,7 +33767,7 @@
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="239"/>
+      <c r="A160" s="235"/>
       <c r="B160" s="218"/>
       <c r="C160" s="106" t="s">
         <v>498</v>
@@ -33780,10 +33777,10 @@
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="236" t="s">
+      <c r="A161" s="237" t="s">
         <v>328</v>
       </c>
-      <c r="B161" s="231" t="s">
+      <c r="B161" s="238" t="s">
         <v>439</v>
       </c>
       <c r="C161" s="80" t="s">
@@ -33794,8 +33791,8 @@
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="236"/>
-      <c r="B162" s="231"/>
+      <c r="A162" s="237"/>
+      <c r="B162" s="238"/>
       <c r="C162" s="106" t="s">
         <v>405</v>
       </c>
@@ -33804,42 +33801,42 @@
       </c>
     </row>
     <row r="163" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A163" s="236"/>
-      <c r="B163" s="231"/>
+      <c r="A163" s="237"/>
+      <c r="B163" s="238"/>
       <c r="C163" s="122" t="s">
         <v>408</v>
       </c>
-      <c r="D163" s="242" t="s">
+      <c r="D163" s="220" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A164" s="236"/>
-      <c r="B164" s="231"/>
+      <c r="A164" s="237"/>
+      <c r="B164" s="238"/>
       <c r="C164" s="122" t="s">
         <v>409</v>
       </c>
-      <c r="D164" s="243"/>
+      <c r="D164" s="221"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="236"/>
-      <c r="B165" s="231"/>
+      <c r="A165" s="237"/>
+      <c r="B165" s="238"/>
       <c r="C165" s="122" t="s">
         <v>410</v>
       </c>
-      <c r="D165" s="243"/>
+      <c r="D165" s="221"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="236"/>
-      <c r="B166" s="231"/>
+      <c r="A166" s="237"/>
+      <c r="B166" s="238"/>
       <c r="C166" s="122" t="s">
         <v>411</v>
       </c>
-      <c r="D166" s="243"/>
+      <c r="D166" s="221"/>
     </row>
     <row r="167" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A167" s="236"/>
-      <c r="B167" s="231"/>
+      <c r="A167" s="237"/>
+      <c r="B167" s="238"/>
       <c r="C167" s="122" t="s">
         <v>470</v>
       </c>
@@ -33862,7 +33859,7 @@
       </c>
     </row>
     <row r="169" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="220" t="s">
+      <c r="A169" s="248" t="s">
         <v>32</v>
       </c>
       <c r="B169" s="217" t="s">
@@ -33876,7 +33873,7 @@
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="221"/>
+      <c r="A170" s="249"/>
       <c r="B170" s="218"/>
       <c r="C170" s="106" t="s">
         <v>264</v>
@@ -33886,7 +33883,7 @@
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="221"/>
+      <c r="A171" s="249"/>
       <c r="B171" s="218"/>
       <c r="C171" s="106" t="s">
         <v>263</v>
@@ -33896,7 +33893,7 @@
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="221"/>
+      <c r="A172" s="249"/>
       <c r="B172" s="218"/>
       <c r="C172" s="113" t="s">
         <v>271</v>
@@ -33906,7 +33903,7 @@
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="221"/>
+      <c r="A173" s="249"/>
       <c r="B173" s="218"/>
       <c r="C173" s="106" t="s">
         <v>276</v>
@@ -33916,7 +33913,7 @@
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="221"/>
+      <c r="A174" s="249"/>
       <c r="B174" s="218"/>
       <c r="C174" s="106" t="s">
         <v>277</v>
@@ -33926,7 +33923,7 @@
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="221"/>
+      <c r="A175" s="249"/>
       <c r="B175" s="218"/>
       <c r="C175" s="113" t="s">
         <v>282</v>
@@ -33936,7 +33933,7 @@
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="221"/>
+      <c r="A176" s="249"/>
       <c r="B176" s="218"/>
       <c r="C176" s="113" t="s">
         <v>296</v>
@@ -33946,7 +33943,7 @@
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="221"/>
+      <c r="A177" s="249"/>
       <c r="B177" s="218"/>
       <c r="C177" s="113" t="s">
         <v>283</v>
@@ -33956,7 +33953,7 @@
       </c>
     </row>
     <row r="178" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A178" s="221"/>
+      <c r="A178" s="249"/>
       <c r="B178" s="218"/>
       <c r="C178" s="123" t="s">
         <v>243</v>
@@ -33966,7 +33963,7 @@
       </c>
     </row>
     <row r="179" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A179" s="221"/>
+      <c r="A179" s="249"/>
       <c r="B179" s="218"/>
       <c r="C179" s="117" t="s">
         <v>305</v>
@@ -33976,7 +33973,7 @@
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="221"/>
+      <c r="A180" s="249"/>
       <c r="B180" s="218"/>
       <c r="C180" s="106" t="s">
         <v>306</v>
@@ -33986,7 +33983,7 @@
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="221"/>
+      <c r="A181" s="249"/>
       <c r="B181" s="218"/>
       <c r="C181" s="113" t="s">
         <v>307</v>
@@ -33996,7 +33993,7 @@
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="221"/>
+      <c r="A182" s="249"/>
       <c r="B182" s="218"/>
       <c r="C182" s="113" t="s">
         <v>309</v>
@@ -34006,7 +34003,7 @@
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="221"/>
+      <c r="A183" s="249"/>
       <c r="B183" s="218"/>
       <c r="C183" s="113" t="s">
         <v>262</v>
@@ -34016,7 +34013,7 @@
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="221"/>
+      <c r="A184" s="249"/>
       <c r="B184" s="218"/>
       <c r="C184" s="106" t="s">
         <v>312</v>
@@ -34026,7 +34023,7 @@
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="221"/>
+      <c r="A185" s="249"/>
       <c r="B185" s="218"/>
       <c r="C185" s="113" t="s">
         <v>277</v>
@@ -34036,7 +34033,7 @@
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="221"/>
+      <c r="A186" s="249"/>
       <c r="B186" s="218"/>
       <c r="C186" s="113" t="s">
         <v>313</v>
@@ -34046,7 +34043,7 @@
       </c>
     </row>
     <row r="187" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A187" s="221"/>
+      <c r="A187" s="249"/>
       <c r="B187" s="218"/>
       <c r="C187" s="106"/>
       <c r="D187" s="97" t="s">
@@ -34054,7 +34051,7 @@
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="221"/>
+      <c r="A188" s="249"/>
       <c r="B188" s="218"/>
       <c r="C188" s="113" t="s">
         <v>316</v>
@@ -34064,7 +34061,7 @@
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="221"/>
+      <c r="A189" s="249"/>
       <c r="B189" s="218"/>
       <c r="C189" s="113" t="s">
         <v>262</v>
@@ -34074,7 +34071,7 @@
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="221"/>
+      <c r="A190" s="249"/>
       <c r="B190" s="218"/>
       <c r="C190" s="113" t="s">
         <v>333</v>
@@ -34084,7 +34081,7 @@
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="221"/>
+      <c r="A191" s="249"/>
       <c r="B191" s="218"/>
       <c r="C191" s="113" t="s">
         <v>334</v>
@@ -34094,7 +34091,7 @@
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="221"/>
+      <c r="A192" s="249"/>
       <c r="B192" s="218"/>
       <c r="C192" s="113" t="s">
         <v>318</v>
@@ -34104,7 +34101,7 @@
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="221"/>
+      <c r="A193" s="249"/>
       <c r="B193" s="218"/>
       <c r="C193" s="113" t="s">
         <v>339</v>
@@ -34114,7 +34111,7 @@
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="221"/>
+      <c r="A194" s="249"/>
       <c r="B194" s="218"/>
       <c r="C194" s="113" t="s">
         <v>332</v>
@@ -34124,7 +34121,7 @@
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="221"/>
+      <c r="A195" s="249"/>
       <c r="B195" s="218"/>
       <c r="C195" s="113" t="s">
         <v>347</v>
@@ -34134,7 +34131,7 @@
       </c>
     </row>
     <row r="196" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A196" s="221"/>
+      <c r="A196" s="249"/>
       <c r="B196" s="218"/>
       <c r="C196" s="101" t="s">
         <v>350</v>
@@ -34144,7 +34141,7 @@
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="221"/>
+      <c r="A197" s="249"/>
       <c r="B197" s="218"/>
       <c r="C197" s="113" t="s">
         <v>351</v>
@@ -34154,7 +34151,7 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="221"/>
+      <c r="A198" s="249"/>
       <c r="B198" s="218"/>
       <c r="C198" s="113" t="s">
         <v>352</v>
@@ -34164,7 +34161,7 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="221"/>
+      <c r="A199" s="249"/>
       <c r="B199" s="218"/>
       <c r="C199" s="113" t="s">
         <v>358</v>
@@ -34174,7 +34171,7 @@
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="221"/>
+      <c r="A200" s="249"/>
       <c r="B200" s="218"/>
       <c r="C200" s="113" t="s">
         <v>360</v>
@@ -34184,7 +34181,7 @@
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="221"/>
+      <c r="A201" s="249"/>
       <c r="B201" s="218"/>
       <c r="C201" s="113" t="s">
         <v>366</v>
@@ -34194,7 +34191,7 @@
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="221"/>
+      <c r="A202" s="249"/>
       <c r="B202" s="218"/>
       <c r="C202" s="113" t="s">
         <v>358</v>
@@ -34204,7 +34201,7 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="221"/>
+      <c r="A203" s="249"/>
       <c r="B203" s="218"/>
       <c r="C203" s="118" t="s">
         <v>379</v>
@@ -34214,7 +34211,7 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="221"/>
+      <c r="A204" s="249"/>
       <c r="B204" s="218"/>
       <c r="C204" s="106" t="s">
         <v>383</v>
@@ -34224,7 +34221,7 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="221"/>
+      <c r="A205" s="249"/>
       <c r="B205" s="218"/>
       <c r="C205" s="106" t="s">
         <v>386</v>
@@ -34234,7 +34231,7 @@
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="221"/>
+      <c r="A206" s="249"/>
       <c r="B206" s="218"/>
       <c r="C206" s="106" t="s">
         <v>387</v>
@@ -34244,7 +34241,7 @@
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="221"/>
+      <c r="A207" s="249"/>
       <c r="B207" s="218"/>
       <c r="C207" s="106" t="s">
         <v>388</v>
@@ -34254,7 +34251,7 @@
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="221"/>
+      <c r="A208" s="249"/>
       <c r="B208" s="218"/>
       <c r="C208" s="106" t="s">
         <v>389</v>
@@ -34264,7 +34261,7 @@
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" s="221"/>
+      <c r="A209" s="249"/>
       <c r="B209" s="218"/>
       <c r="C209" s="106" t="s">
         <v>390</v>
@@ -34274,7 +34271,7 @@
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="221"/>
+      <c r="A210" s="249"/>
       <c r="B210" s="218"/>
       <c r="C210" s="106" t="s">
         <v>393</v>
@@ -34284,7 +34281,7 @@
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="221"/>
+      <c r="A211" s="249"/>
       <c r="B211" s="218"/>
       <c r="C211" s="106" t="s">
         <v>403</v>
@@ -34294,7 +34291,7 @@
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="221"/>
+      <c r="A212" s="249"/>
       <c r="B212" s="218"/>
       <c r="C212" s="106" t="s">
         <v>404</v>
@@ -34304,7 +34301,7 @@
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" s="221"/>
+      <c r="A213" s="249"/>
       <c r="B213" s="218"/>
       <c r="C213" s="106" t="s">
         <v>421</v>
@@ -34314,7 +34311,7 @@
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" s="221"/>
+      <c r="A214" s="249"/>
       <c r="B214" s="218"/>
       <c r="C214" s="106" t="s">
         <v>422</v>
@@ -34324,7 +34321,7 @@
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" s="221"/>
+      <c r="A215" s="249"/>
       <c r="B215" s="218"/>
       <c r="C215" s="106" t="s">
         <v>425</v>
@@ -34334,7 +34331,7 @@
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="221"/>
+      <c r="A216" s="249"/>
       <c r="B216" s="218"/>
       <c r="C216" s="58" t="s">
         <v>471</v>
@@ -34344,7 +34341,7 @@
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" s="221"/>
+      <c r="A217" s="249"/>
       <c r="B217" s="218"/>
       <c r="C217" s="58" t="s">
         <v>421</v>
@@ -34354,7 +34351,7 @@
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" s="221"/>
+      <c r="A218" s="249"/>
       <c r="B218" s="218"/>
       <c r="C218" s="58" t="s">
         <v>497</v>
@@ -34364,7 +34361,7 @@
       </c>
     </row>
     <row r="219" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A219" s="221"/>
+      <c r="A219" s="249"/>
       <c r="B219" s="218"/>
       <c r="C219" s="61" t="s">
         <v>522</v>
@@ -34374,7 +34371,7 @@
       </c>
     </row>
     <row r="220" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A220" s="222"/>
+      <c r="A220" s="250"/>
       <c r="B220" s="219"/>
       <c r="C220" s="61" t="s">
         <v>332</v>
@@ -34384,7 +34381,7 @@
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" s="220" t="s">
+      <c r="A221" s="248" t="s">
         <v>415</v>
       </c>
       <c r="B221" s="217" t="s">
@@ -34398,7 +34395,7 @@
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" s="221"/>
+      <c r="A222" s="249"/>
       <c r="B222" s="218"/>
       <c r="C222" s="118" t="s">
         <v>491</v>
@@ -34408,7 +34405,7 @@
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223" s="222"/>
+      <c r="A223" s="250"/>
       <c r="B223" s="219"/>
       <c r="C223" s="113" t="s">
         <v>524</v>
@@ -34454,7 +34451,7 @@
       <c r="D226" s="104"/>
     </row>
     <row r="227" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="227" t="s">
+      <c r="A227" s="234" t="s">
         <v>84</v>
       </c>
       <c r="B227" s="217" t="s">
@@ -34466,7 +34463,7 @@
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" s="239"/>
+      <c r="A228" s="235"/>
       <c r="B228" s="218"/>
       <c r="C228" s="107" t="s">
         <v>245</v>
@@ -34476,7 +34473,7 @@
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="239"/>
+      <c r="A229" s="235"/>
       <c r="B229" s="218"/>
       <c r="C229" s="107">
         <v>10.1</v>
@@ -34486,7 +34483,7 @@
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="239"/>
+      <c r="A230" s="235"/>
       <c r="B230" s="218"/>
       <c r="C230" s="107">
         <v>10.199999999999999</v>
@@ -34496,7 +34493,7 @@
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="239"/>
+      <c r="A231" s="235"/>
       <c r="B231" s="218"/>
       <c r="C231" s="98" t="s">
         <v>287</v>
@@ -34506,7 +34503,7 @@
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="239"/>
+      <c r="A232" s="235"/>
       <c r="B232" s="218"/>
       <c r="C232" s="98" t="s">
         <v>369</v>
@@ -34516,7 +34513,7 @@
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="239"/>
+      <c r="A233" s="235"/>
       <c r="B233" s="218"/>
       <c r="C233" s="98" t="s">
         <v>117</v>
@@ -34526,7 +34523,7 @@
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="239"/>
+      <c r="A234" s="235"/>
       <c r="B234" s="218"/>
       <c r="C234" s="98" t="s">
         <v>416</v>
@@ -34536,7 +34533,7 @@
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="239"/>
+      <c r="A235" s="235"/>
       <c r="B235" s="218"/>
       <c r="C235" s="98" t="s">
         <v>17</v>
@@ -34546,7 +34543,7 @@
       </c>
     </row>
     <row r="236" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A236" s="239"/>
+      <c r="A236" s="235"/>
       <c r="B236" s="218"/>
       <c r="C236" s="98" t="s">
         <v>496</v>
@@ -34556,7 +34553,7 @@
       </c>
     </row>
     <row r="237" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A237" s="228"/>
+      <c r="A237" s="236"/>
       <c r="B237" s="219"/>
       <c r="C237" s="98" t="s">
         <v>496</v>
@@ -34566,7 +34563,7 @@
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" s="227" t="s">
+      <c r="A238" s="234" t="s">
         <v>246</v>
       </c>
       <c r="B238" s="217" t="s">
@@ -34578,7 +34575,7 @@
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" s="239"/>
+      <c r="A239" s="235"/>
       <c r="B239" s="218"/>
       <c r="C239" s="126" t="s">
         <v>427</v>
@@ -34610,7 +34607,7 @@
       <c r="D241" s="127"/>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="227" t="s">
+      <c r="A242" s="234" t="s">
         <v>58</v>
       </c>
       <c r="B242" s="217" t="s">
@@ -34624,7 +34621,7 @@
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="239"/>
+      <c r="A243" s="235"/>
       <c r="B243" s="218"/>
       <c r="C243" s="128" t="s">
         <v>259</v>
@@ -34634,7 +34631,7 @@
       </c>
     </row>
     <row r="244" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A244" s="228"/>
+      <c r="A244" s="236"/>
       <c r="B244" s="219"/>
       <c r="C244" s="106"/>
       <c r="D244" s="106" t="s">
@@ -34642,7 +34639,7 @@
       </c>
     </row>
     <row r="245" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A245" s="237" t="s">
+      <c r="A245" s="239" t="s">
         <v>59</v>
       </c>
       <c r="B245" s="217" t="s">
@@ -34656,7 +34653,7 @@
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A246" s="238"/>
+      <c r="A246" s="240"/>
       <c r="B246" s="219"/>
       <c r="C246" s="119"/>
       <c r="D246" s="106" t="s">
@@ -34664,7 +34661,7 @@
       </c>
     </row>
     <row r="247" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A247" s="237" t="s">
+      <c r="A247" s="239" t="s">
         <v>285</v>
       </c>
       <c r="B247" s="217" t="s">
@@ -34676,7 +34673,7 @@
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A248" s="238"/>
+      <c r="A248" s="240"/>
       <c r="B248" s="219"/>
       <c r="C248" s="106"/>
       <c r="D248" s="106" t="s">
@@ -34684,7 +34681,7 @@
       </c>
     </row>
     <row r="249" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A249" s="237" t="s">
+      <c r="A249" s="239" t="s">
         <v>60</v>
       </c>
       <c r="B249" s="217" t="s">
@@ -34698,7 +34695,7 @@
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A250" s="238"/>
+      <c r="A250" s="240"/>
       <c r="B250" s="219"/>
       <c r="C250" s="106"/>
       <c r="D250" s="106" t="s">
@@ -34757,6 +34754,56 @@
     </row>
   </sheetData>
   <mergeCells count="66">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B221:B223"/>
+    <mergeCell ref="A221:A223"/>
+    <mergeCell ref="B169:B220"/>
+    <mergeCell ref="A169:A220"/>
+    <mergeCell ref="A19:A28"/>
+    <mergeCell ref="B19:B28"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="A73:A88"/>
+    <mergeCell ref="B73:B88"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="B55:B60"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A55:A60"/>
+    <mergeCell ref="A249:A250"/>
+    <mergeCell ref="B249:B250"/>
+    <mergeCell ref="A245:A246"/>
+    <mergeCell ref="B245:B246"/>
+    <mergeCell ref="A247:A248"/>
+    <mergeCell ref="B247:B248"/>
+    <mergeCell ref="A242:A244"/>
+    <mergeCell ref="B242:B244"/>
+    <mergeCell ref="A238:A239"/>
+    <mergeCell ref="B238:B239"/>
+    <mergeCell ref="B161:B167"/>
+    <mergeCell ref="A147:A151"/>
+    <mergeCell ref="B147:B151"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="A161:A167"/>
+    <mergeCell ref="A227:A237"/>
+    <mergeCell ref="B227:B237"/>
+    <mergeCell ref="A67:A71"/>
+    <mergeCell ref="B130:B143"/>
+    <mergeCell ref="A154:A160"/>
+    <mergeCell ref="B154:B160"/>
+    <mergeCell ref="A130:A143"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="D163:D166"/>
@@ -34773,56 +34820,6 @@
     <mergeCell ref="A144:A146"/>
     <mergeCell ref="B144:B146"/>
     <mergeCell ref="A61:A63"/>
-    <mergeCell ref="A147:A151"/>
-    <mergeCell ref="B147:B151"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="A161:A167"/>
-    <mergeCell ref="A227:A237"/>
-    <mergeCell ref="B227:B237"/>
-    <mergeCell ref="A67:A71"/>
-    <mergeCell ref="B130:B143"/>
-    <mergeCell ref="A154:A160"/>
-    <mergeCell ref="B154:B160"/>
-    <mergeCell ref="A130:A143"/>
-    <mergeCell ref="A242:A244"/>
-    <mergeCell ref="B242:B244"/>
-    <mergeCell ref="A238:A239"/>
-    <mergeCell ref="B238:B239"/>
-    <mergeCell ref="B161:B167"/>
-    <mergeCell ref="A249:A250"/>
-    <mergeCell ref="B249:B250"/>
-    <mergeCell ref="A245:A246"/>
-    <mergeCell ref="B245:B246"/>
-    <mergeCell ref="A247:A248"/>
-    <mergeCell ref="B247:B248"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="A73:A88"/>
-    <mergeCell ref="B73:B88"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="B55:B60"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A55:A60"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B221:B223"/>
-    <mergeCell ref="A221:A223"/>
-    <mergeCell ref="B169:B220"/>
-    <mergeCell ref="A169:A220"/>
-    <mergeCell ref="A19:A28"/>
-    <mergeCell ref="B19:B28"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A15:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -34831,10 +34828,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DBC65A-63D2-46B3-B8B5-A94A70B9EDFE}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34860,7 +34857,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="242" t="s">
+      <c r="A2" s="220" t="s">
         <v>236</v>
       </c>
       <c r="B2" s="217" t="s">
@@ -34874,7 +34871,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="243"/>
+      <c r="A3" s="221"/>
       <c r="B3" s="218"/>
       <c r="C3" s="58" t="s">
         <v>540</v>
@@ -34884,7 +34881,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="243"/>
+      <c r="A4" s="221"/>
       <c r="B4" s="218"/>
       <c r="C4" s="58" t="s">
         <v>541</v>
@@ -34894,7 +34891,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="243"/>
+      <c r="A5" s="221"/>
       <c r="B5" s="218"/>
       <c r="C5" s="58" t="s">
         <v>542</v>
@@ -34904,7 +34901,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="243"/>
+      <c r="A6" s="221"/>
       <c r="B6" s="218"/>
       <c r="C6" s="58" t="s">
         <v>543</v>
@@ -34914,7 +34911,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="243"/>
+      <c r="A7" s="221"/>
       <c r="B7" s="218"/>
       <c r="C7" s="58" t="s">
         <v>537</v>
@@ -34924,7 +34921,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="243"/>
+      <c r="A8" s="221"/>
       <c r="B8" s="218"/>
       <c r="C8" s="58" t="s">
         <v>544</v>
@@ -34934,7 +34931,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="243"/>
+      <c r="A9" s="221"/>
       <c r="B9" s="218"/>
       <c r="C9" s="58" t="s">
         <v>545</v>
@@ -34944,7 +34941,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="243"/>
+      <c r="A10" s="221"/>
       <c r="B10" s="218"/>
       <c r="C10" s="58" t="s">
         <v>546</v>
@@ -34954,7 +34951,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="243"/>
+      <c r="A11" s="221"/>
       <c r="B11" s="218"/>
       <c r="C11" s="58" t="s">
         <v>547</v>
@@ -34964,7 +34961,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="243"/>
+      <c r="A12" s="221"/>
       <c r="B12" s="218"/>
       <c r="C12" s="58" t="s">
         <v>548</v>
@@ -34974,7 +34971,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="243"/>
+      <c r="A13" s="221"/>
       <c r="B13" s="218"/>
       <c r="C13" s="58" t="s">
         <v>539</v>
@@ -34984,7 +34981,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="243"/>
+      <c r="A14" s="221"/>
       <c r="B14" s="218"/>
       <c r="C14" s="58" t="s">
         <v>538</v>
@@ -34994,7 +34991,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="243"/>
+      <c r="A15" s="221"/>
       <c r="B15" s="218"/>
       <c r="C15" s="106" t="s">
         <v>552</v>
@@ -35004,30 +35001,30 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="243"/>
+      <c r="A16" s="221"/>
       <c r="B16" s="218"/>
       <c r="C16" s="58" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D16" s="119" t="s">
         <v>549</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="243"/>
+      <c r="A17" s="221"/>
       <c r="B17" s="218"/>
       <c r="C17" s="119" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D17" s="119" t="s">
         <v>549</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="243"/>
+      <c r="A18" s="221"/>
       <c r="B18" s="218"/>
       <c r="C18" s="58" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D18" s="119" t="s">
         <v>549</v>
@@ -35037,7 +35034,7 @@
       <c r="A19" s="251"/>
       <c r="B19" s="219"/>
       <c r="C19" s="119" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D19" s="119" t="s">
         <v>549</v>
@@ -35047,7 +35044,7 @@
       <c r="A20" s="252" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="231" t="s">
+      <c r="B20" s="238" t="s">
         <v>439</v>
       </c>
       <c r="C20" s="106" t="s">
@@ -35059,7 +35056,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="252"/>
-      <c r="B21" s="231"/>
+      <c r="B21" s="238"/>
       <c r="C21" s="58" t="s">
         <v>540</v>
       </c>
@@ -35069,7 +35066,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="252"/>
-      <c r="B22" s="231"/>
+      <c r="B22" s="238"/>
       <c r="C22" s="58" t="s">
         <v>541</v>
       </c>
@@ -35079,7 +35076,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="252"/>
-      <c r="B23" s="231"/>
+      <c r="B23" s="238"/>
       <c r="C23" s="58" t="s">
         <v>542</v>
       </c>
@@ -35089,7 +35086,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="252"/>
-      <c r="B24" s="231"/>
+      <c r="B24" s="238"/>
       <c r="C24" s="58" t="s">
         <v>543</v>
       </c>
@@ -35099,7 +35096,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="252"/>
-      <c r="B25" s="231"/>
+      <c r="B25" s="238"/>
       <c r="C25" s="58" t="s">
         <v>537</v>
       </c>
@@ -35109,7 +35106,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="252"/>
-      <c r="B26" s="231"/>
+      <c r="B26" s="238"/>
       <c r="C26" s="58" t="s">
         <v>544</v>
       </c>
@@ -35119,7 +35116,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="252"/>
-      <c r="B27" s="231"/>
+      <c r="B27" s="238"/>
       <c r="C27" s="58" t="s">
         <v>545</v>
       </c>
@@ -35129,7 +35126,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="252"/>
-      <c r="B28" s="231"/>
+      <c r="B28" s="238"/>
       <c r="C28" s="58" t="s">
         <v>546</v>
       </c>
@@ -35139,7 +35136,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="252"/>
-      <c r="B29" s="231"/>
+      <c r="B29" s="238"/>
       <c r="C29" s="58" t="s">
         <v>547</v>
       </c>
@@ -35149,7 +35146,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="252"/>
-      <c r="B30" s="231"/>
+      <c r="B30" s="238"/>
       <c r="C30" s="58" t="s">
         <v>548</v>
       </c>
@@ -35159,7 +35156,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="252"/>
-      <c r="B31" s="231"/>
+      <c r="B31" s="238"/>
       <c r="C31" s="58" t="s">
         <v>539</v>
       </c>
@@ -35169,7 +35166,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="252"/>
-      <c r="B32" s="231"/>
+      <c r="B32" s="238"/>
       <c r="C32" s="58" t="s">
         <v>538</v>
       </c>
@@ -35179,7 +35176,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="252"/>
-      <c r="B33" s="231"/>
+      <c r="B33" s="238"/>
       <c r="C33" s="106" t="s">
         <v>552</v>
       </c>
@@ -35189,9 +35186,9 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="252"/>
-      <c r="B34" s="231"/>
+      <c r="B34" s="238"/>
       <c r="C34" s="58" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D34" s="119" t="s">
         <v>549</v>
@@ -35199,9 +35196,9 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="252"/>
-      <c r="B35" s="231"/>
+      <c r="B35" s="238"/>
       <c r="C35" s="119" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D35" s="119" t="s">
         <v>549</v>
@@ -35209,9 +35206,9 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="252"/>
-      <c r="B36" s="231"/>
+      <c r="B36" s="238"/>
       <c r="C36" s="58" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D36" s="119" t="s">
         <v>549</v>
@@ -35219,9 +35216,9 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="252"/>
-      <c r="B37" s="231"/>
+      <c r="B37" s="238"/>
       <c r="C37" s="119" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D37" s="119" t="s">
         <v>549</v>
@@ -35245,20 +35242,20 @@
       <c r="A39" s="218"/>
       <c r="B39" s="218"/>
       <c r="C39" s="106" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D39" s="159" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="253"/>
       <c r="B40" s="253"/>
       <c r="C40" s="106" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D40" s="159" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -35268,9 +35265,7 @@
       <c r="B41" s="112" t="s">
         <v>439</v>
       </c>
-      <c r="C41" s="156" t="s">
-        <v>22</v>
-      </c>
+      <c r="C41" s="156"/>
       <c r="D41" s="155" t="s">
         <v>30</v>
       </c>
@@ -35293,20 +35288,20 @@
       <c r="A43" s="218"/>
       <c r="B43" s="218"/>
       <c r="C43" s="109" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D43" s="159" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="219"/>
       <c r="B44" s="219"/>
       <c r="C44" s="109" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D44" s="159" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -35347,7 +35342,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="126" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B48" s="162" t="s">
         <v>439</v>
@@ -35359,7 +35354,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="126" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B49" s="162" t="s">
         <v>439</v>
@@ -35370,26 +35365,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="126" t="s">
-        <v>558</v>
-      </c>
-      <c r="B50" s="161" t="s">
+      <c r="A50" s="131" t="s">
+        <v>570</v>
+      </c>
+      <c r="B50" s="163" t="s">
         <v>439</v>
       </c>
       <c r="C50" s="109"/>
-      <c r="D50" s="160" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="131" t="s">
-        <v>536</v>
-      </c>
-      <c r="B51" s="163" t="s">
-        <v>439</v>
-      </c>
-      <c r="C51" s="109"/>
-      <c r="D51" s="159" t="s">
+      <c r="D50" s="159" t="s">
         <v>557</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data item documentation updates pkalse
</commit_message>
<xml_diff>
--- a/PIT4/Schema Publication Changelog.xlsx
+++ b/PIT4/Schema Publication Changelog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ERR Rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctrowell\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EA86D20-74BC-405E-97DC-6D124BEC78BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D0422A-8779-4DA4-801D-853D61E5D42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v0.10" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="723">
   <si>
     <t>Document</t>
   </si>
@@ -4051,6 +4051,21 @@
   </si>
   <si>
     <t>Updated Travel &amp; Subsistence site based employees validation rule to (181.68 x 48) which would be: 8720.64</t>
+  </si>
+  <si>
+    <t>ERR - Enhanced Reporting Notification (ERN) Request Data Items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note on case sensitivity added </t>
+  </si>
+  <si>
+    <t>ERR - Enhanced Reporting Submission Request Data Items</t>
+  </si>
+  <si>
+    <t>PAYE Modernisation - Payroll Submission Request Data Items</t>
+  </si>
+  <si>
+    <t>PAYE Modernisation - RPN Data Items</t>
   </si>
 </sst>
 </file>
@@ -5038,10 +5053,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
@@ -5052,6 +5064,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -5095,8 +5110,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -5119,66 +5164,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -5200,6 +5185,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5218,6 +5233,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -5226,6 +5250,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5248,44 +5299,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5626,8 +5641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6178,7 +6193,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6188,7 +6203,7 @@
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -6298,10 +6313,10 @@
       <c r="D6" s="40"/>
     </row>
     <row r="7" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="169" t="s">
+      <c r="A7" s="154" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="168" t="s">
+      <c r="B7" s="155" t="s">
         <v>81</v>
       </c>
       <c r="C7" s="39" t="s">
@@ -6312,8 +6327,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="169"/>
-      <c r="B8" s="168"/>
+      <c r="A8" s="154"/>
+      <c r="B8" s="155"/>
       <c r="C8" s="34" t="s">
         <v>84</v>
       </c>
@@ -6322,8 +6337,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="169"/>
-      <c r="B9" s="168"/>
+      <c r="A9" s="154"/>
+      <c r="B9" s="155"/>
       <c r="C9" s="34" t="s">
         <v>86</v>
       </c>
@@ -6332,8 +6347,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="169"/>
-      <c r="B10" s="168"/>
+      <c r="A10" s="154"/>
+      <c r="B10" s="155"/>
       <c r="C10" s="34" t="s">
         <v>18</v>
       </c>
@@ -6342,8 +6357,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="169"/>
-      <c r="B11" s="168"/>
+      <c r="A11" s="154"/>
+      <c r="B11" s="155"/>
       <c r="C11" s="34" t="s">
         <v>89</v>
       </c>
@@ -6352,8 +6367,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="169"/>
-      <c r="B12" s="168"/>
+      <c r="A12" s="154"/>
+      <c r="B12" s="155"/>
       <c r="C12" s="34" t="s">
         <v>91</v>
       </c>
@@ -6362,10 +6377,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="171" t="s">
+      <c r="A13" s="157" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="168" t="s">
+      <c r="B13" s="155" t="s">
         <v>81</v>
       </c>
       <c r="C13" s="34" t="s">
@@ -6376,8 +6391,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="171"/>
-      <c r="B14" s="168"/>
+      <c r="A14" s="157"/>
+      <c r="B14" s="155"/>
       <c r="C14" s="34" t="s">
         <v>96</v>
       </c>
@@ -6386,8 +6401,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="171"/>
-      <c r="B15" s="168"/>
+      <c r="A15" s="157"/>
+      <c r="B15" s="155"/>
       <c r="C15" s="39" t="s">
         <v>98</v>
       </c>
@@ -6396,10 +6411,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="158" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="163" t="s">
+      <c r="B16" s="159" t="s">
         <v>81</v>
       </c>
       <c r="C16" s="54" t="s">
@@ -6410,8 +6425,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="154"/>
-      <c r="B17" s="163"/>
+      <c r="A17" s="158"/>
+      <c r="B17" s="159"/>
       <c r="C17" s="53" t="s">
         <v>102</v>
       </c>
@@ -6420,8 +6435,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="154"/>
-      <c r="B18" s="163"/>
+      <c r="A18" s="158"/>
+      <c r="B18" s="159"/>
       <c r="C18" s="53" t="s">
         <v>89</v>
       </c>
@@ -6430,8 +6445,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="154"/>
-      <c r="B19" s="163"/>
+      <c r="A19" s="158"/>
+      <c r="B19" s="159"/>
       <c r="C19" s="53" t="s">
         <v>105</v>
       </c>
@@ -6440,8 +6455,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="154"/>
-      <c r="B20" s="163"/>
+      <c r="A20" s="158"/>
+      <c r="B20" s="159"/>
       <c r="C20" s="53" t="s">
         <v>107</v>
       </c>
@@ -6450,8 +6465,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="154"/>
-      <c r="B21" s="163"/>
+      <c r="A21" s="158"/>
+      <c r="B21" s="159"/>
       <c r="C21" s="53" t="s">
         <v>109</v>
       </c>
@@ -6460,8 +6475,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="154"/>
-      <c r="B22" s="163"/>
+      <c r="A22" s="158"/>
+      <c r="B22" s="159"/>
       <c r="C22" s="53" t="s">
         <v>111</v>
       </c>
@@ -6470,8 +6485,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="154"/>
-      <c r="B23" s="163"/>
+      <c r="A23" s="158"/>
+      <c r="B23" s="159"/>
       <c r="C23" s="61" t="s">
         <v>113</v>
       </c>
@@ -6480,26 +6495,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="154"/>
-      <c r="B24" s="163"/>
-      <c r="C24" s="154" t="s">
+      <c r="A24" s="158"/>
+      <c r="B24" s="159"/>
+      <c r="C24" s="158" t="s">
         <v>115</v>
       </c>
-      <c r="D24" s="155" t="s">
+      <c r="D24" s="165" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="154"/>
-      <c r="B25" s="163"/>
-      <c r="C25" s="154"/>
-      <c r="D25" s="155"/>
+      <c r="A25" s="158"/>
+      <c r="B25" s="159"/>
+      <c r="C25" s="158"/>
+      <c r="D25" s="165"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="169" t="s">
+      <c r="A26" s="154" t="s">
         <v>117</v>
       </c>
-      <c r="B26" s="168" t="s">
+      <c r="B26" s="155" t="s">
         <v>81</v>
       </c>
       <c r="C26" s="34" t="s">
@@ -6510,8 +6525,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="169"/>
-      <c r="B27" s="168"/>
+      <c r="A27" s="154"/>
+      <c r="B27" s="155"/>
       <c r="C27" s="34"/>
       <c r="D27" s="37" t="s">
         <v>120</v>
@@ -6538,28 +6553,28 @@
       <c r="D29" s="35"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="170" t="s">
+      <c r="A30" s="156" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="168" t="s">
+      <c r="B30" s="155" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="154" t="s">
+      <c r="C30" s="158" t="s">
         <v>123</v>
       </c>
-      <c r="D30" s="158" t="s">
+      <c r="D30" s="168" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="170"/>
-      <c r="B31" s="168"/>
-      <c r="C31" s="154"/>
-      <c r="D31" s="158"/>
+      <c r="A31" s="156"/>
+      <c r="B31" s="155"/>
+      <c r="C31" s="158"/>
+      <c r="D31" s="168"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="170"/>
-      <c r="B32" s="168"/>
+      <c r="A32" s="156"/>
+      <c r="B32" s="155"/>
       <c r="C32" s="53" t="s">
         <v>125</v>
       </c>
@@ -6568,8 +6583,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="170"/>
-      <c r="B33" s="168"/>
+      <c r="A33" s="156"/>
+      <c r="B33" s="155"/>
       <c r="C33" s="53" t="s">
         <v>127</v>
       </c>
@@ -6578,8 +6593,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="170"/>
-      <c r="B34" s="168"/>
+      <c r="A34" s="156"/>
+      <c r="B34" s="155"/>
       <c r="C34" s="62" t="s">
         <v>129</v>
       </c>
@@ -6588,8 +6603,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="170"/>
-      <c r="B35" s="168"/>
+      <c r="A35" s="156"/>
+      <c r="B35" s="155"/>
       <c r="C35" s="53" t="s">
         <v>111</v>
       </c>
@@ -6598,8 +6613,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="170"/>
-      <c r="B36" s="168"/>
+      <c r="A36" s="156"/>
+      <c r="B36" s="155"/>
       <c r="C36" s="62" t="s">
         <v>113</v>
       </c>
@@ -6608,26 +6623,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="170"/>
-      <c r="B37" s="168"/>
-      <c r="C37" s="159" t="s">
+      <c r="A37" s="156"/>
+      <c r="B37" s="155"/>
+      <c r="C37" s="169" t="s">
         <v>115</v>
       </c>
-      <c r="D37" s="161" t="s">
+      <c r="D37" s="171" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="170"/>
-      <c r="B38" s="168"/>
-      <c r="C38" s="160"/>
-      <c r="D38" s="161"/>
+      <c r="A38" s="156"/>
+      <c r="B38" s="155"/>
+      <c r="C38" s="170"/>
+      <c r="D38" s="171"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="169" t="s">
+      <c r="A39" s="154" t="s">
         <v>134</v>
       </c>
-      <c r="B39" s="168" t="s">
+      <c r="B39" s="155" t="s">
         <v>81</v>
       </c>
       <c r="C39" s="34" t="s">
@@ -6638,8 +6653,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="169"/>
-      <c r="B40" s="168"/>
+      <c r="A40" s="154"/>
+      <c r="B40" s="155"/>
       <c r="C40" s="34"/>
       <c r="D40" s="45" t="s">
         <v>136</v>
@@ -6666,10 +6681,10 @@
       <c r="D42" s="40"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="170" t="s">
+      <c r="A43" s="156" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="168" t="s">
+      <c r="B43" s="155" t="s">
         <v>81</v>
       </c>
       <c r="C43" s="34"/>
@@ -6678,8 +6693,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="170"/>
-      <c r="B44" s="168"/>
+      <c r="A44" s="156"/>
+      <c r="B44" s="155"/>
       <c r="C44" s="34" t="s">
         <v>118</v>
       </c>
@@ -6688,10 +6703,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="165" t="s">
+      <c r="A45" s="162" t="s">
         <v>139</v>
       </c>
-      <c r="B45" s="168" t="s">
+      <c r="B45" s="155" t="s">
         <v>81</v>
       </c>
       <c r="C45" s="34"/>
@@ -6700,8 +6715,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="166"/>
-      <c r="B46" s="168"/>
+      <c r="A46" s="163"/>
+      <c r="B46" s="155"/>
       <c r="C46" s="34" t="s">
         <v>141</v>
       </c>
@@ -6710,8 +6725,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="166"/>
-      <c r="B47" s="168"/>
+      <c r="A47" s="163"/>
+      <c r="B47" s="155"/>
       <c r="C47" s="34" t="s">
         <v>143</v>
       </c>
@@ -6720,8 +6735,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="167"/>
-      <c r="B48" s="168"/>
+      <c r="A48" s="164"/>
+      <c r="B48" s="155"/>
       <c r="C48" s="34" t="s">
         <v>118</v>
       </c>
@@ -6730,10 +6745,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="163" t="s">
+      <c r="A49" s="159" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="163" t="s">
+      <c r="B49" s="159" t="s">
         <v>81</v>
       </c>
       <c r="C49" s="53"/>
@@ -10837,8 +10852,8 @@
       <c r="XFC49" s="38"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="163"/>
-      <c r="B50" s="163"/>
+      <c r="A50" s="159"/>
+      <c r="B50" s="159"/>
       <c r="C50" s="54" t="s">
         <v>146</v>
       </c>
@@ -14942,8 +14957,8 @@
       <c r="XFC50" s="38"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="163"/>
-      <c r="B51" s="163"/>
+      <c r="A51" s="159"/>
+      <c r="B51" s="159"/>
       <c r="C51" s="34" t="s">
         <v>148</v>
       </c>
@@ -19047,8 +19062,8 @@
       <c r="XFC51" s="38"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="163"/>
-      <c r="B52" s="163"/>
+      <c r="A52" s="159"/>
+      <c r="B52" s="159"/>
       <c r="C52" s="53" t="s">
         <v>150</v>
       </c>
@@ -23152,12 +23167,12 @@
       <c r="XFC52" s="38"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="163"/>
-      <c r="B53" s="163"/>
-      <c r="C53" s="157" t="s">
+      <c r="A53" s="159"/>
+      <c r="B53" s="159"/>
+      <c r="C53" s="167" t="s">
         <v>152</v>
       </c>
-      <c r="D53" s="158" t="s">
+      <c r="D53" s="168" t="s">
         <v>153</v>
       </c>
       <c r="G53" s="38"/>
@@ -27257,10 +27272,10 @@
       <c r="XFC53" s="38"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="163"/>
-      <c r="B54" s="163"/>
-      <c r="C54" s="157"/>
-      <c r="D54" s="158"/>
+      <c r="A54" s="159"/>
+      <c r="B54" s="159"/>
+      <c r="C54" s="167"/>
+      <c r="D54" s="168"/>
       <c r="G54" s="38"/>
       <c r="K54" s="38"/>
       <c r="O54" s="38"/>
@@ -31378,10 +31393,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="162" t="s">
+      <c r="A57" s="160" t="s">
         <v>156</v>
       </c>
-      <c r="B57" s="163" t="s">
+      <c r="B57" s="159" t="s">
         <v>81</v>
       </c>
       <c r="C57" s="53" t="s">
@@ -31392,8 +31407,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="162"/>
-      <c r="B58" s="163"/>
+      <c r="A58" s="160"/>
+      <c r="B58" s="159"/>
       <c r="C58" s="56" t="s">
         <v>159</v>
       </c>
@@ -31402,8 +31417,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="162"/>
-      <c r="B59" s="163"/>
+      <c r="A59" s="160"/>
+      <c r="B59" s="159"/>
       <c r="C59" s="53" t="s">
         <v>161</v>
       </c>
@@ -31412,8 +31427,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="162"/>
-      <c r="B60" s="163"/>
+      <c r="A60" s="160"/>
+      <c r="B60" s="159"/>
       <c r="C60" s="53" t="s">
         <v>163</v>
       </c>
@@ -31422,8 +31437,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="162"/>
-      <c r="B61" s="163"/>
+      <c r="A61" s="160"/>
+      <c r="B61" s="159"/>
       <c r="C61" s="34" t="s">
         <v>118</v>
       </c>
@@ -31432,8 +31447,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="162"/>
-      <c r="B62" s="163"/>
+      <c r="A62" s="160"/>
+      <c r="B62" s="159"/>
       <c r="C62" s="53" t="s">
         <v>166</v>
       </c>
@@ -31442,8 +31457,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="162"/>
-      <c r="B63" s="163"/>
+      <c r="A63" s="160"/>
+      <c r="B63" s="159"/>
       <c r="C63" s="53" t="s">
         <v>166</v>
       </c>
@@ -31452,16 +31467,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="162"/>
-      <c r="B64" s="163"/>
+      <c r="A64" s="160"/>
+      <c r="B64" s="159"/>
       <c r="C64" s="53"/>
       <c r="D64" s="43" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="162"/>
-      <c r="B65" s="163"/>
+      <c r="A65" s="160"/>
+      <c r="B65" s="159"/>
       <c r="C65" s="53" t="s">
         <v>169</v>
       </c>
@@ -31470,16 +31485,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="162"/>
-      <c r="B66" s="163"/>
+      <c r="A66" s="160"/>
+      <c r="B66" s="159"/>
       <c r="C66" s="53"/>
       <c r="D66" s="42" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="162"/>
-      <c r="B67" s="163"/>
+      <c r="A67" s="160"/>
+      <c r="B67" s="159"/>
       <c r="C67" s="53" t="s">
         <v>172</v>
       </c>
@@ -31488,8 +31503,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="162"/>
-      <c r="B68" s="163"/>
+      <c r="A68" s="160"/>
+      <c r="B68" s="159"/>
       <c r="C68" s="53" t="s">
         <v>174</v>
       </c>
@@ -31498,8 +31513,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="162"/>
-      <c r="B69" s="163"/>
+      <c r="A69" s="160"/>
+      <c r="B69" s="159"/>
       <c r="C69" s="56" t="s">
         <v>176</v>
       </c>
@@ -31508,8 +31523,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="162"/>
-      <c r="B70" s="163"/>
+      <c r="A70" s="160"/>
+      <c r="B70" s="159"/>
       <c r="C70" s="56" t="s">
         <v>178</v>
       </c>
@@ -31518,8 +31533,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="162"/>
-      <c r="B71" s="163"/>
+      <c r="A71" s="160"/>
+      <c r="B71" s="159"/>
       <c r="C71" s="53" t="s">
         <v>179</v>
       </c>
@@ -31528,8 +31543,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="162"/>
-      <c r="B72" s="163"/>
+      <c r="A72" s="160"/>
+      <c r="B72" s="159"/>
       <c r="C72" s="53" t="s">
         <v>181</v>
       </c>
@@ -31538,16 +31553,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="162"/>
-      <c r="B73" s="163"/>
+      <c r="A73" s="160"/>
+      <c r="B73" s="159"/>
       <c r="C73" s="53"/>
       <c r="D73" s="45" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="162"/>
-      <c r="B74" s="163"/>
+      <c r="A74" s="160"/>
+      <c r="B74" s="159"/>
       <c r="C74" s="53" t="s">
         <v>182</v>
       </c>
@@ -31556,18 +31571,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="162"/>
-      <c r="B75" s="163"/>
-      <c r="C75" s="156"/>
-      <c r="D75" s="164" t="s">
+      <c r="A75" s="160"/>
+      <c r="B75" s="159"/>
+      <c r="C75" s="166"/>
+      <c r="D75" s="161" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="162"/>
-      <c r="B76" s="163"/>
-      <c r="C76" s="156"/>
-      <c r="D76" s="164"/>
+      <c r="A76" s="160"/>
+      <c r="B76" s="159"/>
+      <c r="C76" s="166"/>
+      <c r="D76" s="161"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="35" t="s">
@@ -31591,8 +31606,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -31601,13 +31616,29 @@
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -31622,22 +31653,6 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -31691,10 +31706,10 @@
       <c r="D3" s="40"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="169" t="s">
+      <c r="A4" s="154" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="168" t="s">
+      <c r="B4" s="155" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="67" t="s">
@@ -31705,133 +31720,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="169"/>
-      <c r="B5" s="168"/>
-      <c r="C5" s="179" t="s">
+      <c r="A5" s="154"/>
+      <c r="B5" s="155"/>
+      <c r="C5" s="181" t="s">
         <v>188</v>
       </c>
-      <c r="D5" s="178" t="s">
+      <c r="D5" s="180" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="169"/>
-      <c r="B6" s="168"/>
-      <c r="C6" s="179"/>
-      <c r="D6" s="178"/>
+      <c r="A6" s="154"/>
+      <c r="B6" s="155"/>
+      <c r="C6" s="181"/>
+      <c r="D6" s="180"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="169"/>
-      <c r="B7" s="168"/>
+      <c r="A7" s="154"/>
+      <c r="B7" s="155"/>
       <c r="C7" s="53"/>
       <c r="D7" s="53"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="169"/>
-      <c r="B8" s="168"/>
+      <c r="A8" s="154"/>
+      <c r="B8" s="155"/>
       <c r="C8" s="53"/>
       <c r="D8" s="53"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="169"/>
-      <c r="B9" s="168"/>
+      <c r="A9" s="154"/>
+      <c r="B9" s="155"/>
       <c r="C9" s="66"/>
       <c r="D9" s="45"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="171" t="s">
+      <c r="A10" s="157" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="168" t="s">
+      <c r="B10" s="155" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="181"/>
-      <c r="D10" s="178" t="s">
+      <c r="C10" s="179"/>
+      <c r="D10" s="180" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="171"/>
-      <c r="B11" s="168"/>
-      <c r="C11" s="181"/>
-      <c r="D11" s="178"/>
+      <c r="A11" s="157"/>
+      <c r="B11" s="155"/>
+      <c r="C11" s="179"/>
+      <c r="D11" s="180"/>
     </row>
     <row r="12" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="171"/>
-      <c r="B12" s="168"/>
-      <c r="C12" s="181"/>
-      <c r="D12" s="178"/>
+      <c r="A12" s="157"/>
+      <c r="B12" s="155"/>
+      <c r="C12" s="179"/>
+      <c r="D12" s="180"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="154" t="s">
+      <c r="A13" s="158" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="163" t="s">
+      <c r="B13" s="159" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="180"/>
-      <c r="D13" s="178" t="s">
+      <c r="C13" s="182"/>
+      <c r="D13" s="180" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="154"/>
-      <c r="B14" s="163"/>
-      <c r="C14" s="180"/>
-      <c r="D14" s="178"/>
+      <c r="A14" s="158"/>
+      <c r="B14" s="159"/>
+      <c r="C14" s="182"/>
+      <c r="D14" s="180"/>
     </row>
     <row r="15" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="154"/>
-      <c r="B15" s="163"/>
-      <c r="C15" s="180"/>
+      <c r="A15" s="158"/>
+      <c r="B15" s="159"/>
+      <c r="C15" s="182"/>
       <c r="D15" s="45"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="154"/>
-      <c r="B16" s="163"/>
-      <c r="C16" s="180"/>
+      <c r="A16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="182"/>
       <c r="D16" s="45"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="154"/>
-      <c r="B17" s="163"/>
-      <c r="C17" s="180"/>
+      <c r="A17" s="158"/>
+      <c r="B17" s="159"/>
+      <c r="C17" s="182"/>
       <c r="D17" s="45"/>
     </row>
     <row r="18" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="154"/>
-      <c r="B18" s="163"/>
-      <c r="C18" s="180"/>
+      <c r="A18" s="158"/>
+      <c r="B18" s="159"/>
+      <c r="C18" s="182"/>
       <c r="D18" s="45"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="154"/>
-      <c r="B19" s="163"/>
-      <c r="C19" s="180"/>
+      <c r="A19" s="158"/>
+      <c r="B19" s="159"/>
+      <c r="C19" s="182"/>
       <c r="D19" s="45"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="154"/>
-      <c r="B20" s="163"/>
-      <c r="C20" s="180"/>
+      <c r="A20" s="158"/>
+      <c r="B20" s="159"/>
+      <c r="C20" s="182"/>
       <c r="D20" s="45"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="154"/>
-      <c r="B21" s="163"/>
-      <c r="C21" s="180"/>
+      <c r="A21" s="158"/>
+      <c r="B21" s="159"/>
+      <c r="C21" s="182"/>
       <c r="D21" s="45"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="154"/>
-      <c r="B22" s="163"/>
-      <c r="C22" s="180"/>
+      <c r="A22" s="158"/>
+      <c r="B22" s="159"/>
+      <c r="C22" s="182"/>
       <c r="D22" s="45"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="154"/>
-      <c r="B23" s="163"/>
-      <c r="C23" s="180"/>
+      <c r="A23" s="158"/>
+      <c r="B23" s="159"/>
+      <c r="C23" s="182"/>
       <c r="D23" s="53" t="s">
         <v>192</v>
       </c>
@@ -31929,10 +31944,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="172" t="s">
+      <c r="A32" s="183" t="s">
         <v>205</v>
       </c>
-      <c r="B32" s="175" t="s">
+      <c r="B32" s="186" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="79" t="s">
@@ -31943,26 +31958,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="173"/>
-      <c r="B33" s="176"/>
+      <c r="A33" s="184"/>
+      <c r="B33" s="187"/>
       <c r="C33" s="65"/>
       <c r="D33" s="69"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="173"/>
-      <c r="B34" s="176"/>
+      <c r="A34" s="184"/>
+      <c r="B34" s="187"/>
       <c r="C34" s="65"/>
       <c r="D34" s="69"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="173"/>
-      <c r="B35" s="176"/>
+      <c r="A35" s="184"/>
+      <c r="B35" s="187"/>
       <c r="C35" s="65"/>
       <c r="D35" s="69"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="174"/>
-      <c r="B36" s="177"/>
+      <c r="A36" s="185"/>
+      <c r="B36" s="188"/>
       <c r="C36" s="65" t="s">
         <v>208</v>
       </c>
@@ -31991,10 +32006,10 @@
       <c r="D38" s="40"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="170" t="s">
+      <c r="A39" s="156" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="168" t="s">
+      <c r="B39" s="155" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="70" t="s">
@@ -32005,8 +32020,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="170"/>
-      <c r="B40" s="168"/>
+      <c r="A40" s="156"/>
+      <c r="B40" s="155"/>
       <c r="C40" s="64" t="s">
         <v>188</v>
       </c>
@@ -32015,84 +32030,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="169" t="s">
+      <c r="A41" s="154" t="s">
         <v>139</v>
       </c>
-      <c r="B41" s="168" t="s">
+      <c r="B41" s="155" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="181" t="s">
+      <c r="C41" s="179" t="s">
         <v>212</v>
       </c>
-      <c r="D41" s="154" t="s">
+      <c r="D41" s="158" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="169"/>
-      <c r="B42" s="168"/>
-      <c r="C42" s="181"/>
-      <c r="D42" s="154"/>
+      <c r="A42" s="154"/>
+      <c r="B42" s="155"/>
+      <c r="C42" s="179"/>
+      <c r="D42" s="158"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="169"/>
-      <c r="B43" s="168"/>
-      <c r="C43" s="181" t="s">
+      <c r="A43" s="154"/>
+      <c r="B43" s="155"/>
+      <c r="C43" s="179" t="s">
         <v>188</v>
       </c>
-      <c r="D43" s="164" t="s">
+      <c r="D43" s="161" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="169"/>
-      <c r="B44" s="168"/>
-      <c r="C44" s="181"/>
-      <c r="D44" s="164"/>
+      <c r="A44" s="154"/>
+      <c r="B44" s="155"/>
+      <c r="C44" s="179"/>
+      <c r="D44" s="161"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="162" t="s">
+      <c r="A45" s="160" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="163" t="s">
+      <c r="B45" s="159" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="185"/>
+      <c r="C45" s="175"/>
       <c r="D45" s="78" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="162"/>
-      <c r="B46" s="163"/>
-      <c r="C46" s="186"/>
-      <c r="D46" s="182" t="s">
+      <c r="A46" s="160"/>
+      <c r="B46" s="159"/>
+      <c r="C46" s="176"/>
+      <c r="D46" s="172" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="162"/>
-      <c r="B47" s="163"/>
-      <c r="C47" s="186"/>
-      <c r="D47" s="183"/>
+      <c r="A47" s="160"/>
+      <c r="B47" s="159"/>
+      <c r="C47" s="176"/>
+      <c r="D47" s="173"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="162"/>
-      <c r="B48" s="163"/>
-      <c r="C48" s="187"/>
-      <c r="D48" s="183"/>
+      <c r="A48" s="160"/>
+      <c r="B48" s="159"/>
+      <c r="C48" s="177"/>
+      <c r="D48" s="173"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="162"/>
-      <c r="B49" s="163"/>
-      <c r="C49" s="157"/>
-      <c r="D49" s="183"/>
+      <c r="A49" s="160"/>
+      <c r="B49" s="159"/>
+      <c r="C49" s="167"/>
+      <c r="D49" s="173"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="162"/>
-      <c r="B50" s="163"/>
-      <c r="C50" s="157"/>
-      <c r="D50" s="184"/>
+      <c r="A50" s="160"/>
+      <c r="B50" s="159"/>
+      <c r="C50" s="167"/>
+      <c r="D50" s="174"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="35" t="s">
@@ -32115,10 +32130,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="163" t="s">
+      <c r="A53" s="159" t="s">
         <v>156</v>
       </c>
-      <c r="B53" s="163" t="s">
+      <c r="B53" s="159" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="65" t="s">
@@ -32129,8 +32144,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="163"/>
-      <c r="B54" s="163"/>
+      <c r="A54" s="159"/>
+      <c r="B54" s="159"/>
       <c r="C54" s="65" t="s">
         <v>188</v>
       </c>
@@ -32139,8 +32154,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="163"/>
-      <c r="B55" s="163"/>
+      <c r="A55" s="159"/>
+      <c r="B55" s="159"/>
       <c r="C55" s="65" t="s">
         <v>218</v>
       </c>
@@ -32149,9 +32164,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="163"/>
-      <c r="B56" s="163"/>
-      <c r="C56" s="188" t="s">
+      <c r="A56" s="159"/>
+      <c r="B56" s="159"/>
+      <c r="C56" s="178" t="s">
         <v>220</v>
       </c>
       <c r="D56" s="71" t="s">
@@ -32159,16 +32174,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="163"/>
-      <c r="B57" s="163"/>
-      <c r="C57" s="188"/>
+      <c r="A57" s="159"/>
+      <c r="B57" s="159"/>
+      <c r="C57" s="178"/>
       <c r="D57" s="43" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="163"/>
-      <c r="B58" s="163"/>
+      <c r="A58" s="159"/>
+      <c r="B58" s="159"/>
       <c r="C58" s="65" t="s">
         <v>223</v>
       </c>
@@ -32177,8 +32192,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="163"/>
-      <c r="B59" s="163"/>
+      <c r="A59" s="159"/>
+      <c r="B59" s="159"/>
       <c r="C59" s="65" t="s">
         <v>225</v>
       </c>
@@ -32187,9 +32202,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="163"/>
-      <c r="B60" s="163"/>
-      <c r="C60" s="188" t="s">
+      <c r="A60" s="159"/>
+      <c r="B60" s="159"/>
+      <c r="C60" s="178" t="s">
         <v>227</v>
       </c>
       <c r="D60" s="42" t="s">
@@ -32197,25 +32212,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="163"/>
-      <c r="B61" s="163"/>
-      <c r="C61" s="188"/>
+      <c r="A61" s="159"/>
+      <c r="B61" s="159"/>
+      <c r="C61" s="178"/>
       <c r="D61" s="42" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="163"/>
-      <c r="B62" s="163"/>
-      <c r="C62" s="188"/>
+      <c r="A62" s="159"/>
+      <c r="B62" s="159"/>
+      <c r="C62" s="178"/>
       <c r="D62" s="71" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="163"/>
-      <c r="B63" s="163"/>
-      <c r="C63" s="181" t="s">
+      <c r="A63" s="159"/>
+      <c r="B63" s="159"/>
+      <c r="C63" s="179" t="s">
         <v>231</v>
       </c>
       <c r="D63" s="41" t="s">
@@ -32223,30 +32238,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="163"/>
-      <c r="B64" s="163"/>
-      <c r="C64" s="181"/>
-      <c r="D64" s="164" t="s">
+      <c r="A64" s="159"/>
+      <c r="B64" s="159"/>
+      <c r="C64" s="179"/>
+      <c r="D64" s="161" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="163"/>
-      <c r="B65" s="163"/>
-      <c r="C65" s="181"/>
-      <c r="D65" s="164"/>
+      <c r="A65" s="159"/>
+      <c r="B65" s="159"/>
+      <c r="C65" s="179"/>
+      <c r="D65" s="161"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="163"/>
-      <c r="B66" s="163"/>
-      <c r="C66" s="181"/>
-      <c r="D66" s="164"/>
+      <c r="A66" s="159"/>
+      <c r="B66" s="159"/>
+      <c r="C66" s="179"/>
+      <c r="D66" s="161"/>
     </row>
     <row r="67" spans="1:4" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="163"/>
-      <c r="B67" s="163"/>
-      <c r="C67" s="181"/>
-      <c r="D67" s="164"/>
+      <c r="A67" s="159"/>
+      <c r="B67" s="159"/>
+      <c r="C67" s="179"/>
+      <c r="D67" s="161"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="35"/>
@@ -32272,6 +32287,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -32288,23 +32320,6 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -32313,10 +32328,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D276"/>
+  <dimension ref="A1:D277"/>
   <sheetViews>
-    <sheetView topLeftCell="A248" workbookViewId="0">
-      <selection activeCell="A275" sqref="A275"/>
+    <sheetView tabSelected="1" topLeftCell="A251" workbookViewId="0">
+      <selection activeCell="B282" sqref="B282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32384,7 +32399,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="195" t="s">
+      <c r="A6" s="198" t="s">
         <v>243</v>
       </c>
       <c r="B6" s="192" t="s">
@@ -32396,7 +32411,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="196"/>
+      <c r="A7" s="199"/>
       <c r="B7" s="193"/>
       <c r="C7" s="84"/>
       <c r="D7" s="53" t="s">
@@ -32404,7 +32419,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="196"/>
+      <c r="A8" s="199"/>
       <c r="B8" s="193"/>
       <c r="C8" s="84"/>
       <c r="D8" s="104" t="s">
@@ -32412,7 +32427,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="196"/>
+      <c r="A9" s="199"/>
       <c r="B9" s="193"/>
       <c r="C9" s="84"/>
       <c r="D9" s="104" t="s">
@@ -32420,7 +32435,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="197"/>
+      <c r="A10" s="200"/>
       <c r="B10" s="194"/>
       <c r="C10" s="84" t="s">
         <v>248</v>
@@ -32472,7 +32487,7 @@
       <c r="D14" s="88"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="159" t="s">
+      <c r="A15" s="169" t="s">
         <v>256</v>
       </c>
       <c r="B15" s="192" t="s">
@@ -32486,7 +32501,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="160"/>
+      <c r="A16" s="170"/>
       <c r="B16" s="194"/>
       <c r="C16" s="99" t="s">
         <v>259</v>
@@ -32626,7 +32641,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="195" t="s">
+      <c r="A29" s="198" t="s">
         <v>281</v>
       </c>
       <c r="B29" s="192" t="s">
@@ -32640,7 +32655,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="196"/>
+      <c r="A30" s="199"/>
       <c r="B30" s="193"/>
       <c r="C30" s="84" t="s">
         <v>279</v>
@@ -32650,7 +32665,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="196"/>
+      <c r="A31" s="199"/>
       <c r="B31" s="193"/>
       <c r="C31" s="84">
         <v>3.3</v>
@@ -32660,7 +32675,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="196"/>
+      <c r="A32" s="199"/>
       <c r="B32" s="193"/>
       <c r="C32" s="90">
         <v>3</v>
@@ -32670,7 +32685,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="197"/>
+      <c r="A33" s="200"/>
       <c r="B33" s="194"/>
       <c r="C33" s="90">
         <v>3.5</v>
@@ -32680,7 +32695,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="195" t="s">
+      <c r="A34" s="198" t="s">
         <v>287</v>
       </c>
       <c r="B34" s="192" t="s">
@@ -32692,7 +32707,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="197"/>
+      <c r="A35" s="200"/>
       <c r="B35" s="194"/>
       <c r="C35" s="84"/>
       <c r="D35" s="62" t="s">
@@ -32700,7 +32715,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="212" t="s">
+      <c r="A36" s="201" t="s">
         <v>290</v>
       </c>
       <c r="B36" s="192" t="s">
@@ -32711,7 +32726,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="212"/>
+      <c r="A37" s="201"/>
       <c r="B37" s="193"/>
       <c r="C37" s="106" t="s">
         <v>292</v>
@@ -32721,7 +32736,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="212"/>
+      <c r="A38" s="201"/>
       <c r="B38" s="193"/>
       <c r="C38" s="53" t="s">
         <v>294</v>
@@ -32731,7 +32746,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="212"/>
+      <c r="A39" s="201"/>
       <c r="B39" s="193"/>
       <c r="C39" s="56" t="s">
         <v>296</v>
@@ -32797,7 +32812,7 @@
       <c r="B45" s="192" t="s">
         <v>244</v>
       </c>
-      <c r="C45" s="207"/>
+      <c r="C45" s="202"/>
       <c r="D45" s="107" t="s">
         <v>291</v>
       </c>
@@ -32805,7 +32820,7 @@
     <row r="46" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="191"/>
       <c r="B46" s="194"/>
-      <c r="C46" s="208"/>
+      <c r="C46" s="203"/>
       <c r="D46" s="107" t="s">
         <v>302</v>
       </c>
@@ -32855,10 +32870,10 @@
       <c r="D50" s="88"/>
     </row>
     <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="212" t="s">
+      <c r="A51" s="201" t="s">
         <v>307</v>
       </c>
-      <c r="B51" s="213" t="s">
+      <c r="B51" s="207" t="s">
         <v>244</v>
       </c>
       <c r="C51" s="84" t="s">
@@ -32869,8 +32884,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="212"/>
-      <c r="B52" s="213"/>
+      <c r="A52" s="201"/>
+      <c r="B52" s="207"/>
       <c r="C52" s="84" t="s">
         <v>310</v>
       </c>
@@ -32879,8 +32894,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="212"/>
-      <c r="B53" s="213"/>
+      <c r="A53" s="201"/>
+      <c r="B53" s="207"/>
       <c r="C53" s="84" t="s">
         <v>308</v>
       </c>
@@ -32897,10 +32912,10 @@
       <c r="D54" s="88"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="154" t="s">
+      <c r="A55" s="158" t="s">
         <v>13</v>
       </c>
-      <c r="B55" s="188" t="s">
+      <c r="B55" s="178" t="s">
         <v>244</v>
       </c>
       <c r="C55" s="53"/>
@@ -32909,8 +32924,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="154"/>
-      <c r="B56" s="188"/>
+      <c r="A56" s="158"/>
+      <c r="B56" s="178"/>
       <c r="C56" s="65" t="s">
         <v>314</v>
       </c>
@@ -32919,8 +32934,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="154"/>
-      <c r="B57" s="188"/>
+      <c r="A57" s="158"/>
+      <c r="B57" s="178"/>
       <c r="C57" s="65" t="s">
         <v>316</v>
       </c>
@@ -32929,8 +32944,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="154"/>
-      <c r="B58" s="188"/>
+      <c r="A58" s="158"/>
+      <c r="B58" s="178"/>
       <c r="C58" s="65" t="s">
         <v>316</v>
       </c>
@@ -32939,8 +32954,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="154"/>
-      <c r="B59" s="188"/>
+      <c r="A59" s="158"/>
+      <c r="B59" s="178"/>
       <c r="C59" s="65" t="s">
         <v>248</v>
       </c>
@@ -32949,8 +32964,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="154"/>
-      <c r="B60" s="188"/>
+      <c r="A60" s="158"/>
+      <c r="B60" s="178"/>
       <c r="C60" s="70" t="s">
         <v>248</v>
       </c>
@@ -32959,7 +32974,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="159" t="s">
+      <c r="A61" s="169" t="s">
         <v>26</v>
       </c>
       <c r="B61" s="192" t="s">
@@ -32973,7 +32988,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="198"/>
+      <c r="A62" s="210"/>
       <c r="B62" s="193"/>
       <c r="C62" s="65" t="s">
         <v>322</v>
@@ -32983,7 +32998,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="160"/>
+      <c r="A63" s="170"/>
       <c r="B63" s="194"/>
       <c r="C63" s="103" t="s">
         <v>324</v>
@@ -33033,10 +33048,10 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="154" t="s">
+      <c r="A67" s="158" t="s">
         <v>330</v>
       </c>
-      <c r="B67" s="188" t="s">
+      <c r="B67" s="178" t="s">
         <v>244</v>
       </c>
       <c r="C67" s="53" t="s">
@@ -33047,24 +33062,24 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="154"/>
-      <c r="B68" s="188"/>
+      <c r="A68" s="158"/>
+      <c r="B68" s="178"/>
       <c r="C68" s="53"/>
       <c r="D68" s="71" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="154"/>
-      <c r="B69" s="188"/>
+      <c r="A69" s="158"/>
+      <c r="B69" s="178"/>
       <c r="C69" s="53"/>
       <c r="D69" s="53" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="154"/>
-      <c r="B70" s="188"/>
+      <c r="A70" s="158"/>
+      <c r="B70" s="178"/>
       <c r="C70" s="65" t="s">
         <v>335</v>
       </c>
@@ -33073,8 +33088,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="154"/>
-      <c r="B71" s="188"/>
+      <c r="A71" s="158"/>
+      <c r="B71" s="178"/>
       <c r="C71" s="70" t="s">
         <v>337</v>
       </c>
@@ -33095,7 +33110,7 @@
       <c r="D72" s="53"/>
     </row>
     <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="209" t="s">
+      <c r="A73" s="204" t="s">
         <v>121</v>
       </c>
       <c r="B73" s="192" t="s">
@@ -33107,7 +33122,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="210"/>
+      <c r="A74" s="205"/>
       <c r="B74" s="193"/>
       <c r="C74" s="70" t="s">
         <v>341</v>
@@ -33117,7 +33132,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="210"/>
+      <c r="A75" s="205"/>
       <c r="B75" s="193"/>
       <c r="C75" s="70" t="s">
         <v>343</v>
@@ -33127,7 +33142,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="210"/>
+      <c r="A76" s="205"/>
       <c r="B76" s="193"/>
       <c r="C76" s="91" t="s">
         <v>345</v>
@@ -33137,7 +33152,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="210"/>
+      <c r="A77" s="205"/>
       <c r="B77" s="193"/>
       <c r="C77" s="70" t="s">
         <v>343</v>
@@ -33147,7 +33162,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="210"/>
+      <c r="A78" s="205"/>
       <c r="B78" s="193"/>
       <c r="C78" s="70" t="s">
         <v>348</v>
@@ -33157,7 +33172,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="210"/>
+      <c r="A79" s="205"/>
       <c r="B79" s="193"/>
       <c r="C79" s="70" t="s">
         <v>343</v>
@@ -33167,7 +33182,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="210"/>
+      <c r="A80" s="205"/>
       <c r="B80" s="193"/>
       <c r="C80" s="70" t="s">
         <v>351</v>
@@ -33177,7 +33192,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="210"/>
+      <c r="A81" s="205"/>
       <c r="B81" s="193"/>
       <c r="C81" s="70" t="s">
         <v>353</v>
@@ -33187,7 +33202,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="210"/>
+      <c r="A82" s="205"/>
       <c r="B82" s="193"/>
       <c r="C82" s="70" t="s">
         <v>343</v>
@@ -33197,7 +33212,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="210"/>
+      <c r="A83" s="205"/>
       <c r="B83" s="193"/>
       <c r="C83" s="70" t="s">
         <v>353</v>
@@ -33207,7 +33222,7 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="210"/>
+      <c r="A84" s="205"/>
       <c r="B84" s="193"/>
       <c r="C84" s="70" t="s">
         <v>343</v>
@@ -33217,7 +33232,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="210"/>
+      <c r="A85" s="205"/>
       <c r="B85" s="193"/>
       <c r="C85" s="70" t="s">
         <v>248</v>
@@ -33227,7 +33242,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="210"/>
+      <c r="A86" s="205"/>
       <c r="B86" s="193"/>
       <c r="C86" s="70" t="s">
         <v>248</v>
@@ -33237,7 +33252,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="210"/>
+      <c r="A87" s="205"/>
       <c r="B87" s="193"/>
       <c r="C87" s="91" t="s">
         <v>359</v>
@@ -33247,7 +33262,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="211"/>
+      <c r="A88" s="206"/>
       <c r="B88" s="194"/>
       <c r="C88" s="70" t="s">
         <v>248</v>
@@ -33297,7 +33312,7 @@
       <c r="D91" s="53"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="159" t="s">
+      <c r="A92" s="169" t="s">
         <v>368</v>
       </c>
       <c r="B92" s="192" t="s">
@@ -33309,7 +33324,7 @@
       <c r="D92" s="53"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="160"/>
+      <c r="A93" s="170"/>
       <c r="B93" s="194"/>
       <c r="C93" s="70" t="s">
         <v>337</v>
@@ -33327,7 +33342,7 @@
       <c r="D94" s="87"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="159" t="s">
+      <c r="A95" s="169" t="s">
         <v>369</v>
       </c>
       <c r="B95" s="192" t="s">
@@ -33339,7 +33354,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="198"/>
+      <c r="A96" s="210"/>
       <c r="B96" s="193"/>
       <c r="C96" s="53"/>
       <c r="D96" s="53" t="s">
@@ -33347,7 +33362,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="198"/>
+      <c r="A97" s="210"/>
       <c r="B97" s="193"/>
       <c r="C97" s="53"/>
       <c r="D97" s="53" t="s">
@@ -33355,7 +33370,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="198"/>
+      <c r="A98" s="210"/>
       <c r="B98" s="193"/>
       <c r="C98" s="53" t="s">
         <v>373</v>
@@ -33365,7 +33380,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="198"/>
+      <c r="A99" s="210"/>
       <c r="B99" s="193"/>
       <c r="C99" s="53" t="s">
         <v>375</v>
@@ -33375,7 +33390,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="198"/>
+      <c r="A100" s="210"/>
       <c r="B100" s="193"/>
       <c r="C100" s="53" t="s">
         <v>377</v>
@@ -33385,7 +33400,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="198"/>
+      <c r="A101" s="210"/>
       <c r="B101" s="193"/>
       <c r="C101" s="56" t="s">
         <v>379</v>
@@ -33395,7 +33410,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="198"/>
+      <c r="A102" s="210"/>
       <c r="B102" s="193"/>
       <c r="C102" s="53" t="s">
         <v>41</v>
@@ -33405,7 +33420,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="198"/>
+      <c r="A103" s="210"/>
       <c r="B103" s="193"/>
       <c r="C103" s="90" t="s">
         <v>343</v>
@@ -33415,7 +33430,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="198"/>
+      <c r="A104" s="210"/>
       <c r="B104" s="193"/>
       <c r="C104" s="90" t="s">
         <v>353</v>
@@ -33425,7 +33440,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="198"/>
+      <c r="A105" s="210"/>
       <c r="B105" s="193"/>
       <c r="C105" s="90" t="s">
         <v>377</v>
@@ -33435,7 +33450,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="198"/>
+      <c r="A106" s="210"/>
       <c r="B106" s="193"/>
       <c r="C106" s="90" t="s">
         <v>343</v>
@@ -33445,7 +33460,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="198"/>
+      <c r="A107" s="210"/>
       <c r="B107" s="193"/>
       <c r="C107" s="90" t="s">
         <v>248</v>
@@ -33455,7 +33470,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="198"/>
+      <c r="A108" s="210"/>
       <c r="B108" s="193"/>
       <c r="C108" s="90" t="s">
         <v>248</v>
@@ -33465,7 +33480,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="198"/>
+      <c r="A109" s="210"/>
       <c r="B109" s="193"/>
       <c r="C109" s="91" t="s">
         <v>359</v>
@@ -33475,7 +33490,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="160"/>
+      <c r="A110" s="170"/>
       <c r="B110" s="194"/>
       <c r="C110" s="90" t="s">
         <v>248</v>
@@ -33485,7 +33500,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="199" t="s">
+      <c r="A111" s="211" t="s">
         <v>36</v>
       </c>
       <c r="B111" s="192" t="s">
@@ -33499,7 +33514,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="200"/>
+      <c r="A112" s="212"/>
       <c r="B112" s="193"/>
       <c r="C112" s="53" t="s">
         <v>383</v>
@@ -33509,7 +33524,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="200"/>
+      <c r="A113" s="212"/>
       <c r="B113" s="193"/>
       <c r="C113" s="53"/>
       <c r="D113" s="53" t="s">
@@ -33517,7 +33532,7 @@
       </c>
     </row>
     <row r="114" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="200"/>
+      <c r="A114" s="212"/>
       <c r="B114" s="193"/>
       <c r="C114" s="56" t="s">
         <v>386</v>
@@ -33527,7 +33542,7 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="200"/>
+      <c r="A115" s="212"/>
       <c r="B115" s="193"/>
       <c r="C115" s="56" t="s">
         <v>343</v>
@@ -33537,7 +33552,7 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="200"/>
+      <c r="A116" s="212"/>
       <c r="B116" s="193"/>
       <c r="C116" s="56" t="s">
         <v>345</v>
@@ -33547,7 +33562,7 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="200"/>
+      <c r="A117" s="212"/>
       <c r="B117" s="193"/>
       <c r="C117" s="56" t="s">
         <v>348</v>
@@ -33557,7 +33572,7 @@
       </c>
     </row>
     <row r="118" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="200"/>
+      <c r="A118" s="212"/>
       <c r="B118" s="193"/>
       <c r="C118" s="56" t="s">
         <v>389</v>
@@ -33567,7 +33582,7 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="200"/>
+      <c r="A119" s="212"/>
       <c r="B119" s="193"/>
       <c r="C119" s="90" t="s">
         <v>343</v>
@@ -33577,7 +33592,7 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="200"/>
+      <c r="A120" s="212"/>
       <c r="B120" s="193"/>
       <c r="C120" s="90" t="s">
         <v>351</v>
@@ -33587,7 +33602,7 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="200"/>
+      <c r="A121" s="212"/>
       <c r="B121" s="193"/>
       <c r="C121" s="90" t="s">
         <v>353</v>
@@ -33597,7 +33612,7 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="200"/>
+      <c r="A122" s="212"/>
       <c r="B122" s="193"/>
       <c r="C122" s="90" t="s">
         <v>343</v>
@@ -33607,7 +33622,7 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="200"/>
+      <c r="A123" s="212"/>
       <c r="B123" s="193"/>
       <c r="C123" s="90" t="s">
         <v>353</v>
@@ -33617,7 +33632,7 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="200"/>
+      <c r="A124" s="212"/>
       <c r="B124" s="193"/>
       <c r="C124" s="90" t="s">
         <v>377</v>
@@ -33627,7 +33642,7 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="200"/>
+      <c r="A125" s="212"/>
       <c r="B125" s="193"/>
       <c r="C125" s="90" t="s">
         <v>343</v>
@@ -33637,7 +33652,7 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="200"/>
+      <c r="A126" s="212"/>
       <c r="B126" s="193"/>
       <c r="C126" s="90" t="s">
         <v>248</v>
@@ -33647,7 +33662,7 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="200"/>
+      <c r="A127" s="212"/>
       <c r="B127" s="193"/>
       <c r="C127" s="90" t="s">
         <v>248</v>
@@ -33657,7 +33672,7 @@
       </c>
     </row>
     <row r="128" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A128" s="200"/>
+      <c r="A128" s="212"/>
       <c r="B128" s="193"/>
       <c r="C128" s="91" t="s">
         <v>359</v>
@@ -33667,7 +33682,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="201"/>
+      <c r="A129" s="213"/>
       <c r="B129" s="194"/>
       <c r="C129" s="90" t="s">
         <v>248</v>
@@ -33677,13 +33692,13 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="159" t="s">
+      <c r="A130" s="169" t="s">
         <v>205</v>
       </c>
       <c r="B130" s="192" t="s">
         <v>244</v>
       </c>
-      <c r="C130" s="202" t="s">
+      <c r="C130" s="214" t="s">
         <v>392</v>
       </c>
       <c r="D130" s="80" t="s">
@@ -33691,17 +33706,17 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="198"/>
+      <c r="A131" s="210"/>
       <c r="B131" s="193"/>
-      <c r="C131" s="203"/>
+      <c r="C131" s="215"/>
       <c r="D131" s="53" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="198"/>
+      <c r="A132" s="210"/>
       <c r="B132" s="193"/>
-      <c r="C132" s="204" t="s">
+      <c r="C132" s="216" t="s">
         <v>395</v>
       </c>
       <c r="D132" s="53" t="s">
@@ -33709,15 +33724,15 @@
       </c>
     </row>
     <row r="133" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A133" s="198"/>
+      <c r="A133" s="210"/>
       <c r="B133" s="193"/>
-      <c r="C133" s="204"/>
+      <c r="C133" s="216"/>
       <c r="D133" s="56" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="198"/>
+      <c r="A134" s="210"/>
       <c r="B134" s="193"/>
       <c r="C134" s="70" t="s">
         <v>398</v>
@@ -33727,7 +33742,7 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="198"/>
+      <c r="A135" s="210"/>
       <c r="B135" s="193"/>
       <c r="C135" s="70">
         <v>2.1</v>
@@ -33737,7 +33752,7 @@
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="198"/>
+      <c r="A136" s="210"/>
       <c r="B136" s="193"/>
       <c r="C136" s="70" t="s">
         <v>392</v>
@@ -33747,7 +33762,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="198"/>
+      <c r="A137" s="210"/>
       <c r="B137" s="193"/>
       <c r="C137" s="70" t="s">
         <v>392</v>
@@ -33757,7 +33772,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="198"/>
+      <c r="A138" s="210"/>
       <c r="B138" s="193"/>
       <c r="C138" s="70" t="s">
         <v>392</v>
@@ -33767,7 +33782,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="198"/>
+      <c r="A139" s="210"/>
       <c r="B139" s="193"/>
       <c r="C139" s="93" t="s">
         <v>404</v>
@@ -33777,7 +33792,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="198"/>
+      <c r="A140" s="210"/>
       <c r="B140" s="193"/>
       <c r="C140" s="70">
         <v>2.1</v>
@@ -33787,7 +33802,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="198"/>
+      <c r="A141" s="210"/>
       <c r="B141" s="193"/>
       <c r="C141" s="70" t="s">
         <v>392</v>
@@ -33797,7 +33812,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="198"/>
+      <c r="A142" s="210"/>
       <c r="B142" s="193"/>
       <c r="C142" s="70" t="s">
         <v>392</v>
@@ -33807,7 +33822,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="198"/>
+      <c r="A143" s="210"/>
       <c r="B143" s="193"/>
       <c r="C143" s="70">
         <v>2.1</v>
@@ -33817,7 +33832,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="199" t="s">
+      <c r="A144" s="211" t="s">
         <v>409</v>
       </c>
       <c r="B144" s="192" t="s">
@@ -33831,7 +33846,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A145" s="200"/>
+      <c r="A145" s="212"/>
       <c r="B145" s="193"/>
       <c r="C145" s="56" t="s">
         <v>412</v>
@@ -33841,7 +33856,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="201"/>
+      <c r="A146" s="213"/>
       <c r="B146" s="194"/>
       <c r="C146" s="53" t="s">
         <v>414</v>
@@ -33851,7 +33866,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="159" t="s">
+      <c r="A147" s="169" t="s">
         <v>416</v>
       </c>
       <c r="B147" s="192" t="s">
@@ -33863,7 +33878,7 @@
       <c r="D147" s="53"/>
     </row>
     <row r="148" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="198"/>
+      <c r="A148" s="210"/>
       <c r="B148" s="193"/>
       <c r="C148" s="70" t="s">
         <v>404</v>
@@ -33873,7 +33888,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="198"/>
+      <c r="A149" s="210"/>
       <c r="B149" s="193"/>
       <c r="C149" s="70">
         <v>2.1</v>
@@ -33883,7 +33898,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="198"/>
+      <c r="A150" s="210"/>
       <c r="B150" s="193"/>
       <c r="C150" s="70" t="s">
         <v>395</v>
@@ -33893,7 +33908,7 @@
       </c>
     </row>
     <row r="151" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="198"/>
+      <c r="A151" s="210"/>
       <c r="B151" s="193"/>
       <c r="C151" s="70" t="s">
         <v>392</v>
@@ -33923,7 +33938,7 @@
       <c r="D153" s="53"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="159" t="s">
+      <c r="A154" s="169" t="s">
         <v>420</v>
       </c>
       <c r="B154" s="192" t="s">
@@ -33935,7 +33950,7 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="198"/>
+      <c r="A155" s="210"/>
       <c r="B155" s="193"/>
       <c r="C155" s="53"/>
       <c r="D155" s="53" t="s">
@@ -33943,7 +33958,7 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="198"/>
+      <c r="A156" s="210"/>
       <c r="B156" s="193"/>
       <c r="C156" s="53"/>
       <c r="D156" s="53" t="s">
@@ -33951,7 +33966,7 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="198"/>
+      <c r="A157" s="210"/>
       <c r="B157" s="193"/>
       <c r="C157" s="53" t="s">
         <v>422</v>
@@ -33961,7 +33976,7 @@
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="198"/>
+      <c r="A158" s="210"/>
       <c r="B158" s="193"/>
       <c r="C158" s="53" t="s">
         <v>423</v>
@@ -33971,7 +33986,7 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="198"/>
+      <c r="A159" s="210"/>
       <c r="B159" s="193"/>
       <c r="C159" s="53" t="s">
         <v>316</v>
@@ -33981,7 +33996,7 @@
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="198"/>
+      <c r="A160" s="210"/>
       <c r="B160" s="193"/>
       <c r="C160" s="53" t="s">
         <v>248</v>
@@ -33991,10 +34006,10 @@
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="154" t="s">
+      <c r="A161" s="158" t="s">
         <v>426</v>
       </c>
-      <c r="B161" s="188" t="s">
+      <c r="B161" s="178" t="s">
         <v>244</v>
       </c>
       <c r="C161" s="71" t="s">
@@ -34005,8 +34020,8 @@
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="154"/>
-      <c r="B162" s="188"/>
+      <c r="A162" s="158"/>
+      <c r="B162" s="178"/>
       <c r="C162" s="53" t="s">
         <v>429</v>
       </c>
@@ -34015,8 +34030,8 @@
       </c>
     </row>
     <row r="163" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A163" s="154"/>
-      <c r="B163" s="188"/>
+      <c r="A163" s="158"/>
+      <c r="B163" s="178"/>
       <c r="C163" s="94" t="s">
         <v>431</v>
       </c>
@@ -34025,32 +34040,32 @@
       </c>
     </row>
     <row r="164" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A164" s="154"/>
-      <c r="B164" s="188"/>
+      <c r="A164" s="158"/>
+      <c r="B164" s="178"/>
       <c r="C164" s="94" t="s">
         <v>433</v>
       </c>
       <c r="D164" s="193"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="154"/>
-      <c r="B165" s="188"/>
+      <c r="A165" s="158"/>
+      <c r="B165" s="178"/>
       <c r="C165" s="94" t="s">
         <v>434</v>
       </c>
       <c r="D165" s="193"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="154"/>
-      <c r="B166" s="188"/>
+      <c r="A166" s="158"/>
+      <c r="B166" s="178"/>
       <c r="C166" s="94" t="s">
         <v>435</v>
       </c>
       <c r="D166" s="193"/>
     </row>
     <row r="167" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A167" s="154"/>
-      <c r="B167" s="188"/>
+      <c r="A167" s="158"/>
+      <c r="B167" s="178"/>
       <c r="C167" s="94" t="s">
         <v>436</v>
       </c>
@@ -34073,7 +34088,7 @@
       </c>
     </row>
     <row r="169" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="214" t="s">
+      <c r="A169" s="195" t="s">
         <v>43</v>
       </c>
       <c r="B169" s="192" t="s">
@@ -34087,7 +34102,7 @@
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="215"/>
+      <c r="A170" s="196"/>
       <c r="B170" s="193"/>
       <c r="C170" s="53" t="s">
         <v>439</v>
@@ -34097,7 +34112,7 @@
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="215"/>
+      <c r="A171" s="196"/>
       <c r="B171" s="193"/>
       <c r="C171" s="53" t="s">
         <v>440</v>
@@ -34107,7 +34122,7 @@
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="215"/>
+      <c r="A172" s="196"/>
       <c r="B172" s="193"/>
       <c r="C172" s="53" t="s">
         <v>441</v>
@@ -34117,7 +34132,7 @@
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="215"/>
+      <c r="A173" s="196"/>
       <c r="B173" s="193"/>
       <c r="C173" s="53" t="s">
         <v>442</v>
@@ -34127,7 +34142,7 @@
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="215"/>
+      <c r="A174" s="196"/>
       <c r="B174" s="193"/>
       <c r="C174" s="53" t="s">
         <v>443</v>
@@ -34137,7 +34152,7 @@
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="215"/>
+      <c r="A175" s="196"/>
       <c r="B175" s="193"/>
       <c r="C175" s="53" t="s">
         <v>445</v>
@@ -34147,7 +34162,7 @@
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="215"/>
+      <c r="A176" s="196"/>
       <c r="B176" s="193"/>
       <c r="C176" s="53" t="s">
         <v>446</v>
@@ -34157,7 +34172,7 @@
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="215"/>
+      <c r="A177" s="196"/>
       <c r="B177" s="193"/>
       <c r="C177" s="53" t="s">
         <v>447</v>
@@ -34167,7 +34182,7 @@
       </c>
     </row>
     <row r="178" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A178" s="215"/>
+      <c r="A178" s="196"/>
       <c r="B178" s="193"/>
       <c r="C178" s="95" t="s">
         <v>448</v>
@@ -34177,7 +34192,7 @@
       </c>
     </row>
     <row r="179" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A179" s="215"/>
+      <c r="A179" s="196"/>
       <c r="B179" s="193"/>
       <c r="C179" s="56" t="s">
         <v>450</v>
@@ -34187,7 +34202,7 @@
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="215"/>
+      <c r="A180" s="196"/>
       <c r="B180" s="193"/>
       <c r="C180" s="53" t="s">
         <v>451</v>
@@ -34197,7 +34212,7 @@
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="215"/>
+      <c r="A181" s="196"/>
       <c r="B181" s="193"/>
       <c r="C181" s="53" t="s">
         <v>452</v>
@@ -34207,7 +34222,7 @@
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="215"/>
+      <c r="A182" s="196"/>
       <c r="B182" s="193"/>
       <c r="C182" s="53" t="s">
         <v>454</v>
@@ -34217,7 +34232,7 @@
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="215"/>
+      <c r="A183" s="196"/>
       <c r="B183" s="193"/>
       <c r="C183" s="53" t="s">
         <v>438</v>
@@ -34227,7 +34242,7 @@
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="215"/>
+      <c r="A184" s="196"/>
       <c r="B184" s="193"/>
       <c r="C184" s="53" t="s">
         <v>455</v>
@@ -34237,7 +34252,7 @@
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="215"/>
+      <c r="A185" s="196"/>
       <c r="B185" s="193"/>
       <c r="C185" s="53" t="s">
         <v>443</v>
@@ -34247,7 +34262,7 @@
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="215"/>
+      <c r="A186" s="196"/>
       <c r="B186" s="193"/>
       <c r="C186" s="53" t="s">
         <v>457</v>
@@ -34257,7 +34272,7 @@
       </c>
     </row>
     <row r="187" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A187" s="215"/>
+      <c r="A187" s="196"/>
       <c r="B187" s="193"/>
       <c r="C187" s="53"/>
       <c r="D187" s="81" t="s">
@@ -34265,7 +34280,7 @@
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="215"/>
+      <c r="A188" s="196"/>
       <c r="B188" s="193"/>
       <c r="C188" s="53" t="s">
         <v>459</v>
@@ -34275,7 +34290,7 @@
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="215"/>
+      <c r="A189" s="196"/>
       <c r="B189" s="193"/>
       <c r="C189" s="53" t="s">
         <v>438</v>
@@ -34285,7 +34300,7 @@
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="215"/>
+      <c r="A190" s="196"/>
       <c r="B190" s="193"/>
       <c r="C190" s="53" t="s">
         <v>460</v>
@@ -34295,7 +34310,7 @@
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="215"/>
+      <c r="A191" s="196"/>
       <c r="B191" s="193"/>
       <c r="C191" s="53" t="s">
         <v>461</v>
@@ -34305,7 +34320,7 @@
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="215"/>
+      <c r="A192" s="196"/>
       <c r="B192" s="193"/>
       <c r="C192" s="53" t="s">
         <v>462</v>
@@ -34315,7 +34330,7 @@
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="215"/>
+      <c r="A193" s="196"/>
       <c r="B193" s="193"/>
       <c r="C193" s="53" t="s">
         <v>464</v>
@@ -34325,7 +34340,7 @@
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="215"/>
+      <c r="A194" s="196"/>
       <c r="B194" s="193"/>
       <c r="C194" s="53" t="s">
         <v>465</v>
@@ -34335,7 +34350,7 @@
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="215"/>
+      <c r="A195" s="196"/>
       <c r="B195" s="193"/>
       <c r="C195" s="53" t="s">
         <v>467</v>
@@ -34345,7 +34360,7 @@
       </c>
     </row>
     <row r="196" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A196" s="215"/>
+      <c r="A196" s="196"/>
       <c r="B196" s="193"/>
       <c r="C196" s="85" t="s">
         <v>469</v>
@@ -34355,7 +34370,7 @@
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="215"/>
+      <c r="A197" s="196"/>
       <c r="B197" s="193"/>
       <c r="C197" s="53" t="s">
         <v>471</v>
@@ -34365,7 +34380,7 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="215"/>
+      <c r="A198" s="196"/>
       <c r="B198" s="193"/>
       <c r="C198" s="53" t="s">
         <v>472</v>
@@ -34375,7 +34390,7 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="215"/>
+      <c r="A199" s="196"/>
       <c r="B199" s="193"/>
       <c r="C199" s="53" t="s">
         <v>473</v>
@@ -34385,7 +34400,7 @@
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="215"/>
+      <c r="A200" s="196"/>
       <c r="B200" s="193"/>
       <c r="C200" s="53" t="s">
         <v>474</v>
@@ -34395,7 +34410,7 @@
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="215"/>
+      <c r="A201" s="196"/>
       <c r="B201" s="193"/>
       <c r="C201" s="53" t="s">
         <v>475</v>
@@ -34405,7 +34420,7 @@
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="215"/>
+      <c r="A202" s="196"/>
       <c r="B202" s="193"/>
       <c r="C202" s="53" t="s">
         <v>473</v>
@@ -34415,7 +34430,7 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="215"/>
+      <c r="A203" s="196"/>
       <c r="B203" s="193"/>
       <c r="C203" s="92" t="s">
         <v>476</v>
@@ -34425,7 +34440,7 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="215"/>
+      <c r="A204" s="196"/>
       <c r="B204" s="193"/>
       <c r="C204" s="53" t="s">
         <v>478</v>
@@ -34435,7 +34450,7 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="215"/>
+      <c r="A205" s="196"/>
       <c r="B205" s="193"/>
       <c r="C205" s="53" t="s">
         <v>480</v>
@@ -34445,7 +34460,7 @@
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="215"/>
+      <c r="A206" s="196"/>
       <c r="B206" s="193"/>
       <c r="C206" s="53" t="s">
         <v>482</v>
@@ -34455,7 +34470,7 @@
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="215"/>
+      <c r="A207" s="196"/>
       <c r="B207" s="193"/>
       <c r="C207" s="53" t="s">
         <v>484</v>
@@ -34465,7 +34480,7 @@
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="215"/>
+      <c r="A208" s="196"/>
       <c r="B208" s="193"/>
       <c r="C208" s="53" t="s">
         <v>485</v>
@@ -34475,7 +34490,7 @@
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" s="215"/>
+      <c r="A209" s="196"/>
       <c r="B209" s="193"/>
       <c r="C209" s="53" t="s">
         <v>486</v>
@@ -34485,7 +34500,7 @@
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="215"/>
+      <c r="A210" s="196"/>
       <c r="B210" s="193"/>
       <c r="C210" s="53" t="s">
         <v>487</v>
@@ -34495,7 +34510,7 @@
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="215"/>
+      <c r="A211" s="196"/>
       <c r="B211" s="193"/>
       <c r="C211" s="53" t="s">
         <v>488</v>
@@ -34505,7 +34520,7 @@
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="215"/>
+      <c r="A212" s="196"/>
       <c r="B212" s="193"/>
       <c r="C212" s="53" t="s">
         <v>489</v>
@@ -34515,7 +34530,7 @@
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" s="215"/>
+      <c r="A213" s="196"/>
       <c r="B213" s="193"/>
       <c r="C213" s="53" t="s">
         <v>490</v>
@@ -34525,7 +34540,7 @@
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" s="215"/>
+      <c r="A214" s="196"/>
       <c r="B214" s="193"/>
       <c r="C214" s="53" t="s">
         <v>491</v>
@@ -34535,7 +34550,7 @@
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" s="215"/>
+      <c r="A215" s="196"/>
       <c r="B215" s="193"/>
       <c r="C215" s="53" t="s">
         <v>492</v>
@@ -34545,7 +34560,7 @@
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="215"/>
+      <c r="A216" s="196"/>
       <c r="B216" s="193"/>
       <c r="C216" s="53" t="s">
         <v>494</v>
@@ -34555,7 +34570,7 @@
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" s="215"/>
+      <c r="A217" s="196"/>
       <c r="B217" s="193"/>
       <c r="C217" s="53" t="s">
         <v>490</v>
@@ -34565,7 +34580,7 @@
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" s="215"/>
+      <c r="A218" s="196"/>
       <c r="B218" s="193"/>
       <c r="C218" s="53" t="s">
         <v>495</v>
@@ -34575,7 +34590,7 @@
       </c>
     </row>
     <row r="219" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A219" s="215"/>
+      <c r="A219" s="196"/>
       <c r="B219" s="193"/>
       <c r="C219" s="56" t="s">
         <v>496</v>
@@ -34585,7 +34600,7 @@
       </c>
     </row>
     <row r="220" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A220" s="216"/>
+      <c r="A220" s="197"/>
       <c r="B220" s="194"/>
       <c r="C220" s="56" t="s">
         <v>465</v>
@@ -34595,7 +34610,7 @@
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" s="214" t="s">
+      <c r="A221" s="195" t="s">
         <v>497</v>
       </c>
       <c r="B221" s="192" t="s">
@@ -34609,7 +34624,7 @@
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" s="215"/>
+      <c r="A222" s="196"/>
       <c r="B222" s="193"/>
       <c r="C222" s="92" t="s">
         <v>499</v>
@@ -34619,7 +34634,7 @@
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223" s="216"/>
+      <c r="A223" s="197"/>
       <c r="B223" s="194"/>
       <c r="C223" s="53" t="s">
         <v>500</v>
@@ -34665,7 +34680,7 @@
       <c r="D226" s="88"/>
     </row>
     <row r="227" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="159" t="s">
+      <c r="A227" s="169" t="s">
         <v>156</v>
       </c>
       <c r="B227" s="192" t="s">
@@ -34677,7 +34692,7 @@
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" s="198"/>
+      <c r="A228" s="210"/>
       <c r="B228" s="193"/>
       <c r="C228" s="65" t="s">
         <v>503</v>
@@ -34687,7 +34702,7 @@
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="198"/>
+      <c r="A229" s="210"/>
       <c r="B229" s="193"/>
       <c r="C229" s="65">
         <v>10.1</v>
@@ -34697,7 +34712,7 @@
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="198"/>
+      <c r="A230" s="210"/>
       <c r="B230" s="193"/>
       <c r="C230" s="65">
         <v>10.199999999999999</v>
@@ -34707,7 +34722,7 @@
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="198"/>
+      <c r="A231" s="210"/>
       <c r="B231" s="193"/>
       <c r="C231" s="82" t="s">
         <v>506</v>
@@ -34717,7 +34732,7 @@
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="198"/>
+      <c r="A232" s="210"/>
       <c r="B232" s="193"/>
       <c r="C232" s="82" t="s">
         <v>508</v>
@@ -34727,7 +34742,7 @@
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="198"/>
+      <c r="A233" s="210"/>
       <c r="B233" s="193"/>
       <c r="C233" s="82" t="s">
         <v>166</v>
@@ -34737,7 +34752,7 @@
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="198"/>
+      <c r="A234" s="210"/>
       <c r="B234" s="193"/>
       <c r="C234" s="82" t="s">
         <v>511</v>
@@ -34747,7 +34762,7 @@
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="198"/>
+      <c r="A235" s="210"/>
       <c r="B235" s="193"/>
       <c r="C235" s="82" t="s">
         <v>60</v>
@@ -34757,7 +34772,7 @@
       </c>
     </row>
     <row r="236" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A236" s="198"/>
+      <c r="A236" s="210"/>
       <c r="B236" s="193"/>
       <c r="C236" s="82" t="s">
         <v>514</v>
@@ -34767,7 +34782,7 @@
       </c>
     </row>
     <row r="237" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A237" s="160"/>
+      <c r="A237" s="170"/>
       <c r="B237" s="194"/>
       <c r="C237" s="82" t="s">
         <v>514</v>
@@ -34777,7 +34792,7 @@
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" s="159" t="s">
+      <c r="A238" s="169" t="s">
         <v>517</v>
       </c>
       <c r="B238" s="192" t="s">
@@ -34789,7 +34804,7 @@
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" s="198"/>
+      <c r="A239" s="210"/>
       <c r="B239" s="193"/>
       <c r="C239" s="62" t="s">
         <v>518</v>
@@ -34821,7 +34836,7 @@
       <c r="D241" s="98"/>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="159" t="s">
+      <c r="A242" s="169" t="s">
         <v>74</v>
       </c>
       <c r="B242" s="192" t="s">
@@ -34835,7 +34850,7 @@
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="198"/>
+      <c r="A243" s="210"/>
       <c r="B243" s="193"/>
       <c r="C243" s="99" t="s">
         <v>257</v>
@@ -34845,7 +34860,7 @@
       </c>
     </row>
     <row r="244" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A244" s="160"/>
+      <c r="A244" s="170"/>
       <c r="B244" s="194"/>
       <c r="C244" s="53"/>
       <c r="D244" s="53" t="s">
@@ -34853,7 +34868,7 @@
       </c>
     </row>
     <row r="245" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A245" s="205" t="s">
+      <c r="A245" s="208" t="s">
         <v>75</v>
       </c>
       <c r="B245" s="192" t="s">
@@ -34867,7 +34882,7 @@
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A246" s="206"/>
+      <c r="A246" s="209"/>
       <c r="B246" s="194"/>
       <c r="C246" s="56"/>
       <c r="D246" s="53" t="s">
@@ -34875,7 +34890,7 @@
       </c>
     </row>
     <row r="247" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A247" s="205" t="s">
+      <c r="A247" s="208" t="s">
         <v>527</v>
       </c>
       <c r="B247" s="192" t="s">
@@ -34887,7 +34902,7 @@
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A248" s="206"/>
+      <c r="A248" s="209"/>
       <c r="B248" s="194"/>
       <c r="C248" s="53"/>
       <c r="D248" s="53" t="s">
@@ -34895,7 +34910,7 @@
       </c>
     </row>
     <row r="249" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A249" s="205" t="s">
+      <c r="A249" s="208" t="s">
         <v>76</v>
       </c>
       <c r="B249" s="192" t="s">
@@ -34909,7 +34924,7 @@
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A250" s="206"/>
+      <c r="A250" s="209"/>
       <c r="B250" s="194"/>
       <c r="C250" s="53"/>
       <c r="D250" s="53" t="s">
@@ -35161,7 +35176,7 @@
       <c r="A272" s="90" t="s">
         <v>707</v>
       </c>
-      <c r="B272" s="137" t="str">
+      <c r="B272" s="135" t="str">
         <f>$B$270</f>
         <v>PIT Next Version</v>
       </c>
@@ -35176,7 +35191,7 @@
       <c r="A273" s="90" t="s">
         <v>287</v>
       </c>
-      <c r="B273" s="138" t="str">
+      <c r="B273" s="136" t="str">
         <f>$B$270</f>
         <v>PIT Next Version</v>
       </c>
@@ -35191,7 +35206,7 @@
       <c r="A274" s="90" t="s">
         <v>714</v>
       </c>
-      <c r="B274" s="138" t="str">
+      <c r="B274" s="136" t="str">
         <f>$B$270</f>
         <v>PIT Next Version</v>
       </c>
@@ -35206,7 +35221,7 @@
       <c r="A275" s="90" t="s">
         <v>715</v>
       </c>
-      <c r="B275" s="138" t="str">
+      <c r="B275" s="136" t="str">
         <f>$B$270</f>
         <v>PIT Next Version</v>
       </c>
@@ -35217,14 +35232,88 @@
         <v>713</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A276" s="135"/>
-      <c r="B276" s="136"/>
-      <c r="C276" s="135"/>
-      <c r="D276" s="135"/>
+    <row r="276" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A276" s="56" t="s">
+        <v>721</v>
+      </c>
+      <c r="B276" s="138" t="str">
+        <f t="shared" ref="B276:B277" si="0">$B$270</f>
+        <v>PIT Next Version</v>
+      </c>
+      <c r="C276" s="90" t="s">
+        <v>39</v>
+      </c>
+      <c r="D276" s="90" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A277" s="53" t="s">
+        <v>722</v>
+      </c>
+      <c r="B277" s="138" t="str">
+        <f t="shared" si="0"/>
+        <v>PIT Next Version</v>
+      </c>
+      <c r="C277" s="90" t="s">
+        <v>39</v>
+      </c>
+      <c r="D277" s="90" t="s">
+        <v>719</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="66">
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="D163:D166"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="A95:A110"/>
+    <mergeCell ref="B95:B110"/>
+    <mergeCell ref="A111:A129"/>
+    <mergeCell ref="B111:B129"/>
+    <mergeCell ref="C130:C131"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="A144:A146"/>
+    <mergeCell ref="B144:B146"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="A147:A151"/>
+    <mergeCell ref="B147:B151"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="A161:A167"/>
+    <mergeCell ref="A227:A237"/>
+    <mergeCell ref="B227:B237"/>
+    <mergeCell ref="A67:A71"/>
+    <mergeCell ref="B130:B143"/>
+    <mergeCell ref="A154:A160"/>
+    <mergeCell ref="B154:B160"/>
+    <mergeCell ref="A130:A143"/>
+    <mergeCell ref="A242:A244"/>
+    <mergeCell ref="B242:B244"/>
+    <mergeCell ref="A238:A239"/>
+    <mergeCell ref="B238:B239"/>
+    <mergeCell ref="B161:B167"/>
+    <mergeCell ref="A249:A250"/>
+    <mergeCell ref="B249:B250"/>
+    <mergeCell ref="A245:A246"/>
+    <mergeCell ref="B245:B246"/>
+    <mergeCell ref="A247:A248"/>
+    <mergeCell ref="B247:B248"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="A73:A88"/>
+    <mergeCell ref="B73:B88"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="B55:B60"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A55:A60"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B221:B223"/>
@@ -35241,56 +35330,6 @@
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="A73:A88"/>
-    <mergeCell ref="B73:B88"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="B55:B60"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A55:A60"/>
-    <mergeCell ref="A249:A250"/>
-    <mergeCell ref="B249:B250"/>
-    <mergeCell ref="A245:A246"/>
-    <mergeCell ref="B245:B246"/>
-    <mergeCell ref="A247:A248"/>
-    <mergeCell ref="B247:B248"/>
-    <mergeCell ref="A242:A244"/>
-    <mergeCell ref="B242:B244"/>
-    <mergeCell ref="A238:A239"/>
-    <mergeCell ref="B238:B239"/>
-    <mergeCell ref="B161:B167"/>
-    <mergeCell ref="A147:A151"/>
-    <mergeCell ref="B147:B151"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="A161:A167"/>
-    <mergeCell ref="A227:A237"/>
-    <mergeCell ref="B227:B237"/>
-    <mergeCell ref="A67:A71"/>
-    <mergeCell ref="B130:B143"/>
-    <mergeCell ref="A154:A160"/>
-    <mergeCell ref="B154:B160"/>
-    <mergeCell ref="A130:A143"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="D163:D166"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="A95:A110"/>
-    <mergeCell ref="B95:B110"/>
-    <mergeCell ref="A111:A129"/>
-    <mergeCell ref="B111:B129"/>
-    <mergeCell ref="C130:C131"/>
-    <mergeCell ref="C132:C133"/>
-    <mergeCell ref="A144:A146"/>
-    <mergeCell ref="B144:B146"/>
-    <mergeCell ref="A61:A63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -35299,10 +35338,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DBC65A-63D2-46B3-B8B5-A94A70B9EDFE}">
-  <dimension ref="A1:D153"/>
+  <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C121" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D152" sqref="D152"/>
+    <sheetView topLeftCell="A137" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A159" sqref="A159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35522,10 +35561,10 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="163" t="s">
+      <c r="A21" s="159" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="188" t="s">
+      <c r="B21" s="178" t="s">
         <v>244</v>
       </c>
       <c r="C21" s="53" t="s">
@@ -35536,8 +35575,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="163"/>
-      <c r="B22" s="188"/>
+      <c r="A22" s="159"/>
+      <c r="B22" s="178"/>
       <c r="C22" s="53" t="s">
         <v>547</v>
       </c>
@@ -35546,8 +35585,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="163"/>
-      <c r="B23" s="188"/>
+      <c r="A23" s="159"/>
+      <c r="B23" s="178"/>
       <c r="C23" s="53" t="s">
         <v>549</v>
       </c>
@@ -35556,8 +35595,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="163"/>
-      <c r="B24" s="188"/>
+      <c r="A24" s="159"/>
+      <c r="B24" s="178"/>
       <c r="C24" s="53" t="s">
         <v>551</v>
       </c>
@@ -35566,8 +35605,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="163"/>
-      <c r="B25" s="188"/>
+      <c r="A25" s="159"/>
+      <c r="B25" s="178"/>
       <c r="C25" s="53" t="s">
         <v>552</v>
       </c>
@@ -35576,8 +35615,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="163"/>
-      <c r="B26" s="188"/>
+      <c r="A26" s="159"/>
+      <c r="B26" s="178"/>
       <c r="C26" s="53" t="s">
         <v>553</v>
       </c>
@@ -35586,8 +35625,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="163"/>
-      <c r="B27" s="188"/>
+      <c r="A27" s="159"/>
+      <c r="B27" s="178"/>
       <c r="C27" s="53" t="s">
         <v>554</v>
       </c>
@@ -35596,8 +35635,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="163"/>
-      <c r="B28" s="188"/>
+      <c r="A28" s="159"/>
+      <c r="B28" s="178"/>
       <c r="C28" s="53" t="s">
         <v>555</v>
       </c>
@@ -35606,8 +35645,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="163"/>
-      <c r="B29" s="188"/>
+      <c r="A29" s="159"/>
+      <c r="B29" s="178"/>
       <c r="C29" s="53" t="s">
         <v>556</v>
       </c>
@@ -35616,8 +35655,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="163"/>
-      <c r="B30" s="188"/>
+      <c r="A30" s="159"/>
+      <c r="B30" s="178"/>
       <c r="C30" s="53" t="s">
         <v>557</v>
       </c>
@@ -35626,8 +35665,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="163"/>
-      <c r="B31" s="188"/>
+      <c r="A31" s="159"/>
+      <c r="B31" s="178"/>
       <c r="C31" s="53" t="s">
         <v>558</v>
       </c>
@@ -35636,8 +35675,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="163"/>
-      <c r="B32" s="188"/>
+      <c r="A32" s="159"/>
+      <c r="B32" s="178"/>
       <c r="C32" s="53" t="s">
         <v>559</v>
       </c>
@@ -35646,8 +35685,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="163"/>
-      <c r="B33" s="188"/>
+      <c r="A33" s="159"/>
+      <c r="B33" s="178"/>
       <c r="C33" s="53" t="s">
         <v>560</v>
       </c>
@@ -35656,8 +35695,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="163"/>
-      <c r="B34" s="188"/>
+      <c r="A34" s="159"/>
+      <c r="B34" s="178"/>
       <c r="C34" s="53" t="s">
         <v>561</v>
       </c>
@@ -35666,8 +35705,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="163"/>
-      <c r="B35" s="188"/>
+      <c r="A35" s="159"/>
+      <c r="B35" s="178"/>
       <c r="C35" s="53" t="s">
         <v>562</v>
       </c>
@@ -35676,8 +35715,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="163"/>
-      <c r="B36" s="188"/>
+      <c r="A36" s="159"/>
+      <c r="B36" s="178"/>
       <c r="C36" s="53" t="s">
         <v>564</v>
       </c>
@@ -35686,8 +35725,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="163"/>
-      <c r="B37" s="188"/>
+      <c r="A37" s="159"/>
+      <c r="B37" s="178"/>
       <c r="C37" s="56" t="s">
         <v>565</v>
       </c>
@@ -35696,8 +35735,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="163"/>
-      <c r="B38" s="188"/>
+      <c r="A38" s="159"/>
+      <c r="B38" s="178"/>
       <c r="C38" s="53" t="s">
         <v>566</v>
       </c>
@@ -35706,8 +35745,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="163"/>
-      <c r="B39" s="188"/>
+      <c r="A39" s="159"/>
+      <c r="B39" s="178"/>
       <c r="C39" s="56" t="s">
         <v>567</v>
       </c>
@@ -36032,10 +36071,10 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="188" t="s">
+      <c r="A66" s="178" t="s">
         <v>579</v>
       </c>
-      <c r="B66" s="188" t="s">
+      <c r="B66" s="178" t="s">
         <v>244</v>
       </c>
       <c r="C66" s="53" t="s">
@@ -36046,8 +36085,8 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="188"/>
-      <c r="B67" s="188"/>
+      <c r="A67" s="178"/>
+      <c r="B67" s="178"/>
       <c r="C67" s="53" t="s">
         <v>601</v>
       </c>
@@ -36056,8 +36095,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="188"/>
-      <c r="B68" s="188"/>
+      <c r="A68" s="178"/>
+      <c r="B68" s="178"/>
       <c r="C68" s="53" t="s">
         <v>602</v>
       </c>
@@ -36066,8 +36105,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="188"/>
-      <c r="B69" s="188"/>
+      <c r="A69" s="178"/>
+      <c r="B69" s="178"/>
       <c r="C69" s="53" t="s">
         <v>603</v>
       </c>
@@ -36076,8 +36115,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="188"/>
-      <c r="B70" s="188"/>
+      <c r="A70" s="178"/>
+      <c r="B70" s="178"/>
       <c r="C70" s="53" t="s">
         <v>604</v>
       </c>
@@ -36110,10 +36149,10 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="188" t="s">
+      <c r="A73" s="178" t="s">
         <v>369</v>
       </c>
-      <c r="B73" s="188" t="s">
+      <c r="B73" s="178" t="s">
         <v>244</v>
       </c>
       <c r="C73" s="53"/>
@@ -36122,8 +36161,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="188"/>
-      <c r="B74" s="188"/>
+      <c r="A74" s="178"/>
+      <c r="B74" s="178"/>
       <c r="C74" s="53" t="s">
         <v>599</v>
       </c>
@@ -36132,8 +36171,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="188"/>
-      <c r="B75" s="188"/>
+      <c r="A75" s="178"/>
+      <c r="B75" s="178"/>
       <c r="C75" s="53" t="s">
         <v>601</v>
       </c>
@@ -36142,8 +36181,8 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="188"/>
-      <c r="B76" s="188"/>
+      <c r="A76" s="178"/>
+      <c r="B76" s="178"/>
       <c r="C76" s="53" t="s">
         <v>602</v>
       </c>
@@ -36152,8 +36191,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="188"/>
-      <c r="B77" s="188"/>
+      <c r="A77" s="178"/>
+      <c r="B77" s="178"/>
       <c r="C77" s="53" t="s">
         <v>603</v>
       </c>
@@ -36162,8 +36201,8 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="188"/>
-      <c r="B78" s="188"/>
+      <c r="A78" s="178"/>
+      <c r="B78" s="178"/>
       <c r="C78" s="53" t="s">
         <v>604</v>
       </c>
@@ -36172,8 +36211,8 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="188"/>
-      <c r="B79" s="188"/>
+      <c r="A79" s="178"/>
+      <c r="B79" s="178"/>
       <c r="C79" s="53" t="s">
         <v>607</v>
       </c>
@@ -36182,10 +36221,10 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="188" t="s">
+      <c r="A80" s="178" t="s">
         <v>36</v>
       </c>
-      <c r="B80" s="188" t="s">
+      <c r="B80" s="178" t="s">
         <v>244</v>
       </c>
       <c r="C80" s="53"/>
@@ -36194,8 +36233,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="188"/>
-      <c r="B81" s="188"/>
+      <c r="A81" s="178"/>
+      <c r="B81" s="178"/>
       <c r="C81" s="53" t="s">
         <v>599</v>
       </c>
@@ -36204,8 +36243,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="188"/>
-      <c r="B82" s="188"/>
+      <c r="A82" s="178"/>
+      <c r="B82" s="178"/>
       <c r="C82" s="53" t="s">
         <v>601</v>
       </c>
@@ -36214,8 +36253,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="188"/>
-      <c r="B83" s="188"/>
+      <c r="A83" s="178"/>
+      <c r="B83" s="178"/>
       <c r="C83" s="53" t="s">
         <v>602</v>
       </c>
@@ -36224,8 +36263,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="188"/>
-      <c r="B84" s="188"/>
+      <c r="A84" s="178"/>
+      <c r="B84" s="178"/>
       <c r="C84" s="53" t="s">
         <v>603</v>
       </c>
@@ -36234,8 +36273,8 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="188"/>
-      <c r="B85" s="188"/>
+      <c r="A85" s="178"/>
+      <c r="B85" s="178"/>
       <c r="C85" s="53" t="s">
         <v>604</v>
       </c>
@@ -36244,8 +36283,8 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="188"/>
-      <c r="B86" s="188"/>
+      <c r="A86" s="178"/>
+      <c r="B86" s="178"/>
       <c r="C86" s="53" t="s">
         <v>607</v>
       </c>
@@ -36720,10 +36759,10 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="188" t="s">
+      <c r="A125" s="178" t="s">
         <v>583</v>
       </c>
-      <c r="B125" s="188" t="s">
+      <c r="B125" s="178" t="s">
         <v>244</v>
       </c>
       <c r="C125" s="89" t="s">
@@ -36734,8 +36773,8 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="188"/>
-      <c r="B126" s="188"/>
+      <c r="A126" s="178"/>
+      <c r="B126" s="178"/>
       <c r="C126" s="53" t="s">
         <v>653</v>
       </c>
@@ -36744,8 +36783,8 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="188"/>
-      <c r="B127" s="188"/>
+      <c r="A127" s="178"/>
+      <c r="B127" s="178"/>
       <c r="C127" s="53" t="s">
         <v>655</v>
       </c>
@@ -36754,8 +36793,8 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="188"/>
-      <c r="B128" s="188"/>
+      <c r="A128" s="178"/>
+      <c r="B128" s="178"/>
       <c r="C128" s="53" t="s">
         <v>657</v>
       </c>
@@ -36764,8 +36803,8 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="188"/>
-      <c r="B129" s="188"/>
+      <c r="A129" s="178"/>
+      <c r="B129" s="178"/>
       <c r="C129" s="53" t="s">
         <v>659</v>
       </c>
@@ -36802,7 +36841,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="159" t="s">
+      <c r="A132" s="169" t="s">
         <v>663</v>
       </c>
       <c r="B132" s="117" t="s">
@@ -36816,7 +36855,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="160"/>
+      <c r="A133" s="170"/>
       <c r="B133" s="118" t="s">
         <v>244</v>
       </c>
@@ -36884,10 +36923,10 @@
       </c>
     </row>
     <row r="138" spans="1:4" s="125" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="188" t="s">
+      <c r="A138" s="178" t="s">
         <v>574</v>
       </c>
-      <c r="B138" s="188" t="s">
+      <c r="B138" s="178" t="s">
         <v>244</v>
       </c>
       <c r="C138" s="53" t="s">
@@ -36898,8 +36937,8 @@
       </c>
     </row>
     <row r="139" spans="1:4" s="125" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="188"/>
-      <c r="B139" s="188"/>
+      <c r="A139" s="178"/>
+      <c r="B139" s="178"/>
       <c r="C139" s="53" t="s">
         <v>684</v>
       </c>
@@ -36922,7 +36961,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="159" t="s">
+      <c r="A141" s="169" t="s">
         <v>681</v>
       </c>
       <c r="B141" s="192" t="s">
@@ -36936,7 +36975,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="160"/>
+      <c r="A142" s="170"/>
       <c r="B142" s="194"/>
       <c r="C142" s="53" t="s">
         <v>686</v>
@@ -37089,29 +37128,46 @@
       <c r="A153" s="90" t="s">
         <v>681</v>
       </c>
-      <c r="B153" s="139" t="s">
+      <c r="B153" s="137" t="s">
         <v>244</v>
       </c>
       <c r="C153" s="53" t="s">
         <v>716</v>
       </c>
-      <c r="D153" s="217" t="s">
+      <c r="D153" s="139" t="s">
         <v>717</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A154" s="217" t="s">
+        <v>718</v>
+      </c>
+      <c r="B154" s="138" t="s">
+        <v>244</v>
+      </c>
+      <c r="C154" s="90" t="s">
+        <v>39</v>
+      </c>
+      <c r="D154" s="90" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A155" s="56" t="s">
+        <v>720</v>
+      </c>
+      <c r="B155" s="138" t="s">
+        <v>244</v>
+      </c>
+      <c r="C155" s="90" t="s">
+        <v>39</v>
+      </c>
+      <c r="D155" s="90" t="s">
+        <v>719</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B102:B105"/>
-    <mergeCell ref="A106:A109"/>
-    <mergeCell ref="B106:B109"/>
-    <mergeCell ref="A2:A20"/>
-    <mergeCell ref="B2:B20"/>
-    <mergeCell ref="A21:A39"/>
-    <mergeCell ref="B21:B39"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:B42"/>
     <mergeCell ref="A141:A142"/>
     <mergeCell ref="B141:B142"/>
     <mergeCell ref="A66:A70"/>
@@ -37128,6 +37184,17 @@
     <mergeCell ref="A125:A129"/>
     <mergeCell ref="B125:B129"/>
     <mergeCell ref="A102:A105"/>
+    <mergeCell ref="B102:B105"/>
+    <mergeCell ref="A106:A109"/>
+    <mergeCell ref="B106:B109"/>
+    <mergeCell ref="A2:A20"/>
+    <mergeCell ref="B2:B20"/>
+    <mergeCell ref="A21:A39"/>
+    <mergeCell ref="B21:B39"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:B42"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37136,6 +37203,60 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <nb82aa7489a64919aab5fd247ffa0d1e xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Enhanced Reporting Requirements</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b99d9e68-488f-45bf-a303-a86e26269b90</TermId>
+        </TermInfo>
+      </Terms>
+    </nb82aa7489a64919aab5fd247ffa0d1e>
+    <e9be08524f454d8b979862330e952271 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </e9be08524f454d8b979862330e952271>
+    <ade64af1c6a24cfdbe8da7f962b31d74 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ade64af1c6a24cfdbe8da7f962b31d74>
+    <e62af2f156934d1aab35222180c5fbb1 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Project Site</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">7b0ab4a9-6be8-4c6c-983c-945fdef69f95</TermId>
+        </TermInfo>
+      </Terms>
+    </e62af2f156934d1aab35222180c5fbb1>
+    <TaxCatchAll xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Value>97</Value>
+      <Value>45</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+    <f62107d924a7469492625f91956e46a6 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Development</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bc803685-9f6b-4a9c-85fc-59591d8af7f6</TermId>
+        </TermInfo>
+      </Terms>
+    </f62107d924a7469492625f91956e46a6>
+    <l29cd52af9b640b690e3347aa75f97a9 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l29cd52af9b640b690e3347aa75f97a9>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Word document" ma:contentTypeID="0x010100852E11B2A94E4937B655CB4FCD918453006DFD5C59A7CB45AAB5046F3899BB7DEC00F397826DF95DEB4B8DB89BEACF2240F1" ma:contentTypeVersion="79" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="2efa76ee5d5cd602cc18ca32df57176e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9394a98c30c487d0596bd1768260a67a" ns2:_="">
     <xsd:import namespace="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
@@ -37355,61 +37476,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <nb82aa7489a64919aab5fd247ffa0d1e xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Enhanced Reporting Requirements</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b99d9e68-488f-45bf-a303-a86e26269b90</TermId>
-        </TermInfo>
-      </Terms>
-    </nb82aa7489a64919aab5fd247ffa0d1e>
-    <e9be08524f454d8b979862330e952271 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </e9be08524f454d8b979862330e952271>
-    <ade64af1c6a24cfdbe8da7f962b31d74 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ade64af1c6a24cfdbe8da7f962b31d74>
-    <e62af2f156934d1aab35222180c5fbb1 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Project Site</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">7b0ab4a9-6be8-4c6c-983c-945fdef69f95</TermId>
-        </TermInfo>
-      </Terms>
-    </e62af2f156934d1aab35222180c5fbb1>
-    <TaxCatchAll xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Value>97</Value>
-      <Value>45</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-    <f62107d924a7469492625f91956e46a6 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Development</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bc803685-9f6b-4a9c-85fc-59591d8af7f6</TermId>
-        </TermInfo>
-      </Terms>
-    </f62107d924a7469492625f91956e46a6>
-    <l29cd52af9b640b690e3347aa75f97a9 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l29cd52af9b640b690e3347aa75f97a9>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E83ECEA-8E14-42A0-80EE-042ED267BA0C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F5A24BE-BB8C-4A62-B10D-ABDF1081592A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA064B24-F175-41F6-9C06-3B56F1D75E8F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37425,22 +37510,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F5A24BE-BB8C-4A62-B10D-ABDF1081592A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E83ECEA-8E14-42A0-80EE-042ED267BA0C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>